<commit_message>
Added more parameter descriptions
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0AEA1D-8DAF-4A10-BA30-3795F94E8AE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1583A6B5-9EF1-4480-8404-502DB7687538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -447,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -580,16 +580,16 @@
         <v>161</v>
       </c>
       <c r="C3">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D3">
         <v>1451</v>
       </c>
       <c r="E3">
-        <v>303</v>
+        <v>377</v>
       </c>
       <c r="F3">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>20</v>
@@ -605,15 +605,15 @@
       </c>
       <c r="L3" s="3">
         <f>100*C3/B3</f>
-        <v>39.751552795031053</v>
+        <v>40.372670807453417</v>
       </c>
       <c r="M3" s="3">
         <f>100*E3/D3</f>
-        <v>20.882150241212958</v>
+        <v>25.982081323225362</v>
       </c>
       <c r="N3" s="3">
         <f>100*F3/B3</f>
-        <v>14.285714285714286</v>
+        <v>15.527950310559007</v>
       </c>
       <c r="O3" s="3">
         <f>100*H3/G3</f>
@@ -623,6 +623,13 @@
         <f>100*J3/I3</f>
         <v>39.71291866028708</v>
       </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
A few more bits of documentation
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1583A6B5-9EF1-4480-8404-502DB7687538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933DE247-0353-44F8-B20A-F0DD821CBF4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -148,6 +148,1170 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% module desc.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>44054</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44056</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>39.751552795031053</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.372670807453417</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44.720496894409941</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-35B7-4A69-BAB0-F6230ED95096}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% params</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>44054</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44056</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>15.575465196416264</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.982081323225362</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.719723183391004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-35B7-4A69-BAB0-F6230ED95096}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% param sets</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>44054</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44056</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>14.285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.527950310559007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.496894409937887</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-35B7-4A69-BAB0-F6230ED95096}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% image meas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>44054</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44056</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-35B7-4A69-BAB0-F6230ED95096}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% object meas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>44054</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44056</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>39.71291866028708</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.71291866028708</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.71291866028708</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-35B7-4A69-BAB0-F6230ED95096}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1381721568"/>
+        <c:axId val="1552787824"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="1381721568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1552787824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1552787824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1381721568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46BC78FD-A061-462E-9537-30CCB76E65DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -447,193 +1611,243 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44054</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2"/>
+      <c r="C2" s="4">
         <v>161</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>64</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1451</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>226</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>23</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>20</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>209</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>83</v>
       </c>
-      <c r="L2" s="3">
-        <f>100*C2/B2</f>
+      <c r="M2" s="3">
+        <f>100*D2/C2</f>
         <v>39.751552795031053</v>
       </c>
-      <c r="M2" s="3">
-        <f>100*E2/D2</f>
+      <c r="N2" s="3">
+        <f>100*F2/E2</f>
         <v>15.575465196416264</v>
       </c>
-      <c r="N2" s="3">
-        <f>100*F2/B2</f>
+      <c r="O2" s="3">
+        <f>100*G2/C2</f>
         <v>14.285714285714286</v>
       </c>
-      <c r="O2" s="3">
-        <f>100*H2/G2</f>
+      <c r="P2" s="3">
+        <f>100*I2/H2</f>
         <v>10</v>
       </c>
-      <c r="P2" s="3">
-        <f>100*J2/I2</f>
+      <c r="Q2" s="3">
+        <f>100*K2/J2</f>
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44055</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2"/>
+      <c r="C3">
         <v>161</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>65</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1451</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>377</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>25</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>20</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>209</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>83</v>
       </c>
-      <c r="L3" s="3">
-        <f>100*C3/B3</f>
+      <c r="M3" s="3">
+        <f>100*D3/C3</f>
         <v>40.372670807453417</v>
       </c>
-      <c r="M3" s="3">
-        <f>100*E3/D3</f>
+      <c r="N3" s="3">
+        <f>100*F3/E3</f>
         <v>25.982081323225362</v>
       </c>
-      <c r="N3" s="3">
-        <f>100*F3/B3</f>
+      <c r="O3" s="3">
+        <f>100*G3/C3</f>
         <v>15.527950310559007</v>
       </c>
-      <c r="O3" s="3">
-        <f>100*H3/G3</f>
+      <c r="P3" s="3">
+        <f>100*I3/H3</f>
         <v>10</v>
       </c>
-      <c r="P3" s="3">
-        <f>100*J3/I3</f>
+      <c r="Q3" s="3">
+        <f>100*K3/J3</f>
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4">
+        <v>161</v>
+      </c>
+      <c r="D4">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>1445</v>
+      </c>
+      <c r="F4">
+        <v>415</v>
+      </c>
+      <c r="G4">
+        <v>33</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>209</v>
+      </c>
+      <c r="K4">
+        <v>83</v>
+      </c>
+      <c r="M4" s="3">
+        <f>100*D4/C4</f>
+        <v>44.720496894409941</v>
+      </c>
+      <c r="N4" s="3">
+        <f>100*F4/E4</f>
+        <v>28.719723183391004</v>
+      </c>
+      <c r="O4" s="3">
+        <f>100*G4/C4</f>
+        <v>20.496894409937887</v>
+      </c>
+      <c r="P4" s="3">
+        <f>100*I4/H4</f>
+        <v>10</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>100*K4/J4</f>
+        <v>39.71291866028708</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a bit more documentation
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933DE247-0353-44F8-B20A-F0DD821CBF4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202BB9DC-422E-41C9-8974-DD173AE9109A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -211,6 +211,9 @@
                 <c:pt idx="2">
                   <c:v>44056</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44057</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -228,6 +231,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>44.720496894409941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45.341614906832298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -280,6 +286,9 @@
                 <c:pt idx="2">
                   <c:v>44056</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44057</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -297,6 +306,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>28.719723183391004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.550173010380622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -349,6 +361,9 @@
                 <c:pt idx="2">
                   <c:v>44056</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44057</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -366,6 +381,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>20.496894409937887</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.118012422360248</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -418,6 +436,9 @@
                 <c:pt idx="2">
                   <c:v>44056</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44057</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -434,6 +455,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -487,6 +511,9 @@
                 <c:pt idx="2">
                   <c:v>44056</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44057</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -503,6 +530,9 @@
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>39.71291866028708</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
               </c:numCache>
@@ -1611,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B5" sqref="B5:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,6 +1874,58 @@
         <v>39.71291866028708</v>
       </c>
     </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>44057</v>
+      </c>
+      <c r="C5">
+        <v>161</v>
+      </c>
+      <c r="D5">
+        <v>73</v>
+      </c>
+      <c r="E5">
+        <v>1445</v>
+      </c>
+      <c r="F5">
+        <v>427</v>
+      </c>
+      <c r="G5">
+        <v>34</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>209</v>
+      </c>
+      <c r="K5">
+        <v>83</v>
+      </c>
+      <c r="M5" s="3">
+        <f>100*D5/C5</f>
+        <v>45.341614906832298</v>
+      </c>
+      <c r="N5" s="3">
+        <f>100*F5/E5</f>
+        <v>29.550173010380622</v>
+      </c>
+      <c r="O5" s="3">
+        <f>100*G5/C5</f>
+        <v>21.118012422360248</v>
+      </c>
+      <c r="P5" s="3">
+        <f>100*I5/H5</f>
+        <v>10</v>
+      </c>
+      <c r="Q5" s="3">
+        <f>100*K5/J5</f>
+        <v>39.71291866028708</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added wand selection to ManuallyIdentifyObjects
Also added more parameter descriptions.
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202BB9DC-422E-41C9-8974-DD173AE9109A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F2DFB1-0BCD-4753-ADFE-C83516467DF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -214,6 +214,9 @@
                 <c:pt idx="3">
                   <c:v>44057</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>44058</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -233,6 +236,9 @@
                   <c:v>44.720496894409941</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>45.341614906832298</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>45.341614906832298</c:v>
                 </c:pt>
               </c:numCache>
@@ -289,6 +295,9 @@
                 <c:pt idx="3">
                   <c:v>44057</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>44058</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -309,6 +318,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>29.550173010380622</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.380622837370243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -364,6 +376,9 @@
                 <c:pt idx="3">
                   <c:v>44057</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>44058</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -384,6 +399,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>21.118012422360248</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.739130434782609</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -439,6 +457,9 @@
                 <c:pt idx="3">
                   <c:v>44057</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>44058</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -458,6 +479,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -514,6 +538,9 @@
                 <c:pt idx="3">
                   <c:v>44057</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>44058</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -533,6 +560,9 @@
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>39.71291866028708</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
               </c:numCache>
@@ -1641,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:K5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1926,6 +1956,58 @@
         <v>39.71291866028708</v>
       </c>
     </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>44058</v>
+      </c>
+      <c r="C6">
+        <v>161</v>
+      </c>
+      <c r="D6">
+        <v>73</v>
+      </c>
+      <c r="E6">
+        <v>1445</v>
+      </c>
+      <c r="F6">
+        <v>439</v>
+      </c>
+      <c r="G6">
+        <v>35</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>209</v>
+      </c>
+      <c r="K6">
+        <v>83</v>
+      </c>
+      <c r="M6" s="3">
+        <f>100*D6/C6</f>
+        <v>45.341614906832298</v>
+      </c>
+      <c r="N6" s="3">
+        <f>100*F6/E6</f>
+        <v>30.380622837370243</v>
+      </c>
+      <c r="O6" s="3">
+        <f>100*G6/C6</f>
+        <v>21.739130434782609</v>
+      </c>
+      <c r="P6" s="3">
+        <f>100*I6/H6</f>
+        <v>10</v>
+      </c>
+      <c r="Q6" s="3">
+        <f>100*K6/J6</f>
+        <v>39.71291866028708</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added some image measurement descriptions
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F2DFB1-0BCD-4753-ADFE-C83516467DF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE44D9F5-38E4-45A4-BABB-DC042FD00B37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -482,7 +482,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1674,7 +1674,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,7 +1979,7 @@
         <v>20</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="J6">
         <v>209</v>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="P6" s="3">
         <f>100*I6/H6</f>
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="Q6" s="3">
         <f>100*K6/J6</f>

</xml_diff>

<commit_message>
Moved to version 0.14.14
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE44D9F5-38E4-45A4-BABB-DC042FD00B37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E13CA4-E404-45DB-BCC4-5627DE6CF454}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -239,7 +239,7 @@
                   <c:v>45.341614906832298</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.341614906832298</c:v>
+                  <c:v>46.58385093167702</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -320,7 +320,7 @@
                   <c:v>29.550173010380622</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.380622837370243</c:v>
+                  <c:v>33.494809688581313</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -401,7 +401,7 @@
                   <c:v>21.118012422360248</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.739130434782609</c:v>
+                  <c:v>22.981366459627328</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1964,16 +1964,16 @@
         <v>161</v>
       </c>
       <c r="D6">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E6">
         <v>1445</v>
       </c>
       <c r="F6">
-        <v>439</v>
+        <v>484</v>
       </c>
       <c r="G6">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H6">
         <v>20</v>
@@ -1989,15 +1989,15 @@
       </c>
       <c r="M6" s="3">
         <f>100*D6/C6</f>
-        <v>45.341614906832298</v>
+        <v>46.58385093167702</v>
       </c>
       <c r="N6" s="3">
         <f>100*F6/E6</f>
-        <v>30.380622837370243</v>
+        <v>33.494809688581313</v>
       </c>
       <c r="O6" s="3">
         <f>100*G6/C6</f>
-        <v>21.739130434782609</v>
+        <v>22.981366459627328</v>
       </c>
       <c r="P6" s="3">
         <f>100*I6/H6</f>

</xml_diff>

<commit_message>
Updated parameter coverage history
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E13CA4-E404-45DB-BCC4-5627DE6CF454}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A01984-96C8-4D17-8A29-2714A27F4107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="384" yWindow="-108" windowWidth="22764" windowHeight="13176" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$1</c:f>
+              <c:f>Sheet1!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -198,31 +198,34 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:f>Sheet1!$B$2:$B$40</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>44054</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44055</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44056</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44057</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44058</c:v>
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$40</c:f>
+              <c:f>Sheet1!$N$2:$N$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="39"/>
@@ -240,6 +243,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>46.58385093167702</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47.204968944099377</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -256,7 +262,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$1</c:f>
+              <c:f>Sheet1!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -279,31 +285,34 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:f>Sheet1!$B$2:$B$40</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>44054</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44055</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44056</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44057</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44058</c:v>
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$40</c:f>
+              <c:f>Sheet1!$O$2:$O$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="39"/>
@@ -321,6 +330,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>33.494809688581313</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33.840830449826989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -337,7 +349,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$1</c:f>
+              <c:f>Sheet1!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -360,31 +372,34 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:f>Sheet1!$B$2:$B$40</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>44054</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44055</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44056</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44057</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44058</c:v>
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$40</c:f>
+              <c:f>Sheet1!$P$2:$P$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="39"/>
@@ -402,6 +417,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>22.981366459627328</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.602484472049689</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -418,7 +436,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$1</c:f>
+              <c:f>Sheet1!$Q$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -441,31 +459,34 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:f>Sheet1!$B$2:$B$40</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>44054</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44055</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44056</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44057</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44058</c:v>
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$40</c:f>
+              <c:f>Sheet1!$Q$2:$Q$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="39"/>
@@ -482,6 +503,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -499,7 +523,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$1</c:f>
+              <c:f>Sheet1!$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -522,31 +546,34 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:f>Sheet1!$B$2:$B$40</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>44054</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44055</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44056</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44057</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44058</c:v>
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$40</c:f>
+              <c:f>Sheet1!$R$2:$R$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="39"/>
@@ -564,6 +591,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>39.71291866028708</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39.523809523809526</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -587,14 +617,14 @@
         <c:axId val="1381721568"/>
         <c:axId val="1552787824"/>
       </c:lineChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="1381721568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -634,9 +664,10 @@
         <c:crossAx val="1552787824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="1552787824"/>
         <c:scaling>
@@ -1337,13 +1368,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>238124</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>180974</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
@@ -1671,341 +1702,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:K6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44054</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="4">
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="4">
         <v>161</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>64</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1451</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>226</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>23</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>20</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>2</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>209</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>83</v>
       </c>
-      <c r="M2" s="3">
-        <f>100*D2/C2</f>
+      <c r="N2" s="3">
+        <f>100*E2/D2</f>
         <v>39.751552795031053</v>
       </c>
-      <c r="N2" s="3">
-        <f>100*F2/E2</f>
+      <c r="O2" s="3">
+        <f>100*G2/F2</f>
         <v>15.575465196416264</v>
       </c>
-      <c r="O2" s="3">
-        <f>100*G2/C2</f>
+      <c r="P2" s="3">
+        <f>100*H2/D2</f>
         <v>14.285714285714286</v>
       </c>
-      <c r="P2" s="3">
-        <f>100*I2/H2</f>
+      <c r="Q2" s="3">
+        <f>100*J2/I2</f>
         <v>10</v>
       </c>
-      <c r="Q2" s="3">
-        <f>100*K2/J2</f>
+      <c r="R2" s="3">
+        <f>100*L2/K2</f>
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44055</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3">
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3">
         <v>161</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>65</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1451</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>377</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>25</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>20</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>209</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>83</v>
       </c>
-      <c r="M3" s="3">
-        <f>100*D3/C3</f>
+      <c r="N3" s="3">
+        <f>100*E3/D3</f>
         <v>40.372670807453417</v>
       </c>
-      <c r="N3" s="3">
-        <f>100*F3/E3</f>
+      <c r="O3" s="3">
+        <f>100*G3/F3</f>
         <v>25.982081323225362</v>
       </c>
-      <c r="O3" s="3">
-        <f>100*G3/C3</f>
+      <c r="P3" s="3">
+        <f>100*H3/D3</f>
         <v>15.527950310559007</v>
       </c>
-      <c r="P3" s="3">
-        <f>100*I3/H3</f>
+      <c r="Q3" s="3">
+        <f>100*J3/I3</f>
         <v>10</v>
       </c>
-      <c r="Q3" s="3">
-        <f>100*K3/J3</f>
+      <c r="R3" s="3">
+        <f>100*L3/K3</f>
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44056</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4">
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4">
         <v>161</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>72</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1445</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>415</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>33</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>20</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>209</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>83</v>
       </c>
-      <c r="M4" s="3">
-        <f>100*D4/C4</f>
+      <c r="N4" s="3">
+        <f>100*E4/D4</f>
         <v>44.720496894409941</v>
       </c>
-      <c r="N4" s="3">
-        <f>100*F4/E4</f>
+      <c r="O4" s="3">
+        <f>100*G4/F4</f>
         <v>28.719723183391004</v>
       </c>
-      <c r="O4" s="3">
-        <f>100*G4/C4</f>
+      <c r="P4" s="3">
+        <f>100*H4/D4</f>
         <v>20.496894409937887</v>
       </c>
-      <c r="P4" s="3">
-        <f>100*I4/H4</f>
+      <c r="Q4" s="3">
+        <f>100*J4/I4</f>
         <v>10</v>
       </c>
-      <c r="Q4" s="3">
-        <f>100*K4/J4</f>
+      <c r="R4" s="3">
+        <f>100*L4/K4</f>
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44057</v>
       </c>
-      <c r="C5">
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="D5">
         <v>161</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>73</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1445</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>427</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>34</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>20</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>2</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>209</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>83</v>
       </c>
-      <c r="M5" s="3">
-        <f>100*D5/C5</f>
+      <c r="N5" s="3">
+        <f>100*E5/D5</f>
         <v>45.341614906832298</v>
       </c>
-      <c r="N5" s="3">
-        <f>100*F5/E5</f>
+      <c r="O5" s="3">
+        <f>100*G5/F5</f>
         <v>29.550173010380622</v>
       </c>
-      <c r="O5" s="3">
-        <f>100*G5/C5</f>
+      <c r="P5" s="3">
+        <f>100*H5/D5</f>
         <v>21.118012422360248</v>
       </c>
-      <c r="P5" s="3">
-        <f>100*I5/H5</f>
+      <c r="Q5" s="3">
+        <f>100*J5/I5</f>
         <v>10</v>
       </c>
-      <c r="Q5" s="3">
-        <f>100*K5/J5</f>
+      <c r="R5" s="3">
+        <f>100*L5/K5</f>
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44058</v>
       </c>
-      <c r="C6">
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+      <c r="D6">
         <v>161</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>75</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1445</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>484</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>37</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>20</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>14</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>209</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>83</v>
       </c>
-      <c r="M6" s="3">
-        <f>100*D6/C6</f>
+      <c r="N6" s="3">
+        <f>100*E6/D6</f>
         <v>46.58385093167702</v>
       </c>
-      <c r="N6" s="3">
-        <f>100*F6/E6</f>
+      <c r="O6" s="3">
+        <f>100*G6/F6</f>
         <v>33.494809688581313</v>
       </c>
-      <c r="O6" s="3">
-        <f>100*G6/C6</f>
+      <c r="P6" s="3">
+        <f>100*H6/D6</f>
         <v>22.981366459627328</v>
       </c>
-      <c r="P6" s="3">
-        <f>100*I6/H6</f>
+      <c r="Q6" s="3">
+        <f>100*J6/I6</f>
         <v>70</v>
       </c>
-      <c r="Q6" s="3">
-        <f>100*K6/J6</f>
+      <c r="R6" s="3">
+        <f>100*L6/K6</f>
         <v>39.71291866028708</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>161</v>
+      </c>
+      <c r="E7">
+        <v>76</v>
+      </c>
+      <c r="F7">
+        <v>1445</v>
+      </c>
+      <c r="G7">
+        <v>489</v>
+      </c>
+      <c r="H7">
+        <v>38</v>
+      </c>
+      <c r="I7">
+        <v>20</v>
+      </c>
+      <c r="J7">
+        <v>14</v>
+      </c>
+      <c r="K7">
+        <v>210</v>
+      </c>
+      <c r="L7">
+        <v>83</v>
+      </c>
+      <c r="N7" s="3">
+        <f>100*E7/D7</f>
+        <v>47.204968944099377</v>
+      </c>
+      <c r="O7" s="3">
+        <f>100*G7/F7</f>
+        <v>33.840830449826989</v>
+      </c>
+      <c r="P7" s="3">
+        <f>100*H7/D7</f>
+        <v>23.602484472049689</v>
+      </c>
+      <c r="Q7" s="3">
+        <f>100*J7/I7</f>
+        <v>70</v>
+      </c>
+      <c r="R7" s="3">
+        <f>100*L7/K7</f>
+        <v>39.523809523809526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moving to version 0.14.15
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Java Projects\MIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A01984-96C8-4D17-8A29-2714A27F4107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9452ABAD-AE57-4E44-BCA7-25195DADB78A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="-108" windowWidth="22764" windowHeight="13176" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -198,10 +198,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$40</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -219,16 +219,28 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$40</c:f>
+              <c:f>Sheet1!$N$2:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -245,6 +257,9 @@
                   <c:v>46.58385093167702</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>47.204968944099377</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>47.204968944099377</c:v>
                 </c:pt>
               </c:numCache>
@@ -285,10 +300,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$40</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -306,16 +321,28 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$40</c:f>
+              <c:f>Sheet1!$O$2:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>15.575465196416264</c:v>
                 </c:pt>
@@ -333,6 +360,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>33.840830449826989</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.294117647058826</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -372,10 +402,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$40</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -393,16 +423,28 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$40</c:f>
+              <c:f>Sheet1!$P$2:$P$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -419,6 +461,9 @@
                   <c:v>22.981366459627328</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>23.602484472049689</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>23.602484472049689</c:v>
                 </c:pt>
               </c:numCache>
@@ -459,10 +504,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$40</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -480,16 +525,28 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$40</c:f>
+              <c:f>Sheet1!$Q$2:$Q$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -506,6 +563,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -546,10 +606,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$40</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -567,16 +627,28 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$40</c:f>
+              <c:f>Sheet1!$R$2:$R$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -593,6 +665,9 @@
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>39.523809523809526</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>39.523809523809526</c:v>
                 </c:pt>
               </c:numCache>
@@ -1368,16 +1443,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1702,34 +1777,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1776,7 +1851,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44054</v>
       </c>
@@ -1812,27 +1887,27 @@
         <v>83</v>
       </c>
       <c r="N2" s="3">
-        <f>100*E2/D2</f>
+        <f t="shared" ref="N2:N7" si="0">100*E2/D2</f>
         <v>39.751552795031053</v>
       </c>
       <c r="O2" s="3">
-        <f>100*G2/F2</f>
+        <f t="shared" ref="O2:O7" si="1">100*G2/F2</f>
         <v>15.575465196416264</v>
       </c>
       <c r="P2" s="3">
-        <f>100*H2/D2</f>
+        <f t="shared" ref="P2:P7" si="2">100*H2/D2</f>
         <v>14.285714285714286</v>
       </c>
       <c r="Q2" s="3">
-        <f>100*J2/I2</f>
+        <f t="shared" ref="Q2:Q7" si="3">100*J2/I2</f>
         <v>10</v>
       </c>
       <c r="R2" s="3">
-        <f>100*L2/K2</f>
+        <f t="shared" ref="R2:R7" si="4">100*L2/K2</f>
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44055</v>
       </c>
@@ -1868,27 +1943,27 @@
         <v>83</v>
       </c>
       <c r="N3" s="3">
-        <f>100*E3/D3</f>
+        <f t="shared" si="0"/>
         <v>40.372670807453417</v>
       </c>
       <c r="O3" s="3">
-        <f>100*G3/F3</f>
+        <f t="shared" si="1"/>
         <v>25.982081323225362</v>
       </c>
       <c r="P3" s="3">
-        <f>100*H3/D3</f>
+        <f t="shared" si="2"/>
         <v>15.527950310559007</v>
       </c>
       <c r="Q3" s="3">
-        <f>100*J3/I3</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="R3" s="3">
-        <f>100*L3/K3</f>
+        <f t="shared" si="4"/>
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44056</v>
       </c>
@@ -1924,27 +1999,27 @@
         <v>83</v>
       </c>
       <c r="N4" s="3">
-        <f>100*E4/D4</f>
+        <f t="shared" si="0"/>
         <v>44.720496894409941</v>
       </c>
       <c r="O4" s="3">
-        <f>100*G4/F4</f>
+        <f t="shared" si="1"/>
         <v>28.719723183391004</v>
       </c>
       <c r="P4" s="3">
-        <f>100*H4/D4</f>
+        <f t="shared" si="2"/>
         <v>20.496894409937887</v>
       </c>
       <c r="Q4" s="3">
-        <f>100*J4/I4</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="R4" s="3">
-        <f>100*L4/K4</f>
+        <f t="shared" si="4"/>
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44057</v>
       </c>
@@ -1979,27 +2054,27 @@
         <v>83</v>
       </c>
       <c r="N5" s="3">
-        <f>100*E5/D5</f>
+        <f t="shared" si="0"/>
         <v>45.341614906832298</v>
       </c>
       <c r="O5" s="3">
-        <f>100*G5/F5</f>
+        <f t="shared" si="1"/>
         <v>29.550173010380622</v>
       </c>
       <c r="P5" s="3">
-        <f>100*H5/D5</f>
+        <f t="shared" si="2"/>
         <v>21.118012422360248</v>
       </c>
       <c r="Q5" s="3">
-        <f>100*J5/I5</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="R5" s="3">
-        <f>100*L5/K5</f>
+        <f t="shared" si="4"/>
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44058</v>
       </c>
@@ -2034,27 +2109,27 @@
         <v>83</v>
       </c>
       <c r="N6" s="3">
-        <f>100*E6/D6</f>
+        <f t="shared" si="0"/>
         <v>46.58385093167702</v>
       </c>
       <c r="O6" s="3">
-        <f>100*G6/F6</f>
+        <f t="shared" si="1"/>
         <v>33.494809688581313</v>
       </c>
       <c r="P6" s="3">
-        <f>100*H6/D6</f>
+        <f t="shared" si="2"/>
         <v>22.981366459627328</v>
       </c>
       <c r="Q6" s="3">
-        <f>100*J6/I6</f>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="R6" s="3">
-        <f>100*L6/K6</f>
+        <f t="shared" si="4"/>
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44064</v>
       </c>
@@ -2089,24 +2164,244 @@
         <v>83</v>
       </c>
       <c r="N7" s="3">
-        <f>100*E7/D7</f>
+        <f t="shared" si="0"/>
         <v>47.204968944099377</v>
       </c>
       <c r="O7" s="3">
-        <f>100*G7/F7</f>
+        <f t="shared" si="1"/>
         <v>33.840830449826989</v>
       </c>
       <c r="P7" s="3">
-        <f>100*H7/D7</f>
+        <f t="shared" si="2"/>
         <v>23.602484472049689</v>
       </c>
       <c r="Q7" s="3">
-        <f>100*J7/I7</f>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="R7" s="3">
-        <f>100*L7/K7</f>
+        <f t="shared" si="4"/>
         <v>39.523809523809526</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B8" s="4">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>161</v>
+      </c>
+      <c r="E8">
+        <v>76</v>
+      </c>
+      <c r="F8">
+        <v>1445</v>
+      </c>
+      <c r="G8">
+        <v>510</v>
+      </c>
+      <c r="H8">
+        <v>38</v>
+      </c>
+      <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8">
+        <v>14</v>
+      </c>
+      <c r="K8">
+        <v>210</v>
+      </c>
+      <c r="L8">
+        <v>83</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" ref="N8" si="5">100*E8/D8</f>
+        <v>47.204968944099377</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" ref="O8" si="6">100*G8/F8</f>
+        <v>35.294117647058826</v>
+      </c>
+      <c r="P8" s="3">
+        <f t="shared" ref="P8" si="7">100*H8/D8</f>
+        <v>23.602484472049689</v>
+      </c>
+      <c r="Q8" s="3">
+        <f t="shared" ref="Q8" si="8">100*J8/I8</f>
+        <v>70</v>
+      </c>
+      <c r="R8" s="3">
+        <f t="shared" ref="R8" si="9">100*L8/K8</f>
+        <v>39.523809523809526</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="4">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved to version 0.14.15
Added some more documentation
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stephen\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9452ABAD-AE57-4E44-BCA7-25195DADB78A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DA0140-4846-4FDB-9323-C3F601BAB7D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -262,6 +262,9 @@
                 <c:pt idx="6">
                   <c:v>47.204968944099377</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>48.148148148148145</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -364,6 +367,9 @@
                 <c:pt idx="6">
                   <c:v>35.294117647058826</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>36.082474226804123</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -466,6 +472,9 @@
                 <c:pt idx="6">
                   <c:v>23.602484472049689</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.691358024691358</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -568,6 +577,9 @@
                 <c:pt idx="6">
                   <c:v>70</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -668,6 +680,9 @@
                   <c:v>39.523809523809526</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>39.523809523809526</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>39.523809523809526</c:v>
                 </c:pt>
               </c:numCache>
@@ -707,9 +722,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -803,7 +817,11 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -1443,16 +1461,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>666749</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>428624</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1780,7 +1798,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="C9" sqref="C9:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2240,8 +2258,58 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>44070</v>
+      </c>
       <c r="B9" s="4">
         <v>8</v>
+      </c>
+      <c r="D9">
+        <v>162</v>
+      </c>
+      <c r="E9">
+        <v>78</v>
+      </c>
+      <c r="F9">
+        <v>1455</v>
+      </c>
+      <c r="G9">
+        <v>525</v>
+      </c>
+      <c r="H9">
+        <v>40</v>
+      </c>
+      <c r="I9">
+        <v>20</v>
+      </c>
+      <c r="J9">
+        <v>14</v>
+      </c>
+      <c r="K9">
+        <v>210</v>
+      </c>
+      <c r="L9">
+        <v>83</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" ref="N9" si="10">100*E9/D9</f>
+        <v>48.148148148148145</v>
+      </c>
+      <c r="O9" s="3">
+        <f t="shared" ref="O9" si="11">100*G9/F9</f>
+        <v>36.082474226804123</v>
+      </c>
+      <c r="P9" s="3">
+        <f t="shared" ref="P9" si="12">100*H9/D9</f>
+        <v>24.691358024691358</v>
+      </c>
+      <c r="Q9" s="3">
+        <f t="shared" ref="Q9" si="13">100*J9/I9</f>
+        <v>70</v>
+      </c>
+      <c r="R9" s="3">
+        <f t="shared" ref="R9" si="14">100*L9/K9</f>
+        <v>39.523809523809526</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added documentation to numeric object filters
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stephen\Java Projects\MIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DA0140-4846-4FDB-9323-C3F601BAB7D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2263C0A2-C71C-4DC4-8D6E-E20E6EF97919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -229,9 +229,6 @@
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -263,6 +260,9 @@
                   <c:v>47.204968944099377</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>48.148148148148145</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>48.148148148148145</c:v>
                 </c:pt>
               </c:numCache>
@@ -334,9 +334,6 @@
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -369,6 +366,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>36.082474226804123</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.731958762886599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -439,9 +439,6 @@
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -473,6 +470,9 @@
                   <c:v>23.602484472049689</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>24.691358024691358</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>24.691358024691358</c:v>
                 </c:pt>
               </c:numCache>
@@ -544,9 +544,6 @@
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -578,6 +575,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -649,9 +649,6 @@
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -683,6 +680,9 @@
                   <c:v>39.523809523809526</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>39.523809523809526</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>39.523809523809526</c:v>
                 </c:pt>
               </c:numCache>
@@ -1798,7 +1798,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:L9"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2313,164 +2313,152 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>44081</v>
+      </c>
       <c r="B10" s="4">
         <v>9</v>
       </c>
+      <c r="D10">
+        <v>162</v>
+      </c>
+      <c r="E10">
+        <v>78</v>
+      </c>
+      <c r="F10">
+        <v>1455</v>
+      </c>
+      <c r="G10">
+        <v>549</v>
+      </c>
+      <c r="H10">
+        <v>40</v>
+      </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
+      <c r="J10">
+        <v>14</v>
+      </c>
+      <c r="K10">
+        <v>210</v>
+      </c>
+      <c r="L10">
+        <v>83</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" ref="N10" si="15">100*E10/D10</f>
+        <v>48.148148148148145</v>
+      </c>
+      <c r="O10" s="3">
+        <f t="shared" ref="O10" si="16">100*G10/F10</f>
+        <v>37.731958762886599</v>
+      </c>
+      <c r="P10" s="3">
+        <f t="shared" ref="P10" si="17">100*H10/D10</f>
+        <v>24.691358024691358</v>
+      </c>
+      <c r="Q10" s="3">
+        <f t="shared" ref="Q10" si="18">100*J10/I10</f>
+        <v>70</v>
+      </c>
+      <c r="R10" s="3">
+        <f t="shared" ref="R10" si="19">100*L10/K10</f>
+        <v>39.523809523809526</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
-        <v>10</v>
-      </c>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="4">
-        <v>11</v>
-      </c>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="4">
-        <v>12</v>
-      </c>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
-        <v>13</v>
-      </c>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
-        <v>14</v>
-      </c>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="4">
-        <v>15</v>
-      </c>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="4">
-        <v>16</v>
-      </c>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="4">
-        <v>17</v>
-      </c>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="4">
-        <v>18</v>
-      </c>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
-        <v>19</v>
-      </c>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="4">
-        <v>20</v>
-      </c>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="4">
-        <v>21</v>
-      </c>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="4">
-        <v>22</v>
-      </c>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="4">
-        <v>23</v>
-      </c>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="4">
-        <v>24</v>
-      </c>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="4">
-        <v>25</v>
-      </c>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="4">
-        <v>26</v>
-      </c>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="4">
-        <v>27</v>
-      </c>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="4">
-        <v>28</v>
-      </c>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="4">
-        <v>29</v>
-      </c>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="4">
-        <v>30</v>
-      </c>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="4">
-        <v>31</v>
-      </c>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="4">
-        <v>32</v>
-      </c>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="4">
-        <v>33</v>
-      </c>
+      <c r="B34" s="4"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="4">
-        <v>34</v>
-      </c>
+      <c r="B35" s="4"/>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="4">
-        <v>35</v>
-      </c>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="4">
-        <v>36</v>
-      </c>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="4">
-        <v>37</v>
-      </c>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="4">
-        <v>38</v>
-      </c>
+      <c r="B39" s="4"/>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="4">
-        <v>39</v>
-      </c>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="4">
-        <v>40</v>
-      </c>
+      <c r="B41" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Completed object filter parameter descriptions
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2263C0A2-C71C-4DC4-8D6E-E20E6EF97919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCDB213-EDCF-4581-BDB5-8AF965A8DD62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -229,6 +229,9 @@
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -264,6 +267,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>48.148148148148145</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51.851851851851855</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -334,6 +340,9 @@
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -369,6 +378,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>37.731958762886599</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.762886597938142</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -439,6 +451,9 @@
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -474,6 +489,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>24.691358024691358</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.395061728395063</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -544,6 +562,9 @@
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -578,6 +599,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -649,6 +673,9 @@
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -683,6 +710,9 @@
                   <c:v>39.523809523809526</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>39.523809523809526</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>39.523809523809526</c:v>
                 </c:pt>
               </c:numCache>
@@ -1461,15 +1491,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>666749</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1798,7 +1828,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2368,7 +2398,59 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
+      <c r="A11" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B11" s="4">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>162</v>
+      </c>
+      <c r="E11">
+        <v>84</v>
+      </c>
+      <c r="F11">
+        <v>1455</v>
+      </c>
+      <c r="G11">
+        <v>564</v>
+      </c>
+      <c r="H11">
+        <v>46</v>
+      </c>
+      <c r="I11">
+        <v>20</v>
+      </c>
+      <c r="J11">
+        <v>14</v>
+      </c>
+      <c r="K11">
+        <v>210</v>
+      </c>
+      <c r="L11">
+        <v>83</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" ref="N11" si="20">100*E11/D11</f>
+        <v>51.851851851851855</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" ref="O11" si="21">100*G11/F11</f>
+        <v>38.762886597938142</v>
+      </c>
+      <c r="P11" s="3">
+        <f t="shared" ref="P11" si="22">100*H11/D11</f>
+        <v>28.395061728395063</v>
+      </c>
+      <c r="Q11" s="3">
+        <f t="shared" ref="Q11" si="23">100*J11/I11</f>
+        <v>70</v>
+      </c>
+      <c r="R11" s="3">
+        <f t="shared" ref="R11" si="24">100*L11/K11</f>
+        <v>39.523809523809526</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>

</xml_diff>

<commit_message>
Started adding parameter descriptions to OutputControl.
Removed WorkflowParameters module as this has since been replaced by GlobalParameters.
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCDB213-EDCF-4581-BDB5-8AF965A8DD62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96EC33A-83E0-4237-AFF7-06625D157987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -198,10 +198,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -231,16 +231,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$11</c:f>
+              <c:f>Sheet1!$N$2:$N$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -270,6 +273,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>51.851851851851855</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53.41614906832298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -309,10 +315,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -342,16 +348,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$11</c:f>
+              <c:f>Sheet1!$O$2:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>15.575465196416264</c:v>
                 </c:pt>
@@ -381,6 +390,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>38.762886597938142</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39.243986254295535</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -420,10 +432,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -453,16 +465,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$11</c:f>
+              <c:f>Sheet1!$P$2:$P$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -492,6 +507,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>28.395061728395063</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28.571428571428573</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -531,10 +549,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -564,16 +582,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$11</c:f>
+              <c:f>Sheet1!$Q$2:$Q$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -602,6 +623,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -642,10 +666,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -675,16 +699,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$11</c:f>
+              <c:f>Sheet1!$R$2:$R$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -713,6 +740,9 @@
                   <c:v>39.523809523809526</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>39.523809523809526</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>39.523809523809526</c:v>
                 </c:pt>
               </c:numCache>
@@ -1492,15 +1522,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>247649</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1828,7 +1858,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2453,7 +2483,59 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
+      <c r="A12" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B12" s="4">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>161</v>
+      </c>
+      <c r="E12">
+        <v>86</v>
+      </c>
+      <c r="F12">
+        <v>1455</v>
+      </c>
+      <c r="G12">
+        <v>571</v>
+      </c>
+      <c r="H12">
+        <v>46</v>
+      </c>
+      <c r="I12">
+        <v>20</v>
+      </c>
+      <c r="J12">
+        <v>14</v>
+      </c>
+      <c r="K12">
+        <v>210</v>
+      </c>
+      <c r="L12">
+        <v>83</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" ref="N12" si="25">100*E12/D12</f>
+        <v>53.41614906832298</v>
+      </c>
+      <c r="O12" s="3">
+        <f t="shared" ref="O12" si="26">100*G12/F12</f>
+        <v>39.243986254295535</v>
+      </c>
+      <c r="P12" s="3">
+        <f t="shared" ref="P12" si="27">100*H12/D12</f>
+        <v>28.571428571428573</v>
+      </c>
+      <c r="Q12" s="3">
+        <f t="shared" ref="Q12" si="28">100*J12/I12</f>
+        <v>70</v>
+      </c>
+      <c r="R12" s="3">
+        <f t="shared" ref="R12" si="29">100*L12/K12</f>
+        <v>39.523809523809526</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>

</xml_diff>

<commit_message>
Moved to version 0.14.17
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96EC33A-83E0-4237-AFF7-06625D157987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2CE15D-5038-4EB8-B21E-0017D177D111}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -198,10 +198,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -234,16 +234,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$12</c:f>
+              <c:f>Sheet1!$N$2:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -276,6 +279,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>53.41614906832298</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54.037267080745345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -315,10 +321,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -351,16 +357,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$12</c:f>
+              <c:f>Sheet1!$O$2:$O$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>15.575465196416264</c:v>
                 </c:pt>
@@ -393,6 +402,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>39.243986254295535</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39.835164835164832</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -432,10 +444,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -468,16 +480,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$12</c:f>
+              <c:f>Sheet1!$P$2:$P$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -510,6 +525,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>28.571428571428573</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29.19254658385093</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -549,10 +567,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -585,16 +603,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$12</c:f>
+              <c:f>Sheet1!$Q$2:$Q$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -626,6 +647,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -666,10 +690,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -702,16 +726,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$12</c:f>
+              <c:f>Sheet1!$R$2:$R$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -743,6 +770,9 @@
                   <c:v>39.523809523809526</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>39.523809523809526</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>39.523809523809526</c:v>
                 </c:pt>
               </c:numCache>
@@ -1522,15 +1552,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>266699</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>647699</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1858,7 +1888,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2538,7 +2568,59 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
+      <c r="A13" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B13" s="4">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>161</v>
+      </c>
+      <c r="E13">
+        <v>87</v>
+      </c>
+      <c r="F13">
+        <v>1456</v>
+      </c>
+      <c r="G13">
+        <v>580</v>
+      </c>
+      <c r="H13">
+        <v>47</v>
+      </c>
+      <c r="I13">
+        <v>20</v>
+      </c>
+      <c r="J13">
+        <v>14</v>
+      </c>
+      <c r="K13">
+        <v>210</v>
+      </c>
+      <c r="L13">
+        <v>83</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" ref="N13" si="30">100*E13/D13</f>
+        <v>54.037267080745345</v>
+      </c>
+      <c r="O13" s="3">
+        <f t="shared" ref="O13" si="31">100*G13/F13</f>
+        <v>39.835164835164832</v>
+      </c>
+      <c r="P13" s="3">
+        <f t="shared" ref="P13" si="32">100*H13/D13</f>
+        <v>29.19254658385093</v>
+      </c>
+      <c r="Q13" s="3">
+        <f t="shared" ref="Q13" si="33">100*J13/I13</f>
+        <v>70</v>
+      </c>
+      <c r="R13" s="3">
+        <f t="shared" ref="R13" si="34">100*L13/K13</f>
+        <v>39.523809523809526</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>

</xml_diff>

<commit_message>
Final updates before version 0.14.17
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2CE15D-5038-4EB8-B21E-0017D177D111}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD27039-5426-4863-8C2C-BB076D7933B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -1551,16 +1551,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>647699</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>1057275</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added a few more parameter descriptions
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD27039-5426-4863-8C2C-BB076D7933B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A5ED2A-C3DB-447F-A9CC-C4596161FB20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -198,10 +198,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>Sheet1!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -237,16 +237,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$13</c:f>
+              <c:f>Sheet1!$N$2:$N$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -281,6 +284,9 @@
                   <c:v>53.41614906832298</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>54.037267080745345</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>54.037267080745345</c:v>
                 </c:pt>
               </c:numCache>
@@ -321,10 +327,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>Sheet1!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -360,16 +366,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$13</c:f>
+              <c:f>Sheet1!$O$2:$O$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>15.575465196416264</c:v>
                 </c:pt>
@@ -405,6 +414,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>39.835164835164832</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40.356897735072067</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -444,10 +456,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>Sheet1!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -483,16 +495,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$13</c:f>
+              <c:f>Sheet1!$P$2:$P$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -528,6 +543,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>29.19254658385093</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>31.055900621118013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -567,10 +585,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>Sheet1!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -606,16 +624,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$13</c:f>
+              <c:f>Sheet1!$Q$2:$Q$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -650,6 +671,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -690,10 +714,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>Sheet1!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -729,16 +753,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$13</c:f>
+              <c:f>Sheet1!$R$2:$R$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -773,6 +800,9 @@
                   <c:v>39.523809523809526</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>39.523809523809526</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>39.523809523809526</c:v>
                 </c:pt>
               </c:numCache>
@@ -1553,14 +1583,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>390524</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>1057275</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1888,7 +1918,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="C14" sqref="C14:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,7 +2653,59 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
+      <c r="A14" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B14" s="4">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>161</v>
+      </c>
+      <c r="E14">
+        <v>87</v>
+      </c>
+      <c r="F14">
+        <v>1457</v>
+      </c>
+      <c r="G14">
+        <v>588</v>
+      </c>
+      <c r="H14">
+        <v>50</v>
+      </c>
+      <c r="I14">
+        <v>20</v>
+      </c>
+      <c r="J14">
+        <v>14</v>
+      </c>
+      <c r="K14">
+        <v>210</v>
+      </c>
+      <c r="L14">
+        <v>83</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" ref="N14" si="35">100*E14/D14</f>
+        <v>54.037267080745345</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" ref="O14" si="36">100*G14/F14</f>
+        <v>40.356897735072067</v>
+      </c>
+      <c r="P14" s="3">
+        <f t="shared" ref="P14" si="37">100*H14/D14</f>
+        <v>31.055900621118013</v>
+      </c>
+      <c r="Q14" s="3">
+        <f t="shared" ref="Q14" si="38">100*J14/I14</f>
+        <v>70</v>
+      </c>
+      <c r="R14" s="3">
+        <f t="shared" ref="R14" si="39">100*L14/K14</f>
+        <v>39.523809523809526</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>

</xml_diff>

<commit_message>
A few extra changes before v0.15.0
Bugfix for pre 0.10.0 legacy analysis reader.
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Java Projects\MIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C108909-C4A6-42D8-9CAB-8C6D36B4979B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D269CC7-BABF-473E-979D-CEB722C796F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="-108" windowWidth="22668" windowHeight="13176" activeTab="1" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -668,10 +668,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$17</c:f>
+              <c:f>Sheet1!$B$2:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -719,16 +719,19 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$17</c:f>
+              <c:f>Sheet1!$N$2:$N$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -776,6 +779,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>58.385093167701861</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>57.31707317073171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,10 +821,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$17</c:f>
+              <c:f>Sheet1!$B$2:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -866,16 +872,19 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$17</c:f>
+              <c:f>Sheet1!$O$2:$O$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -923,6 +932,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>44.32576769025367</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43.865435356200528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -962,10 +974,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$17</c:f>
+              <c:f>Sheet1!$B$2:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1013,16 +1025,19 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$17</c:f>
+              <c:f>Sheet1!$P$2:$P$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -1070,6 +1085,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>37.267080745341616</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>36.585365853658537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1109,10 +1127,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$17</c:f>
+              <c:f>Sheet1!$B$2:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1160,16 +1178,19 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$17</c:f>
+              <c:f>Sheet1!$Q$2:$Q$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1216,6 +1237,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -1256,10 +1280,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$17</c:f>
+              <c:f>Sheet1!$B$2:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1307,16 +1331,19 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$17</c:f>
+              <c:f>Sheet1!$R$2:$R$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -1364,6 +1391,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>39.523809523809526</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>38.967136150234744</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2477,32 +2507,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2549,7 +2579,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44054</v>
       </c>
@@ -2605,7 +2635,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44055</v>
       </c>
@@ -2661,7 +2691,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44056</v>
       </c>
@@ -2717,7 +2747,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44057</v>
       </c>
@@ -2772,7 +2802,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44058</v>
       </c>
@@ -2827,7 +2857,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44064</v>
       </c>
@@ -2882,7 +2912,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44069</v>
       </c>
@@ -2937,7 +2967,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44070</v>
       </c>
@@ -2992,7 +3022,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44081</v>
       </c>
@@ -3047,7 +3077,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44082</v>
       </c>
@@ -3102,7 +3132,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44083</v>
       </c>
@@ -3157,7 +3187,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44084</v>
       </c>
@@ -3212,7 +3242,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44085</v>
       </c>
@@ -3267,7 +3297,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44089</v>
       </c>
@@ -3322,7 +3352,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44090</v>
       </c>
@@ -3377,7 +3407,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44091</v>
       </c>
@@ -3432,77 +3462,128 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B18" s="4"/>
-      <c r="O18" s="3"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B18" s="4">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>164</v>
+      </c>
+      <c r="E18">
+        <v>94</v>
+      </c>
+      <c r="F18">
+        <v>1516</v>
+      </c>
+      <c r="G18">
+        <v>665</v>
+      </c>
+      <c r="H18">
+        <v>60</v>
+      </c>
+      <c r="I18">
+        <v>20</v>
+      </c>
+      <c r="J18">
+        <v>14</v>
+      </c>
+      <c r="K18">
+        <v>213</v>
+      </c>
+      <c r="L18">
+        <v>83</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" ref="N18" si="55">100*E18/D18</f>
+        <v>57.31707317073171</v>
+      </c>
+      <c r="O18" s="3">
+        <f t="shared" ref="O18" si="56">100*G18/F18</f>
+        <v>43.865435356200528</v>
+      </c>
+      <c r="P18" s="3">
+        <f t="shared" ref="P18" si="57">100*H18/D18</f>
+        <v>36.585365853658537</v>
+      </c>
+      <c r="Q18" s="3">
+        <f t="shared" ref="Q18" si="58">100*J18/I18</f>
+        <v>70</v>
+      </c>
+      <c r="R18" s="3">
+        <f t="shared" ref="R18" si="59">100*L18/K18</f>
+        <v>38.967136150234744</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
     </row>
   </sheetData>
@@ -3517,18 +3598,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{626E3B8F-11F4-4CEC-B58F-ACDF97F078AF}">
   <dimension ref="A1:G156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="G56" activeCellId="1" sqref="C55 G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3540,7 +3621,7 @@
       </c>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -3552,7 +3633,7 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -3564,7 +3645,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -3576,7 +3657,7 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -3588,7 +3669,7 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3600,7 +3681,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -3612,7 +3693,7 @@
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -3624,7 +3705,7 @@
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -3636,7 +3717,7 @@
       </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -3648,7 +3729,7 @@
       </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -3660,7 +3741,7 @@
       </c>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -3672,7 +3753,7 @@
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -3684,7 +3765,7 @@
       </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -3696,7 +3777,7 @@
       </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -3708,7 +3789,7 @@
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -3720,7 +3801,7 @@
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -3732,7 +3813,7 @@
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -3744,7 +3825,7 @@
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -3756,7 +3837,7 @@
       </c>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -3768,7 +3849,7 @@
       </c>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -3780,7 +3861,7 @@
       </c>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -3792,7 +3873,7 @@
       </c>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>113</v>
       </c>
@@ -3804,7 +3885,7 @@
       </c>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>115</v>
       </c>
@@ -3816,7 +3897,7 @@
       </c>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>116</v>
       </c>
@@ -3828,7 +3909,7 @@
       </c>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>117</v>
       </c>
@@ -3840,7 +3921,7 @@
       </c>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>119</v>
       </c>
@@ -3852,7 +3933,7 @@
       </c>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>125</v>
       </c>
@@ -3864,7 +3945,7 @@
       </c>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>126</v>
       </c>
@@ -3876,7 +3957,7 @@
       </c>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>127</v>
       </c>
@@ -3888,7 +3969,7 @@
       </c>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>128</v>
       </c>
@@ -3900,7 +3981,7 @@
       </c>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>129</v>
       </c>
@@ -3912,7 +3993,7 @@
       </c>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>130</v>
       </c>
@@ -3924,7 +4005,7 @@
       </c>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>131</v>
       </c>
@@ -3936,7 +4017,7 @@
       </c>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>132</v>
       </c>
@@ -3948,7 +4029,7 @@
       </c>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>133</v>
       </c>
@@ -3960,7 +4041,7 @@
       </c>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>134</v>
       </c>
@@ -3972,7 +4053,7 @@
       </c>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>138</v>
       </c>
@@ -3984,7 +4065,7 @@
       </c>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -3996,7 +4077,7 @@
       </c>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -4008,7 +4089,7 @@
       </c>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>150</v>
       </c>
@@ -4020,7 +4101,7 @@
       </c>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -4032,7 +4113,7 @@
       </c>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -4044,7 +4125,7 @@
       </c>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -4056,7 +4137,7 @@
       </c>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>154</v>
       </c>
@@ -4068,7 +4149,7 @@
       </c>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>155</v>
       </c>
@@ -4080,7 +4161,7 @@
       </c>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>156</v>
       </c>
@@ -4092,7 +4173,7 @@
       </c>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>157</v>
       </c>
@@ -4104,7 +4185,7 @@
       </c>
       <c r="G48" s="5"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>158</v>
       </c>
@@ -4116,7 +4197,7 @@
       </c>
       <c r="G49" s="5"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>159</v>
       </c>
@@ -4128,7 +4209,7 @@
       </c>
       <c r="G50" s="5"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>160</v>
       </c>
@@ -4140,7 +4221,7 @@
       </c>
       <c r="G51" s="5"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>162</v>
       </c>
@@ -4152,7 +4233,7 @@
       </c>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>163</v>
       </c>
@@ -4164,7 +4245,7 @@
       </c>
       <c r="G53" s="5"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>164</v>
       </c>
@@ -4176,7 +4257,7 @@
       </c>
       <c r="G54" s="5"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>165</v>
       </c>
@@ -4188,7 +4269,7 @@
       </c>
       <c r="G55" s="5"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>101</v>
       </c>
@@ -4200,7 +4281,7 @@
       </c>
       <c r="G56" s="5"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>103</v>
       </c>
@@ -4212,7 +4293,7 @@
       </c>
       <c r="G57" s="5"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>53</v>
       </c>
@@ -4224,7 +4305,7 @@
       </c>
       <c r="G58" s="5"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>54</v>
       </c>
@@ -4236,7 +4317,7 @@
       </c>
       <c r="G59" s="5"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>169</v>
       </c>
@@ -4248,7 +4329,7 @@
       </c>
       <c r="G60" s="5"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -4260,7 +4341,7 @@
       </c>
       <c r="G61" s="5"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>137</v>
       </c>
@@ -4272,7 +4353,7 @@
       </c>
       <c r="G62" s="5"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>66</v>
       </c>
@@ -4284,7 +4365,7 @@
       </c>
       <c r="G63" s="5"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>77</v>
       </c>
@@ -4296,7 +4377,7 @@
       </c>
       <c r="G64" s="5"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>95</v>
       </c>
@@ -4308,7 +4389,7 @@
       </c>
       <c r="G65" s="5"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>135</v>
       </c>
@@ -4320,7 +4401,7 @@
       </c>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>166</v>
       </c>
@@ -4332,7 +4413,7 @@
       </c>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>23</v>
       </c>
@@ -4344,7 +4425,7 @@
       </c>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>34</v>
       </c>
@@ -4356,7 +4437,7 @@
       </c>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>36</v>
       </c>
@@ -4368,7 +4449,7 @@
       </c>
       <c r="G70" s="5"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -4380,7 +4461,7 @@
       </c>
       <c r="G71" s="5"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -4392,7 +4473,7 @@
       </c>
       <c r="G72" s="5"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>41</v>
       </c>
@@ -4404,7 +4485,7 @@
       </c>
       <c r="G73" s="5"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -4416,7 +4497,7 @@
       </c>
       <c r="G74" s="5"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>58</v>
       </c>
@@ -4428,7 +4509,7 @@
       </c>
       <c r="G75" s="5"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -4440,7 +4521,7 @@
       </c>
       <c r="G76" s="5"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>104</v>
       </c>
@@ -4452,7 +4533,7 @@
       </c>
       <c r="G77" s="5"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>109</v>
       </c>
@@ -4464,7 +4545,7 @@
       </c>
       <c r="G78" s="5"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>19</v>
       </c>
@@ -4476,7 +4557,7 @@
       </c>
       <c r="G79" s="5"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>26</v>
       </c>
@@ -4488,7 +4569,7 @@
       </c>
       <c r="G80" s="5"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>29</v>
       </c>
@@ -4500,7 +4581,7 @@
       </c>
       <c r="G81" s="5"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>60</v>
       </c>
@@ -4512,7 +4593,7 @@
       </c>
       <c r="G82" s="5"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>79</v>
       </c>
@@ -4524,7 +4605,7 @@
       </c>
       <c r="G83" s="5"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>93</v>
       </c>
@@ -4536,7 +4617,7 @@
       </c>
       <c r="G84" s="5"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>122</v>
       </c>
@@ -4548,7 +4629,7 @@
       </c>
       <c r="G85" s="5"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>136</v>
       </c>
@@ -4560,7 +4641,7 @@
       </c>
       <c r="G86" s="5"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>146</v>
       </c>
@@ -4572,7 +4653,7 @@
       </c>
       <c r="G87" s="5"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>33</v>
       </c>
@@ -4584,7 +4665,7 @@
       </c>
       <c r="G88" s="5"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -4596,7 +4677,7 @@
       </c>
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>145</v>
       </c>
@@ -4608,7 +4689,7 @@
       </c>
       <c r="G90" s="5"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>32</v>
       </c>
@@ -4620,7 +4701,7 @@
       </c>
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>35</v>
       </c>
@@ -4632,7 +4713,7 @@
       </c>
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>50</v>
       </c>
@@ -4644,7 +4725,7 @@
       </c>
       <c r="G93" s="5"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>82</v>
       </c>
@@ -4656,7 +4737,7 @@
       </c>
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>105</v>
       </c>
@@ -4668,7 +4749,7 @@
       </c>
       <c r="G95" s="5"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>112</v>
       </c>
@@ -4680,7 +4761,7 @@
       </c>
       <c r="G96" s="5"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>124</v>
       </c>
@@ -4692,7 +4773,7 @@
       </c>
       <c r="G97" s="5"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>31</v>
       </c>
@@ -4704,7 +4785,7 @@
       </c>
       <c r="G98" s="5"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>46</v>
       </c>
@@ -4716,7 +4797,7 @@
       </c>
       <c r="G99" s="5"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>57</v>
       </c>
@@ -4728,7 +4809,7 @@
       </c>
       <c r="G100" s="5"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>61</v>
       </c>
@@ -4740,7 +4821,7 @@
       </c>
       <c r="G101" s="5"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>89</v>
       </c>
@@ -4752,7 +4833,7 @@
       </c>
       <c r="G102" s="5"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>96</v>
       </c>
@@ -4764,7 +4845,7 @@
       </c>
       <c r="G103" s="5"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>97</v>
       </c>
@@ -4776,7 +4857,7 @@
       </c>
       <c r="G104" s="5"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>161</v>
       </c>
@@ -4788,7 +4869,7 @@
       </c>
       <c r="G105" s="5"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>21</v>
       </c>
@@ -4800,7 +4881,7 @@
       </c>
       <c r="G106" s="5"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>42</v>
       </c>
@@ -4812,7 +4893,7 @@
       </c>
       <c r="G107" s="5"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>90</v>
       </c>
@@ -4824,7 +4905,7 @@
       </c>
       <c r="G108" s="5"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>91</v>
       </c>
@@ -4836,7 +4917,7 @@
       </c>
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>94</v>
       </c>
@@ -4848,7 +4929,7 @@
       </c>
       <c r="G110" s="5"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>121</v>
       </c>
@@ -4860,7 +4941,7 @@
       </c>
       <c r="G111" s="5"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>168</v>
       </c>
@@ -4872,7 +4953,7 @@
       </c>
       <c r="G112" s="5"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>25</v>
       </c>
@@ -4884,7 +4965,7 @@
       </c>
       <c r="G113" s="5"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>37</v>
       </c>
@@ -4896,7 +4977,7 @@
       </c>
       <c r="G114" s="5"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>64</v>
       </c>
@@ -4908,7 +4989,7 @@
       </c>
       <c r="G115" s="5"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>72</v>
       </c>
@@ -4920,7 +5001,7 @@
       </c>
       <c r="G116" s="5"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>85</v>
       </c>
@@ -4932,7 +5013,7 @@
       </c>
       <c r="G117" s="5"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>86</v>
       </c>
@@ -4944,7 +5025,7 @@
       </c>
       <c r="G118" s="5"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>99</v>
       </c>
@@ -4956,7 +5037,7 @@
       </c>
       <c r="G119" s="5"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>106</v>
       </c>
@@ -4968,7 +5049,7 @@
       </c>
       <c r="G120" s="5"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>111</v>
       </c>
@@ -4980,7 +5061,7 @@
       </c>
       <c r="G121" s="5"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>141</v>
       </c>
@@ -4992,7 +5073,7 @@
       </c>
       <c r="G122" s="5"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>142</v>
       </c>
@@ -5004,7 +5085,7 @@
       </c>
       <c r="G123" s="5"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>144</v>
       </c>
@@ -5016,7 +5097,7 @@
       </c>
       <c r="G124" s="5"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>167</v>
       </c>
@@ -5028,7 +5109,7 @@
       </c>
       <c r="G125" s="5"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>49</v>
       </c>
@@ -5040,7 +5121,7 @@
       </c>
       <c r="G126" s="5"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>81</v>
       </c>
@@ -5052,7 +5133,7 @@
       </c>
       <c r="G127" s="5"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>107</v>
       </c>
@@ -5064,7 +5145,7 @@
       </c>
       <c r="G128" s="5"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>147</v>
       </c>
@@ -5076,7 +5157,7 @@
       </c>
       <c r="G129" s="5"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>40</v>
       </c>
@@ -5088,7 +5169,7 @@
       </c>
       <c r="G130" s="5"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>16</v>
       </c>
@@ -5100,7 +5181,7 @@
       </c>
       <c r="G131" s="5"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>20</v>
       </c>
@@ -5112,7 +5193,7 @@
       </c>
       <c r="G132" s="5"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>80</v>
       </c>
@@ -5124,7 +5205,7 @@
       </c>
       <c r="G133" s="5"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>84</v>
       </c>
@@ -5136,7 +5217,7 @@
       </c>
       <c r="G134" s="5"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>140</v>
       </c>
@@ -5148,7 +5229,7 @@
       </c>
       <c r="G135" s="5"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>24</v>
       </c>
@@ -5160,7 +5241,7 @@
       </c>
       <c r="G136" s="5"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>87</v>
       </c>
@@ -5172,7 +5253,7 @@
       </c>
       <c r="G137" s="5"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>110</v>
       </c>
@@ -5184,7 +5265,7 @@
       </c>
       <c r="G138" s="5"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>120</v>
       </c>
@@ -5196,7 +5277,7 @@
       </c>
       <c r="G139" s="5"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>123</v>
       </c>
@@ -5208,7 +5289,7 @@
       </c>
       <c r="G140" s="5"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>30</v>
       </c>
@@ -5220,7 +5301,7 @@
       </c>
       <c r="G141" s="5"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>114</v>
       </c>
@@ -5232,7 +5313,7 @@
       </c>
       <c r="G142" s="5"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>139</v>
       </c>
@@ -5244,7 +5325,7 @@
       </c>
       <c r="G143" s="5"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>118</v>
       </c>
@@ -5256,7 +5337,7 @@
       </c>
       <c r="G144" s="5"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>170</v>
       </c>
@@ -5268,7 +5349,7 @@
       </c>
       <c r="G145" s="5"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>67</v>
       </c>
@@ -5280,7 +5361,7 @@
       </c>
       <c r="G146" s="5"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>98</v>
       </c>
@@ -5292,7 +5373,7 @@
       </c>
       <c r="G147" s="5"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>75</v>
       </c>
@@ -5304,7 +5385,7 @@
       </c>
       <c r="G148" s="5"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>108</v>
       </c>
@@ -5316,7 +5397,7 @@
       </c>
       <c r="G149" s="5"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>92</v>
       </c>
@@ -5328,7 +5409,7 @@
       </c>
       <c r="G150" s="5"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>102</v>
       </c>
@@ -5340,7 +5421,7 @@
       </c>
       <c r="G151" s="5"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>143</v>
       </c>
@@ -5352,7 +5433,7 @@
       </c>
       <c r="G152" s="5"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>71</v>
       </c>
@@ -5364,7 +5445,7 @@
       </c>
       <c r="G153" s="5"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>100</v>
       </c>
@@ -5376,7 +5457,7 @@
       </c>
       <c r="G154" s="5"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>68</v>
       </c>
@@ -5388,7 +5469,7 @@
       </c>
       <c r="G155" s="5"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Moving to version 0.15.1
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D269CC7-BABF-473E-979D-CEB722C796F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C93B10B-5C51-452B-BA8C-D3AA7A20F913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -668,10 +668,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$18</c:f>
+              <c:f>Sheet1!$B$2:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -722,16 +722,19 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$18</c:f>
+              <c:f>Sheet1!$N$2:$N$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -782,6 +785,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>57.31707317073171</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>59.146341463414636</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -821,10 +827,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$18</c:f>
+              <c:f>Sheet1!$B$2:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -875,16 +881,19 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$18</c:f>
+              <c:f>Sheet1!$O$2:$O$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -935,6 +944,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>43.865435356200528</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45.609436435124508</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -974,10 +986,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$18</c:f>
+              <c:f>Sheet1!$B$2:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1028,16 +1040,19 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$18</c:f>
+              <c:f>Sheet1!$P$2:$P$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -1088,6 +1103,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>36.585365853658537</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40.853658536585364</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,10 +1145,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$18</c:f>
+              <c:f>Sheet1!$B$2:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1181,16 +1199,19 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$18</c:f>
+              <c:f>Sheet1!$Q$2:$Q$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1240,6 +1261,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -1280,10 +1304,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$18</c:f>
+              <c:f>Sheet1!$B$2:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1334,16 +1358,19 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$18</c:f>
+              <c:f>Sheet1!$R$2:$R$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -1394,6 +1421,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>38.967136150234744</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2508,7 +2538,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3518,7 +3548,59 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
+      <c r="A19" s="2">
+        <v>44098</v>
+      </c>
+      <c r="B19" s="4">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>164</v>
+      </c>
+      <c r="E19">
+        <v>97</v>
+      </c>
+      <c r="F19">
+        <v>1526</v>
+      </c>
+      <c r="G19">
+        <v>696</v>
+      </c>
+      <c r="H19">
+        <v>67</v>
+      </c>
+      <c r="I19">
+        <v>20</v>
+      </c>
+      <c r="J19">
+        <v>14</v>
+      </c>
+      <c r="K19">
+        <v>213</v>
+      </c>
+      <c r="L19">
+        <v>86</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" ref="N19" si="60">100*E19/D19</f>
+        <v>59.146341463414636</v>
+      </c>
+      <c r="O19" s="3">
+        <f t="shared" ref="O19" si="61">100*G19/F19</f>
+        <v>45.609436435124508</v>
+      </c>
+      <c r="P19" s="3">
+        <f t="shared" ref="P19" si="62">100*H19/D19</f>
+        <v>40.853658536585364</v>
+      </c>
+      <c r="Q19" s="3">
+        <f t="shared" ref="Q19" si="63">100*J19/I19</f>
+        <v>70</v>
+      </c>
+      <c r="R19" s="3">
+        <f t="shared" ref="R19" si="64">100*L19/K19</f>
+        <v>40.375586854460096</v>
+      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>

</xml_diff>

<commit_message>
Minor bug fixes and updated CoverageHistory.xlsx
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB363C1F-F7B6-4A8B-9E11-ADD2327D18C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D400EA-97B4-4B4B-B45C-53EC33F09FF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="174">
   <si>
     <t>Date</t>
   </si>
@@ -549,13 +549,13 @@
     <t>Fixed text condition</t>
   </si>
   <si>
-    <t>GUI condition</t>
-  </si>
-  <si>
-    <t>Module is enabled condition</t>
-  </si>
-  <si>
     <t>Workflow handling</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Convert image to objects</t>
   </si>
 </sst>
 </file>
@@ -677,10 +677,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$27</c:f>
+              <c:f>Sheet1!$B$2:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -758,16 +758,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$27</c:f>
+              <c:f>Sheet1!$N$2:$N$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -845,6 +848,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>64.024390243902445</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>64.848484848484844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -884,10 +890,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$27</c:f>
+              <c:f>Sheet1!$B$2:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -965,16 +971,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$27</c:f>
+              <c:f>Sheet1!$O$2:$O$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -1052,6 +1061,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>53.590078328981726</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>54.480052321778942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1091,10 +1103,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$27</c:f>
+              <c:f>Sheet1!$B$2:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1172,16 +1184,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$27</c:f>
+              <c:f>Sheet1!$P$2:$P$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -1259,6 +1274,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>51.829268292682926</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>52.727272727272727</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1298,10 +1316,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$27</c:f>
+              <c:f>Sheet1!$B$2:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1379,16 +1397,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$27</c:f>
+              <c:f>Sheet1!$Q$2:$Q$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1465,6 +1486,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -1505,10 +1529,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$27</c:f>
+              <c:f>Sheet1!$B$2:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1586,16 +1610,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$27</c:f>
+              <c:f>Sheet1!$R$2:$R$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -1672,6 +1699,9 @@
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>40.375586854460096</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
@@ -2787,7 +2817,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4292,7 +4322,59 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
+      <c r="A28" s="2">
+        <v>44118</v>
+      </c>
+      <c r="B28" s="4">
+        <v>27</v>
+      </c>
+      <c r="D28">
+        <v>165</v>
+      </c>
+      <c r="E28">
+        <v>107</v>
+      </c>
+      <c r="F28">
+        <v>1529</v>
+      </c>
+      <c r="G28">
+        <v>833</v>
+      </c>
+      <c r="H28">
+        <v>87</v>
+      </c>
+      <c r="I28">
+        <v>20</v>
+      </c>
+      <c r="J28">
+        <v>14</v>
+      </c>
+      <c r="K28">
+        <v>213</v>
+      </c>
+      <c r="L28">
+        <v>86</v>
+      </c>
+      <c r="N28" s="3">
+        <f t="shared" ref="N28" si="104">100*E28/D28</f>
+        <v>64.848484848484844</v>
+      </c>
+      <c r="O28" s="3">
+        <f t="shared" ref="O28" si="105">100*G28/F28</f>
+        <v>54.480052321778942</v>
+      </c>
+      <c r="P28" s="3">
+        <f t="shared" ref="P28" si="106">100*H28/D28</f>
+        <v>52.727272727272727</v>
+      </c>
+      <c r="Q28" s="3">
+        <f t="shared" ref="Q28" si="107">100*J28/I28</f>
+        <v>70</v>
+      </c>
+      <c r="R28" s="3">
+        <f t="shared" ref="R28" si="108">100*L28/K28</f>
+        <v>40.375586854460096</v>
+      </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
@@ -4345,15 +4427,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60F2A9E-CB35-4818-B2AA-21716033EEE9}">
   <dimension ref="A1:G159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4958,7 +5040,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>128</v>
+        <v>173</v>
       </c>
       <c r="B51" s="5">
         <v>1</v>
@@ -4970,7 +5052,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B52" s="5">
         <v>1</v>
@@ -4982,7 +5064,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B53" s="5">
         <v>1</v>
@@ -4994,7 +5076,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B54" s="5">
         <v>1</v>
@@ -5006,7 +5088,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B55" s="5">
         <v>1</v>
@@ -5018,7 +5100,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B56" s="5">
         <v>1</v>
@@ -5030,7 +5112,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B57" s="5">
         <v>1</v>
@@ -5042,7 +5124,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B58" s="5">
         <v>1</v>
@@ -5054,7 +5136,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B59" s="5">
         <v>1</v>
@@ -5066,7 +5148,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B60" s="5">
         <v>1</v>
@@ -5078,7 +5160,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B61" s="5">
         <v>1</v>
@@ -5090,7 +5172,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B62" s="5">
         <v>1</v>
@@ -5102,7 +5184,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B63" s="5">
         <v>1</v>
@@ -5114,7 +5196,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B64" s="5">
         <v>1</v>
@@ -5126,7 +5208,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B65" s="5">
         <v>1</v>
@@ -5138,7 +5220,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B66" s="5">
         <v>1</v>
@@ -5150,7 +5232,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B67" s="5">
         <v>1</v>
@@ -5162,7 +5244,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B68" s="5">
         <v>1</v>
@@ -5174,7 +5256,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B69" s="5">
         <v>1</v>
@@ -5186,7 +5268,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B70" s="5">
         <v>1</v>
@@ -5198,7 +5280,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B71" s="5">
         <v>1</v>
@@ -5210,7 +5292,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B72" s="5">
         <v>1</v>
@@ -5222,7 +5304,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B73" s="5">
         <v>1</v>
@@ -5234,7 +5316,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B74" s="5">
         <v>1</v>
@@ -5246,7 +5328,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B75" s="5">
         <v>1</v>
@@ -5258,7 +5340,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B76" s="5">
         <v>1</v>
@@ -5270,7 +5352,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B77" s="5">
         <v>1</v>
@@ -5282,7 +5364,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B78" s="5">
         <v>1</v>
@@ -5294,7 +5376,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B79" s="5">
         <v>1</v>
@@ -5306,7 +5388,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B80" s="5">
         <v>1</v>
@@ -5318,7 +5400,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B81" s="5">
         <v>1</v>
@@ -5330,7 +5412,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B82" s="5">
         <v>1</v>
@@ -5342,7 +5424,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B83" s="5">
         <v>1</v>
@@ -5354,7 +5436,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B84" s="5">
         <v>1</v>
@@ -5366,7 +5448,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B85" s="5">
         <v>1</v>
@@ -6038,7 +6120,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B141" s="5">
         <v>0</v>
@@ -6050,19 +6132,19 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>126</v>
+        <v>31</v>
       </c>
       <c r="B142" s="5">
         <v>0</v>
       </c>
       <c r="C142">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G142" s="5"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="B143" s="5">
         <v>0</v>
@@ -6074,10 +6156,10 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="B144" s="5">
-        <v>0</v>
+        <v>6.6699999999999995E-2</v>
       </c>
       <c r="C144">
         <v>14</v>
@@ -6086,19 +6168,19 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B145" s="5">
-        <v>6.6699999999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="C145">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G145" s="5"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="B146" s="5">
         <v>0</v>
@@ -6110,10 +6192,10 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="B147" s="5">
-        <v>0</v>
+        <v>0.1176</v>
       </c>
       <c r="C147">
         <v>15</v>
@@ -6122,19 +6204,19 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>173</v>
+        <v>68</v>
       </c>
       <c r="B148" s="5">
-        <v>0.1176</v>
+        <v>0</v>
       </c>
       <c r="C148">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G148" s="5"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="B149" s="5">
         <v>0</v>
@@ -6146,19 +6228,19 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="B150" s="5">
         <v>0</v>
       </c>
       <c r="C150">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G150" s="5"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="B151" s="5">
         <v>0</v>
@@ -6170,19 +6252,19 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B152" s="5">
         <v>0</v>
       </c>
       <c r="C152">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G152" s="5"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B153" s="5">
         <v>0</v>
@@ -6194,7 +6276,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>105</v>
+        <v>146</v>
       </c>
       <c r="B154" s="5">
         <v>0</v>
@@ -6206,19 +6288,19 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="B155" s="5">
         <v>0</v>
       </c>
       <c r="C155">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G155" s="5"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="B156" s="5">
         <v>0</v>
@@ -6230,43 +6312,42 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="B157" s="5">
         <v>0</v>
       </c>
       <c r="C157">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G157" s="5"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B158" s="5">
-        <v>0</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="C158">
-        <v>23</v>
-      </c>
-      <c r="G158" s="5"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A159" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B159" s="5">
-        <v>6.4500000000000002E-2</v>
-      </c>
-      <c r="C159">
-        <v>29</v>
+      <c r="A159" s="5">
+        <v>0</v>
+      </c>
+      <c r="B159" t="s">
+        <v>172</v>
+      </c>
+      <c r="C159" t="s">
+        <v>172</v>
       </c>
       <c r="G159" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C159">
-    <sortCondition ref="C1:C159"/>
+    <sortCondition ref="C2:C159"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added clickable links from GUI
References should now open in a web browser
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stephen\Java Projects\MIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986D8E41-94DC-4BF6-A020-53F36B1E8393}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3679F641-44B7-4273-9D0D-FBF5EA5F6AE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -680,10 +680,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$30</c:f>
+              <c:f>Sheet1!$B$2:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -770,16 +770,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$30</c:f>
+              <c:f>Sheet1!$N$2:$N$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -866,6 +869,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>67.878787878787875</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>68.07228915662651</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -905,10 +911,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$30</c:f>
+              <c:f>Sheet1!$B$2:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -995,16 +1001,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$30</c:f>
+              <c:f>Sheet1!$O$2:$O$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -1091,6 +1100,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>57.357750163505557</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>58.251793868232227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1130,10 +1142,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$30</c:f>
+              <c:f>Sheet1!$B$2:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1220,16 +1232,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$30</c:f>
+              <c:f>Sheet1!$P$2:$P$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -1316,6 +1331,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>55.757575757575758</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>56.024096385542165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1355,10 +1373,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$30</c:f>
+              <c:f>Sheet1!$B$2:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1445,16 +1463,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$30</c:f>
+              <c:f>Sheet1!$Q$2:$Q$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1540,6 +1561,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="28">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -1580,10 +1604,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$30</c:f>
+              <c:f>Sheet1!$B$2:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1670,16 +1694,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$30</c:f>
+              <c:f>Sheet1!$R$2:$R$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -1765,6 +1792,9 @@
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
                 <c:pt idx="28">
+                  <c:v>40.375586854460096</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
@@ -2020,10 +2050,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$30</c:f>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2110,16 +2140,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$30</c:f>
+              <c:f>Sheet1!$N$2:$N$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -2206,6 +2239,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>67.878787878787875</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>68.07228915662651</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2234,10 +2270,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$30</c:f>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2324,16 +2360,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$30</c:f>
+              <c:f>Sheet1!$O$2:$O$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -2420,6 +2459,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>57.357750163505557</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>58.251793868232227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2448,10 +2490,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$30</c:f>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2538,16 +2580,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$30</c:f>
+              <c:f>Sheet1!$P$2:$P$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -2634,6 +2679,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>55.757575757575758</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>56.024096385542165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2662,10 +2710,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$30</c:f>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2752,16 +2800,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$30</c:f>
+              <c:f>Sheet1!$Q$2:$Q$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2847,6 +2898,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="28">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -2876,10 +2930,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$30</c:f>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2966,16 +3020,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$30</c:f>
+              <c:f>Sheet1!$R$2:$R$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -3061,6 +3118,9 @@
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
                 <c:pt idx="28">
+                  <c:v>40.375586854460096</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
@@ -4779,8 +4839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6450,7 +6510,59 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
+      <c r="A31" s="2">
+        <v>44123</v>
+      </c>
+      <c r="B31" s="4">
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <v>166</v>
+      </c>
+      <c r="E31">
+        <v>113</v>
+      </c>
+      <c r="F31">
+        <v>1533</v>
+      </c>
+      <c r="G31">
+        <v>893</v>
+      </c>
+      <c r="H31">
+        <v>93</v>
+      </c>
+      <c r="I31">
+        <v>20</v>
+      </c>
+      <c r="J31">
+        <v>14</v>
+      </c>
+      <c r="K31">
+        <v>213</v>
+      </c>
+      <c r="L31">
+        <v>86</v>
+      </c>
+      <c r="N31" s="3">
+        <f t="shared" ref="N31" si="119">100*E31/D31</f>
+        <v>68.07228915662651</v>
+      </c>
+      <c r="O31" s="3">
+        <f t="shared" ref="O31" si="120">100*G31/F31</f>
+        <v>58.251793868232227</v>
+      </c>
+      <c r="P31" s="3">
+        <f t="shared" ref="P31" si="121">100*H31/D31</f>
+        <v>56.024096385542165</v>
+      </c>
+      <c r="Q31" s="3">
+        <f t="shared" ref="Q31" si="122">100*J31/I31</f>
+        <v>70</v>
+      </c>
+      <c r="R31" s="3">
+        <f t="shared" ref="R31" si="123">100*L31/K31</f>
+        <v>40.375586854460096</v>
+      </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>

</xml_diff>

<commit_message>
Testing methods for stack sorting
Need to get an image similarity metric working.  Currently testing alignment with SIFT, then calculating the cost.
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F852A3AC-42BC-4415-8508-0F7C47C28DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64487B19-726A-42D1-A079-AD3871B5DD56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
   <si>
     <t>Date</t>
   </si>
@@ -559,6 +559,12 @@
   </si>
   <si>
     <t>Module is enabled condition</t>
+  </si>
+  <si>
+    <t>Sort stack</t>
+  </si>
+  <si>
+    <t>Fill holes in objects</t>
   </si>
 </sst>
 </file>
@@ -680,10 +686,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$32</c:f>
+              <c:f>Sheet1!$B$2:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -776,16 +782,19 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$32</c:f>
+              <c:f>Sheet1!$N$2:$N$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -878,6 +887,9 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>68.674698795180717</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>70.059880239520965</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,10 +929,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$32</c:f>
+              <c:f>Sheet1!$B$2:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1013,16 +1025,19 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$32</c:f>
+              <c:f>Sheet1!$O$2:$O$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -1115,6 +1130,9 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>59.360730593607308</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>61.9140625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1154,10 +1172,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$32</c:f>
+              <c:f>Sheet1!$B$2:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1250,16 +1268,19 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$32</c:f>
+              <c:f>Sheet1!$P$2:$P$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -1352,6 +1373,9 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>56.626506024096386</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>58.08383233532934</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1391,10 +1415,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$32</c:f>
+              <c:f>Sheet1!$B$2:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1487,16 +1511,19 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$32</c:f>
+              <c:f>Sheet1!$Q$2:$Q$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1588,6 +1615,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -1628,10 +1658,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$32</c:f>
+              <c:f>Sheet1!$B$2:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1724,16 +1754,19 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$32</c:f>
+              <c:f>Sheet1!$R$2:$R$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -1825,6 +1858,9 @@
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>40.375586854460096</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
@@ -2080,10 +2116,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$32</c:f>
+              <c:f>Sheet1!$A$2:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2176,16 +2212,19 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>44124</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$32</c:f>
+              <c:f>Sheet1!$N$2:$N$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -2278,6 +2317,9 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>68.674698795180717</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>70.059880239520965</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2306,10 +2348,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$32</c:f>
+              <c:f>Sheet1!$A$2:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2402,16 +2444,19 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>44124</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$32</c:f>
+              <c:f>Sheet1!$O$2:$O$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -2504,6 +2549,9 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>59.360730593607308</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>61.9140625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2532,10 +2580,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$32</c:f>
+              <c:f>Sheet1!$A$2:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2628,16 +2676,19 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>44124</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$32</c:f>
+              <c:f>Sheet1!$P$2:$P$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -2730,6 +2781,9 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>56.626506024096386</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>58.08383233532934</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2758,10 +2812,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$32</c:f>
+              <c:f>Sheet1!$A$2:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2854,16 +2908,19 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>44124</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$32</c:f>
+              <c:f>Sheet1!$Q$2:$Q$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2955,6 +3012,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -2984,10 +3044,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$32</c:f>
+              <c:f>Sheet1!$A$2:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3080,16 +3140,19 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>44124</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$32</c:f>
+              <c:f>Sheet1!$R$2:$R$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -3181,6 +3244,9 @@
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>40.375586854460096</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
@@ -4900,8 +4966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O49" sqref="O49"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6680,31 +6746,83 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B33" s="4">
+        <v>32</v>
+      </c>
+      <c r="D33">
+        <v>167</v>
+      </c>
+      <c r="E33">
+        <v>117</v>
+      </c>
+      <c r="F33">
+        <v>1536</v>
+      </c>
+      <c r="G33">
+        <v>951</v>
+      </c>
+      <c r="H33">
+        <v>97</v>
+      </c>
+      <c r="I33">
+        <v>20</v>
+      </c>
+      <c r="J33">
+        <v>14</v>
+      </c>
+      <c r="K33">
+        <v>213</v>
+      </c>
+      <c r="L33">
+        <v>86</v>
+      </c>
+      <c r="N33" s="3">
+        <f t="shared" ref="N33" si="129">100*E33/D33</f>
+        <v>70.059880239520965</v>
+      </c>
+      <c r="O33" s="3">
+        <f t="shared" ref="O33" si="130">100*G33/F33</f>
+        <v>61.9140625</v>
+      </c>
+      <c r="P33" s="3">
+        <f t="shared" ref="P33" si="131">100*H33/D33</f>
+        <v>58.08383233532934</v>
+      </c>
+      <c r="Q33" s="3">
+        <f t="shared" ref="Q33" si="132">100*J33/I33</f>
+        <v>70</v>
+      </c>
+      <c r="R33" s="3">
+        <f t="shared" ref="R33" si="133">100*L33/K33</f>
+        <v>40.375586854460096</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
     </row>
   </sheetData>
@@ -6717,17 +6835,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60F2A9E-CB35-4818-B2AA-21716033EEE9}">
-  <dimension ref="A1:C160"/>
+  <dimension ref="A1:C162"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C135" sqref="A135:C135"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -6842,7 +6960,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
@@ -6853,7 +6971,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="5">
         <v>1</v>
@@ -6864,7 +6982,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -6875,7 +6993,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
@@ -6886,7 +7004,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
@@ -6897,7 +7015,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="5">
         <v>1</v>
@@ -6908,7 +7026,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B17" s="5">
         <v>1</v>
@@ -6919,7 +7037,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
@@ -6930,7 +7048,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="5">
         <v>1</v>
@@ -6941,7 +7059,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
@@ -6952,7 +7070,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" s="5">
         <v>1</v>
@@ -6963,7 +7081,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B22" s="5">
         <v>1</v>
@@ -6974,7 +7092,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B23" s="5">
         <v>1</v>
@@ -6985,7 +7103,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B24" s="5">
         <v>1</v>
@@ -6996,7 +7114,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B25" s="5">
         <v>1</v>
@@ -7007,7 +7125,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
@@ -7018,7 +7136,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B27" s="5">
         <v>1</v>
@@ -7029,7 +7147,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B28" s="5">
         <v>1</v>
@@ -7040,7 +7158,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B29" s="5">
         <v>1</v>
@@ -7051,7 +7169,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B30" s="5">
         <v>1</v>
@@ -7062,7 +7180,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B31" s="5">
         <v>1</v>
@@ -7073,7 +7191,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B32" s="5">
         <v>1</v>
@@ -7084,7 +7202,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B33" s="5">
         <v>1</v>
@@ -7095,7 +7213,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B34" s="5">
         <v>1</v>
@@ -7106,7 +7224,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B35" s="5">
         <v>1</v>
@@ -7117,7 +7235,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B36" s="5">
         <v>1</v>
@@ -7128,7 +7246,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B37" s="5">
         <v>1</v>
@@ -7139,7 +7257,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B38" s="5">
         <v>1</v>
@@ -7150,7 +7268,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B39" s="5">
         <v>1</v>
@@ -7161,7 +7279,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B40" s="5">
         <v>1</v>
@@ -7172,7 +7290,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B41" s="5">
         <v>1</v>
@@ -7183,7 +7301,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B42" s="5">
         <v>1</v>
@@ -7194,7 +7312,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B43" s="5">
         <v>1</v>
@@ -7205,7 +7323,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B44" s="5">
         <v>1</v>
@@ -7216,7 +7334,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B45" s="5">
         <v>1</v>
@@ -7227,7 +7345,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B46" s="5">
         <v>1</v>
@@ -7238,7 +7356,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B47" s="5">
         <v>1</v>
@@ -7249,7 +7367,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B48" s="5">
         <v>1</v>
@@ -7260,7 +7378,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B49" s="5">
         <v>1</v>
@@ -7271,7 +7389,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="B50" s="5">
         <v>1</v>
@@ -7282,7 +7400,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="B51" s="5">
         <v>1</v>
@@ -7293,7 +7411,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="B52" s="5">
         <v>1</v>
@@ -7304,7 +7422,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="B53" s="5">
         <v>1</v>
@@ -7315,7 +7433,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="B54" s="5">
         <v>1</v>
@@ -7326,7 +7444,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>172</v>
+        <v>106</v>
       </c>
       <c r="B55" s="5">
         <v>1</v>
@@ -7337,7 +7455,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B56" s="5">
         <v>1</v>
@@ -7348,7 +7466,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B57" s="5">
         <v>1</v>
@@ -7359,7 +7477,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B58" s="5">
         <v>1</v>
@@ -7370,7 +7488,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B59" s="5">
         <v>1</v>
@@ -7381,7 +7499,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B60" s="5">
         <v>1</v>
@@ -7392,7 +7510,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B61" s="5">
         <v>1</v>
@@ -7403,7 +7521,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B62" s="5">
         <v>1</v>
@@ -7414,7 +7532,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B63" s="5">
         <v>1</v>
@@ -7425,7 +7543,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B64" s="5">
         <v>1</v>
@@ -7436,7 +7554,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B65" s="5">
         <v>1</v>
@@ -7447,7 +7565,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B66" s="5">
         <v>1</v>
@@ -7458,7 +7576,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B67" s="5">
         <v>1</v>
@@ -7469,7 +7587,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B68" s="5">
         <v>1</v>
@@ -7480,7 +7598,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B69" s="5">
         <v>1</v>
@@ -7491,7 +7609,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B70" s="5">
         <v>1</v>
@@ -7502,7 +7620,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B71" s="5">
         <v>1</v>
@@ -7513,7 +7631,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="B72" s="5">
         <v>1</v>
@@ -7524,7 +7642,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B73" s="5">
         <v>1</v>
@@ -7535,7 +7653,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B74" s="5">
         <v>1</v>
@@ -7546,7 +7664,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B75" s="5">
         <v>1</v>
@@ -7557,7 +7675,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B76" s="5">
         <v>1</v>
@@ -7568,7 +7686,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B77" s="5">
         <v>1</v>
@@ -7579,7 +7697,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B78" s="5">
         <v>1</v>
@@ -7590,7 +7708,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B79" s="5">
         <v>1</v>
@@ -7601,7 +7719,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B80" s="5">
         <v>1</v>
@@ -7612,7 +7730,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B81" s="5">
         <v>1</v>
@@ -7623,7 +7741,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B82" s="5">
         <v>1</v>
@@ -7634,7 +7752,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B83" s="5">
         <v>1</v>
@@ -7645,7 +7763,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B84" s="5">
         <v>1</v>
@@ -7656,7 +7774,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B85" s="5">
         <v>1</v>
@@ -7667,7 +7785,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B86" s="5">
         <v>1</v>
@@ -7678,7 +7796,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B87" s="5">
         <v>1</v>
@@ -7689,7 +7807,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B88" s="5">
         <v>1</v>
@@ -7700,7 +7818,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B89" s="5">
         <v>1</v>
@@ -7711,7 +7829,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B90" s="5">
         <v>1</v>
@@ -7722,7 +7840,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B91" s="5">
         <v>1</v>
@@ -7733,7 +7851,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>47</v>
+        <v>167</v>
       </c>
       <c r="B92" s="5">
         <v>1</v>
@@ -7744,65 +7862,65 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>39</v>
+        <v>168</v>
       </c>
       <c r="B93" s="5">
-        <v>0.72729999999999995</v>
+        <v>1</v>
       </c>
       <c r="C93">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>40</v>
+        <v>169</v>
       </c>
       <c r="B94" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C94">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>42</v>
+        <v>170</v>
       </c>
       <c r="B95" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C95">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>49</v>
+        <v>173</v>
       </c>
       <c r="B96" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C96">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
-        <v>83</v>
+      <c r="A97" t="s">
+        <v>174</v>
       </c>
       <c r="B97" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="B98" s="5">
-        <v>0</v>
+        <v>0.72729999999999995</v>
       </c>
       <c r="C98">
         <v>3</v>
@@ -7810,7 +7928,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="B99" s="5">
         <v>0</v>
@@ -7821,73 +7939,73 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B100" s="5">
         <v>0</v>
       </c>
       <c r="C100">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="B101" s="5">
         <v>0</v>
       </c>
       <c r="C101">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>38</v>
+        <v>175</v>
       </c>
       <c r="B102" s="5">
-        <v>0.63639999999999997</v>
+        <v>0</v>
       </c>
       <c r="C102">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="B103" s="5">
         <v>0</v>
       </c>
       <c r="C103">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="B104" s="5">
         <v>0</v>
       </c>
       <c r="C104">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="B105" s="5">
         <v>0</v>
       </c>
       <c r="C105">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>149</v>
+        <v>27</v>
       </c>
       <c r="B106" s="5">
         <v>0</v>
@@ -7898,293 +8016,293 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B107" s="5">
         <v>0</v>
       </c>
       <c r="C107">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="B108" s="5">
-        <v>0</v>
+        <v>0.63639999999999997</v>
       </c>
       <c r="C108">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>148</v>
+        <v>61</v>
       </c>
       <c r="B109" s="5">
         <v>0</v>
       </c>
       <c r="C109">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>51</v>
+        <v>125</v>
       </c>
       <c r="B110" s="5">
         <v>0</v>
       </c>
       <c r="C110">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>82</v>
+        <v>176</v>
       </c>
       <c r="B111" s="5">
         <v>0</v>
       </c>
       <c r="C111">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="B112" s="5">
         <v>0</v>
       </c>
       <c r="C112">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>108</v>
+        <v>149</v>
       </c>
       <c r="B113" s="5">
         <v>0</v>
       </c>
       <c r="C113">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>115</v>
+        <v>34</v>
       </c>
       <c r="B114" s="5">
         <v>0</v>
       </c>
       <c r="C114">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="B115" s="5">
         <v>0</v>
       </c>
       <c r="C115">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="B116" s="5">
-        <v>0.36359999999999998</v>
+        <v>0</v>
       </c>
       <c r="C116">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B117" s="5">
         <v>0</v>
       </c>
       <c r="C117">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B118" s="5">
         <v>0</v>
       </c>
       <c r="C118">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B119" s="5">
         <v>0</v>
       </c>
       <c r="C119">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B120" s="5">
         <v>0</v>
       </c>
       <c r="C120">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>164</v>
+        <v>127</v>
       </c>
       <c r="B121" s="5">
         <v>0</v>
       </c>
       <c r="C121">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B122" s="5">
-        <v>0</v>
+        <v>0.36359999999999998</v>
       </c>
       <c r="C122">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B123" s="5">
         <v>0</v>
       </c>
       <c r="C123">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B124" s="5">
         <v>0</v>
       </c>
       <c r="C124">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B125" s="5">
         <v>0</v>
       </c>
       <c r="C125">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="B126" s="5">
         <v>0</v>
       </c>
       <c r="C126">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>26</v>
+        <v>164</v>
       </c>
       <c r="B127" s="5">
         <v>0</v>
       </c>
       <c r="C127">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="B128" s="5">
         <v>0</v>
       </c>
       <c r="C128">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="B129" s="5">
         <v>0</v>
       </c>
       <c r="C129">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B130" s="5">
         <v>0</v>
       </c>
       <c r="C130">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B131" s="5">
         <v>0</v>
       </c>
       <c r="C131">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="B132" s="5">
         <v>0</v>
       </c>
       <c r="C132">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="B133" s="5">
         <v>0</v>
@@ -8195,7 +8313,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="B134" s="5">
         <v>0</v>
@@ -8206,7 +8324,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>144</v>
+        <v>85</v>
       </c>
       <c r="B135" s="5">
         <v>0</v>
@@ -8217,7 +8335,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>145</v>
+        <v>86</v>
       </c>
       <c r="B136" s="5">
         <v>0</v>
@@ -8228,7 +8346,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>147</v>
+        <v>102</v>
       </c>
       <c r="B137" s="5">
         <v>0</v>
@@ -8239,260 +8357,282 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="B138" s="5">
         <v>0</v>
       </c>
       <c r="C138">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B139" s="5">
         <v>0</v>
       </c>
       <c r="C139">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B140" s="5">
         <v>0</v>
       </c>
       <c r="C140">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>84</v>
+        <v>145</v>
       </c>
       <c r="B141" s="5">
         <v>0</v>
       </c>
       <c r="C141">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="B142" s="5">
         <v>0</v>
       </c>
       <c r="C142">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="B143" s="5">
         <v>0</v>
       </c>
       <c r="C143">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="B144" s="5">
         <v>0</v>
       </c>
       <c r="C144">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>31</v>
+        <v>150</v>
       </c>
       <c r="B145" s="5">
         <v>0</v>
       </c>
       <c r="C145">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="B146" s="5">
-        <v>6.6699999999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="C146">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B147" s="5">
         <v>0</v>
       </c>
       <c r="C147">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="B148" s="5">
         <v>0</v>
       </c>
       <c r="C148">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>171</v>
+        <v>31</v>
       </c>
       <c r="B149" s="5">
-        <v>0.1176</v>
+        <v>0</v>
       </c>
       <c r="C149">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="B150" s="5">
-        <v>0</v>
+        <v>6.6699999999999995E-2</v>
       </c>
       <c r="C150">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="B151" s="5">
         <v>0</v>
       </c>
       <c r="C151">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="B152" s="5">
         <v>0</v>
       </c>
       <c r="C152">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="5" t="s">
-        <v>111</v>
+      <c r="A153" t="s">
+        <v>171</v>
       </c>
       <c r="B153" s="5">
-        <v>0</v>
+        <v>0.1176</v>
       </c>
       <c r="C153">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="B154" s="5">
         <v>0</v>
       </c>
       <c r="C154">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B155" s="5">
         <v>0</v>
       </c>
       <c r="C155">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>146</v>
+        <v>76</v>
       </c>
       <c r="B156" s="5">
         <v>0</v>
       </c>
       <c r="C156">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="B157" s="5">
         <v>0</v>
       </c>
       <c r="C157">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B158" s="5">
         <v>0</v>
       </c>
       <c r="C158">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="B159" s="5">
         <v>0</v>
       </c>
       <c r="C159">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B160" s="5">
-        <v>6.9000000000000006E-2</v>
+        <v>0</v>
       </c>
       <c r="C160">
-        <v>27</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B161" s="5">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B162" s="5">
+        <v>0</v>
+      </c>
+      <c r="C162">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C160">
-    <sortCondition ref="C111:C160"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C162">
+    <sortCondition ref="C2:C162"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added coordinate set duplication to CombineObjectSets
Previously, the objects copied to another set shared a coordinate set with the original object.  This could lead to problems, so now it duplicates first.
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FF0976-A5A8-4BEA-932F-A7EE2B0831A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC460DB6-C692-4BCD-AF41-80A8B87E672E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="480" yWindow="-108" windowWidth="22668" windowHeight="13176" activeTab="1" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5083,32 +5083,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44054</v>
       </c>
@@ -5211,7 +5211,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44055</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44056</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44057</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44058</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>44064</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>44069</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>44070</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44081</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44082</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44083</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44084</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44085</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44089</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>44090</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44091</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>44097</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>38.967136150234744</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>44098</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>44099</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>44102</v>
       </c>
@@ -6258,7 +6258,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>44103</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>44104</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>44110</v>
       </c>
@@ -6423,7 +6423,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>44113</v>
       </c>
@@ -6478,7 +6478,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>44116</v>
       </c>
@@ -6533,7 +6533,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>44117</v>
       </c>
@@ -6588,7 +6588,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>44118</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>44119</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>44120</v>
       </c>
@@ -6753,7 +6753,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>44123</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>44124</v>
       </c>
@@ -6863,7 +6863,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>44125</v>
       </c>
@@ -6918,7 +6918,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>44126</v>
       </c>
@@ -6973,7 +6973,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>44127</v>
       </c>
@@ -7028,22 +7028,22 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B41" s="4"/>
     </row>
   </sheetData>
@@ -7058,18 +7058,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60F2A9E-CB35-4818-B2AA-21716033EEE9}">
   <dimension ref="A1:C162"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G106" sqref="G106"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L90" sqref="L90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
@@ -7080,7 +7080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -7091,7 +7091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -7113,7 +7113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -7124,7 +7124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -7135,7 +7135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -7201,7 +7201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
@@ -7223,7 +7223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
@@ -7234,7 +7234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -7245,7 +7245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>41</v>
       </c>
@@ -7267,7 +7267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>44</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>45</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
@@ -7300,7 +7300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>47</v>
       </c>
@@ -7311,7 +7311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>48</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>52</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>53</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>54</v>
       </c>
@@ -7355,7 +7355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>55</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>56</v>
       </c>
@@ -7377,7 +7377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>57</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>59</v>
       </c>
@@ -7399,7 +7399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>60</v>
       </c>
@@ -7410,7 +7410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>62</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>63</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>64</v>
       </c>
@@ -7443,7 +7443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>66</v>
       </c>
@@ -7454,7 +7454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>67</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>70</v>
       </c>
@@ -7476,7 +7476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>71</v>
       </c>
@@ -7487,7 +7487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>74</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>75</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>77</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>78</v>
       </c>
@@ -7531,7 +7531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>79</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>80</v>
       </c>
@@ -7553,7 +7553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>81</v>
       </c>
@@ -7564,7 +7564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>82</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>87</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>92</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>93</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>94</v>
       </c>
@@ -7619,7 +7619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>95</v>
       </c>
@@ -7630,7 +7630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>96</v>
       </c>
@@ -7641,7 +7641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>97</v>
       </c>
@@ -7652,7 +7652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>98</v>
       </c>
@@ -7663,7 +7663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>99</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>100</v>
       </c>
@@ -7685,7 +7685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>102</v>
       </c>
@@ -7696,7 +7696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>104</v>
       </c>
@@ -7707,7 +7707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>106</v>
       </c>
@@ -7718,7 +7718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>112</v>
       </c>
@@ -7729,7 +7729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>116</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>118</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>119</v>
       </c>
@@ -7762,7 +7762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>120</v>
       </c>
@@ -7773,7 +7773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>122</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>172</v>
       </c>
@@ -7795,7 +7795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>123</v>
       </c>
@@ -7806,7 +7806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>128</v>
       </c>
@@ -7817,7 +7817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>129</v>
       </c>
@@ -7828,7 +7828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>130</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>131</v>
       </c>
@@ -7850,7 +7850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>132</v>
       </c>
@@ -7861,7 +7861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>133</v>
       </c>
@@ -7872,7 +7872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>134</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>135</v>
       </c>
@@ -7894,7 +7894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>136</v>
       </c>
@@ -7905,7 +7905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>137</v>
       </c>
@@ -7916,7 +7916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>138</v>
       </c>
@@ -7927,7 +7927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>140</v>
       </c>
@@ -7938,7 +7938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>141</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>143</v>
       </c>
@@ -7960,7 +7960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>151</v>
       </c>
@@ -7971,7 +7971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>152</v>
       </c>
@@ -7982,7 +7982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>153</v>
       </c>
@@ -7993,7 +7993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>154</v>
       </c>
@@ -8004,7 +8004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>155</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>156</v>
       </c>
@@ -8026,7 +8026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>157</v>
       </c>
@@ -8037,7 +8037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>158</v>
       </c>
@@ -8048,7 +8048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>159</v>
       </c>
@@ -8059,7 +8059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>160</v>
       </c>
@@ -8070,7 +8070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>161</v>
       </c>
@@ -8081,7 +8081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>162</v>
       </c>
@@ -8092,7 +8092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>163</v>
       </c>
@@ -8103,7 +8103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>165</v>
       </c>
@@ -8114,7 +8114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>166</v>
       </c>
@@ -8125,7 +8125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>167</v>
       </c>
@@ -8136,7 +8136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>168</v>
       </c>
@@ -8147,7 +8147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>169</v>
       </c>
@@ -8158,7 +8158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>170</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>173</v>
       </c>
@@ -8180,7 +8180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>174</v>
       </c>
@@ -8191,7 +8191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>39</v>
       </c>
@@ -8202,7 +8202,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>40</v>
       </c>
@@ -8213,7 +8213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>42</v>
       </c>
@@ -8224,18 +8224,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B106" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C106">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>83</v>
       </c>
@@ -8246,7 +8246,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>107</v>
       </c>
@@ -8257,7 +8257,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>27</v>
       </c>
@@ -8268,7 +8268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>30</v>
       </c>
@@ -8279,7 +8279,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>38</v>
       </c>
@@ -8290,7 +8290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>61</v>
       </c>
@@ -8301,7 +8301,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>125</v>
       </c>
@@ -8312,7 +8312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>175</v>
       </c>
@@ -8323,7 +8323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>139</v>
       </c>
@@ -8334,7 +8334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>149</v>
       </c>
@@ -8345,7 +8345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>34</v>
       </c>
@@ -8356,7 +8356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>88</v>
       </c>
@@ -8367,7 +8367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>148</v>
       </c>
@@ -8378,7 +8378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>51</v>
       </c>
@@ -8389,7 +8389,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>108</v>
       </c>
@@ -8400,7 +8400,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>115</v>
       </c>
@@ -8411,7 +8411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>127</v>
       </c>
@@ -8422,7 +8422,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>32</v>
       </c>
@@ -8433,7 +8433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>58</v>
       </c>
@@ -8444,7 +8444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>89</v>
       </c>
@@ -8455,7 +8455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>164</v>
       </c>
@@ -8466,7 +8466,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>22</v>
       </c>
@@ -8477,7 +8477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>43</v>
       </c>
@@ -8488,7 +8488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>90</v>
       </c>
@@ -8499,7 +8499,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>91</v>
       </c>
@@ -8510,7 +8510,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>124</v>
       </c>
@@ -8521,7 +8521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>65</v>
       </c>
@@ -8532,7 +8532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>73</v>
       </c>
@@ -8543,7 +8543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>85</v>
       </c>
@@ -8554,7 +8554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>86</v>
       </c>
@@ -8565,7 +8565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>109</v>
       </c>
@@ -8576,7 +8576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>114</v>
       </c>
@@ -8587,7 +8587,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>144</v>
       </c>
@@ -8598,7 +8598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>145</v>
       </c>
@@ -8609,7 +8609,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>147</v>
       </c>
@@ -8620,7 +8620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>50</v>
       </c>
@@ -8631,7 +8631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>110</v>
       </c>
@@ -8642,7 +8642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>150</v>
       </c>
@@ -8653,7 +8653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>84</v>
       </c>
@@ -8664,7 +8664,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>113</v>
       </c>
@@ -8675,7 +8675,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>126</v>
       </c>
@@ -8686,7 +8686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>31</v>
       </c>
@@ -8697,7 +8697,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>117</v>
       </c>
@@ -8708,7 +8708,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>121</v>
       </c>
@@ -8719,7 +8719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>142</v>
       </c>
@@ -8730,7 +8730,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>171</v>
       </c>
@@ -8741,7 +8741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>68</v>
       </c>
@@ -8752,7 +8752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>101</v>
       </c>
@@ -8763,7 +8763,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>76</v>
       </c>
@@ -8774,7 +8774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>111</v>
       </c>
@@ -8785,7 +8785,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>105</v>
       </c>
@@ -8796,7 +8796,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>146</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>72</v>
       </c>
@@ -8818,7 +8818,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>103</v>
       </c>
@@ -8829,7 +8829,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>69</v>
       </c>
@@ -8840,7 +8840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started adding multidimensional stack support for registration
This will see the registration module split in two (automatic and
manual).
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Java Projects\MIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDDB2ED-25CA-4CBE-B598-97FAE55E47B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E522C5-7FA5-42A5-9BEC-F0439CD20D7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="-108" windowWidth="22668" windowHeight="13176" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -683,10 +683,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$37</c:f>
+              <c:f>Sheet1!$B$2:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -794,16 +794,19 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$37</c:f>
+              <c:f>Sheet1!$N$2:$N$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -911,6 +914,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>75.301204819277103</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>77.108433734939766</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -950,10 +956,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$37</c:f>
+              <c:f>Sheet1!$B$2:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1061,16 +1067,19 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$37</c:f>
+              <c:f>Sheet1!$O$2:$O$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -1178,6 +1187,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>64.986910994764401</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>65.903141361256544</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1217,10 +1229,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$37</c:f>
+              <c:f>Sheet1!$B$2:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1328,16 +1340,19 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$37</c:f>
+              <c:f>Sheet1!$P$2:$P$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -1445,6 +1460,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>63.855421686746986</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>65.662650602409641</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1484,10 +1502,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$37</c:f>
+              <c:f>Sheet1!$B$2:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1595,16 +1613,19 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$37</c:f>
+              <c:f>Sheet1!$Q$2:$Q$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1711,6 +1732,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="35">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -1751,10 +1775,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$37</c:f>
+              <c:f>Sheet1!$B$2:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1862,16 +1886,19 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$37</c:f>
+              <c:f>Sheet1!$R$2:$R$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -1978,6 +2005,9 @@
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
                 <c:pt idx="35">
+                  <c:v>40.375586854460096</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
@@ -2233,10 +2263,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:f>Sheet1!$A$2:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2344,16 +2374,19 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>44131</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$37</c:f>
+              <c:f>Sheet1!$N$2:$N$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -2461,6 +2494,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>75.301204819277103</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>77.108433734939766</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2489,10 +2525,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:f>Sheet1!$A$2:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2600,16 +2636,19 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>44131</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$37</c:f>
+              <c:f>Sheet1!$O$2:$O$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -2717,6 +2756,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>64.986910994764401</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>65.903141361256544</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2745,10 +2787,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:f>Sheet1!$A$2:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2856,16 +2898,19 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>44131</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$37</c:f>
+              <c:f>Sheet1!$P$2:$P$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -2973,6 +3018,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>63.855421686746986</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>65.662650602409641</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3001,10 +3049,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:f>Sheet1!$A$2:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3112,16 +3160,19 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>44131</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$37</c:f>
+              <c:f>Sheet1!$Q$2:$Q$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -3228,6 +3279,9 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="35">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
@@ -3257,10 +3311,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:f>Sheet1!$A$2:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3368,16 +3422,19 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>44131</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$37</c:f>
+              <c:f>Sheet1!$R$2:$R$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -3484,6 +3541,9 @@
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
                 <c:pt idx="35">
+                  <c:v>40.375586854460096</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
@@ -5203,32 +5263,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5275,7 +5335,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44054</v>
       </c>
@@ -5331,7 +5391,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44055</v>
       </c>
@@ -5387,7 +5447,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44056</v>
       </c>
@@ -5443,7 +5503,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44057</v>
       </c>
@@ -5498,7 +5558,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44058</v>
       </c>
@@ -5553,7 +5613,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44064</v>
       </c>
@@ -5608,7 +5668,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44069</v>
       </c>
@@ -5663,7 +5723,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44070</v>
       </c>
@@ -5718,7 +5778,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44081</v>
       </c>
@@ -5773,7 +5833,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44082</v>
       </c>
@@ -5828,7 +5888,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44083</v>
       </c>
@@ -5883,7 +5943,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44084</v>
       </c>
@@ -5938,7 +5998,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44085</v>
       </c>
@@ -5993,7 +6053,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44089</v>
       </c>
@@ -6048,7 +6108,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44090</v>
       </c>
@@ -6103,7 +6163,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44091</v>
       </c>
@@ -6158,7 +6218,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44097</v>
       </c>
@@ -6213,7 +6273,7 @@
         <v>38.967136150234744</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44098</v>
       </c>
@@ -6268,7 +6328,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44099</v>
       </c>
@@ -6323,7 +6383,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44102</v>
       </c>
@@ -6378,7 +6438,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44103</v>
       </c>
@@ -6433,7 +6493,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44104</v>
       </c>
@@ -6488,7 +6548,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44110</v>
       </c>
@@ -6543,7 +6603,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44113</v>
       </c>
@@ -6598,7 +6658,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44116</v>
       </c>
@@ -6653,7 +6713,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44117</v>
       </c>
@@ -6708,7 +6768,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44118</v>
       </c>
@@ -6763,7 +6823,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44119</v>
       </c>
@@ -6818,7 +6878,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44120</v>
       </c>
@@ -6873,7 +6933,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44123</v>
       </c>
@@ -6928,7 +6988,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44124</v>
       </c>
@@ -6983,7 +7043,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44125</v>
       </c>
@@ -7038,7 +7098,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44126</v>
       </c>
@@ -7093,7 +7153,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44127</v>
       </c>
@@ -7148,7 +7208,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44130</v>
       </c>
@@ -7203,7 +7263,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44131</v>
       </c>
@@ -7258,17 +7318,69 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B38" s="4"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>44132</v>
+      </c>
+      <c r="B38" s="4">
+        <v>37</v>
+      </c>
+      <c r="D38">
+        <v>166</v>
+      </c>
+      <c r="E38">
+        <v>128</v>
+      </c>
+      <c r="F38">
+        <v>1528</v>
+      </c>
+      <c r="G38">
+        <v>1007</v>
+      </c>
+      <c r="H38">
+        <v>109</v>
+      </c>
+      <c r="I38">
+        <v>20</v>
+      </c>
+      <c r="J38">
+        <v>14</v>
+      </c>
+      <c r="K38">
+        <v>213</v>
+      </c>
+      <c r="L38">
+        <v>86</v>
+      </c>
+      <c r="N38" s="3">
+        <f t="shared" ref="N38" si="154">100*E38/D38</f>
+        <v>77.108433734939766</v>
+      </c>
+      <c r="O38" s="3">
+        <f t="shared" ref="O38" si="155">100*G38/F38</f>
+        <v>65.903141361256544</v>
+      </c>
+      <c r="P38" s="3">
+        <f t="shared" ref="P38" si="156">100*H38/D38</f>
+        <v>65.662650602409641</v>
+      </c>
+      <c r="Q38" s="3">
+        <f t="shared" ref="Q38" si="157">100*J38/I38</f>
+        <v>70</v>
+      </c>
+      <c r="R38" s="3">
+        <f t="shared" ref="R38" si="158">100*L38/K38</f>
+        <v>40.375586854460096</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
       <c r="P39" s="3"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
     </row>
   </sheetData>
@@ -7281,20 +7393,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60F2A9E-CB35-4818-B2AA-21716033EEE9}">
-  <dimension ref="A1:C162"/>
+  <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109:XFD109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
@@ -7305,7 +7417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -7316,7 +7428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -7327,7 +7439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -7338,7 +7450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -7349,7 +7461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -7360,7 +7472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
@@ -7371,7 +7483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
@@ -7382,7 +7494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
@@ -7393,7 +7505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
@@ -7404,7 +7516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -7415,7 +7527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -7426,7 +7538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
@@ -7437,7 +7549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
@@ -7448,1065 +7560,1065 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="5">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="5">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="5">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="5">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="5">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="5">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="B23" s="5">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="5">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="5">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="B25" s="5">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="5">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="5">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="5">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="5">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="5">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="5">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="B32" s="5">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="5">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="B33" s="5">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="5">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="B34" s="5">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="5">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="5">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="B36" s="5">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="5">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="B37" s="5">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="5">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="B38" s="5">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="5">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+      <c r="B39" s="5">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="5">
-        <v>1</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="B40" s="5">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="5">
-        <v>1</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="B41" s="5">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="5">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+      <c r="B42" s="5">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="5">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+      <c r="B43" s="5">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="5">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="B44" s="5">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="5">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+      <c r="B45" s="5">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="5">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+      <c r="B46" s="5">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="5">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+      <c r="B47" s="5">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="5">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+      <c r="B48" s="5">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B45" s="5">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+      <c r="B49" s="5">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="5">
-        <v>1</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+      <c r="B50" s="5">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B47" s="5">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+      <c r="B51" s="5">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="5">
-        <v>1</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
+      <c r="B52" s="5">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="5">
-        <v>1</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+      <c r="B53" s="5">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="5">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+      <c r="B54" s="5">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="5">
-        <v>1</v>
-      </c>
-      <c r="C51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+      <c r="B55" s="5">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B52" s="5">
-        <v>1</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
+      <c r="B56" s="5">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B53" s="5">
-        <v>1</v>
-      </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
+      <c r="B57" s="5">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="5">
-        <v>1</v>
-      </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
+      <c r="B58" s="5">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B55" s="5">
-        <v>1</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
+      <c r="B59" s="5">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B56" s="5">
-        <v>1</v>
-      </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
+      <c r="B60" s="5">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B57" s="5">
-        <v>1</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
+      <c r="B61" s="5">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B58" s="5">
-        <v>1</v>
-      </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
+      <c r="B62" s="5">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B59" s="5">
-        <v>1</v>
-      </c>
-      <c r="C59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
+      <c r="B63" s="5">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B60" s="5">
-        <v>1</v>
-      </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
+      <c r="B64" s="5">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B61" s="5">
-        <v>1</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
+      <c r="B65" s="5">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B62" s="5">
-        <v>1</v>
-      </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
+      <c r="B66" s="5">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="5">
-        <v>1</v>
-      </c>
-      <c r="C63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
+      <c r="B67" s="5">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B64" s="5">
-        <v>1</v>
-      </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
+      <c r="B68" s="5">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B65" s="5">
-        <v>1</v>
-      </c>
-      <c r="C65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="5" t="s">
+      <c r="B69" s="5">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B66" s="5">
-        <v>1</v>
-      </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="5" t="s">
+      <c r="B70" s="5">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B67" s="5">
-        <v>1</v>
-      </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
+      <c r="B71" s="5">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B72" s="5">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B73" s="5">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B74" s="5">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B68" s="5">
-        <v>1</v>
-      </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
+      <c r="B75" s="5">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B69" s="5">
-        <v>1</v>
-      </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
+      <c r="B76" s="5">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B70" s="5">
-        <v>1</v>
-      </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
+      <c r="B77" s="5">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B71" s="5">
-        <v>1</v>
-      </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="5" t="s">
+      <c r="B78" s="5">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B72" s="5">
-        <v>1</v>
-      </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="5" t="s">
+      <c r="B79" s="5">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B73" s="5">
-        <v>1</v>
-      </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="5" t="s">
+      <c r="B80" s="5">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B74" s="5">
-        <v>1</v>
-      </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="5" t="s">
+      <c r="B81" s="5">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B75" s="5">
-        <v>1</v>
-      </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
+      <c r="B82" s="5">
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B76" s="5">
-        <v>1</v>
-      </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="5" t="s">
+      <c r="B83" s="5">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B77" s="5">
-        <v>1</v>
-      </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="5" t="s">
+      <c r="B84" s="5">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B78" s="5">
-        <v>1</v>
-      </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="5" t="s">
+      <c r="B85" s="5">
+        <v>1</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B79" s="5">
-        <v>1</v>
-      </c>
-      <c r="C79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="5" t="s">
+      <c r="B86" s="5">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B80" s="5">
-        <v>1</v>
-      </c>
-      <c r="C80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="5" t="s">
+      <c r="B87" s="5">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B81" s="5">
-        <v>1</v>
-      </c>
-      <c r="C81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="5" t="s">
+      <c r="B88" s="5">
+        <v>1</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B82" s="5">
-        <v>1</v>
-      </c>
-      <c r="C82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="5" t="s">
+      <c r="B89" s="5">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B83" s="5">
-        <v>1</v>
-      </c>
-      <c r="C83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="5" t="s">
+      <c r="B90" s="5">
+        <v>1</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B84" s="5">
-        <v>1</v>
-      </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="5" t="s">
+      <c r="B91" s="5">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B85" s="5">
-        <v>1</v>
-      </c>
-      <c r="C85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="5" t="s">
+      <c r="B92" s="5">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B86" s="5">
-        <v>1</v>
-      </c>
-      <c r="C86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="5" t="s">
+      <c r="B93" s="5">
+        <v>1</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B87" s="5">
-        <v>1</v>
-      </c>
-      <c r="C87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="5" t="s">
+      <c r="B94" s="5">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B88" s="5">
-        <v>1</v>
-      </c>
-      <c r="C88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="5" t="s">
+      <c r="B95" s="5">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B89" s="5">
-        <v>1</v>
-      </c>
-      <c r="C89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" s="5" t="s">
+      <c r="B96" s="5">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B90" s="5">
-        <v>1</v>
-      </c>
-      <c r="C90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="5" t="s">
+      <c r="B97" s="5">
+        <v>1</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B91" s="5">
-        <v>1</v>
-      </c>
-      <c r="C91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="5" t="s">
+      <c r="B98" s="5">
+        <v>1</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B92" s="5">
-        <v>1</v>
-      </c>
-      <c r="C92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="5" t="s">
+      <c r="B99" s="5">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B93" s="5">
-        <v>1</v>
-      </c>
-      <c r="C93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="5" t="s">
+      <c r="B100" s="5">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B94" s="5">
-        <v>1</v>
-      </c>
-      <c r="C94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="5" t="s">
+      <c r="B101" s="5">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B95" s="5">
-        <v>1</v>
-      </c>
-      <c r="C95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="5" t="s">
+      <c r="B102" s="5">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B96" s="5">
-        <v>1</v>
-      </c>
-      <c r="C96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="5" t="s">
+      <c r="B103" s="5">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B97" s="5">
-        <v>1</v>
-      </c>
-      <c r="C97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="5" t="s">
+      <c r="B104" s="5">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B98" s="5">
-        <v>1</v>
-      </c>
-      <c r="C98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="5" t="s">
+      <c r="B105" s="5">
+        <v>1</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B99" s="5">
-        <v>1</v>
-      </c>
-      <c r="C99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="5" t="s">
+      <c r="B106" s="5">
+        <v>1</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B100" s="5">
-        <v>1</v>
-      </c>
-      <c r="C100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="5" t="s">
+      <c r="B107" s="5">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B101" s="5">
-        <v>1</v>
-      </c>
-      <c r="C101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="5" t="s">
+      <c r="B108" s="5">
+        <v>1</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B102" s="5">
-        <v>1</v>
-      </c>
-      <c r="C102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B103" s="5">
-        <v>1</v>
-      </c>
-      <c r="C103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B104" s="5">
-        <v>1</v>
-      </c>
-      <c r="C104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B105" s="5">
-        <v>1</v>
-      </c>
-      <c r="C105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B106" s="5">
-        <v>1</v>
-      </c>
-      <c r="C106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="5" t="s">
+      <c r="B109" s="5">
+        <v>1</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B107" s="5">
+      <c r="B110" s="5">
         <v>0.72729999999999995</v>
-      </c>
-      <c r="C107">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B108" s="5">
-        <v>0</v>
-      </c>
-      <c r="C108">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B109" s="5">
-        <v>0</v>
-      </c>
-      <c r="C109">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B110" s="5">
-        <v>0</v>
       </c>
       <c r="C110">
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>107</v>
+        <v>42</v>
       </c>
       <c r="B111" s="5">
         <v>0</v>
@@ -8515,42 +8627,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B112" s="5">
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B113" s="5">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B112" s="5">
-        <v>0</v>
-      </c>
-      <c r="C112">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B113" s="5">
-        <v>0</v>
-      </c>
-      <c r="C113">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="B114" s="5">
-        <v>0.63639999999999997</v>
+        <v>0</v>
       </c>
       <c r="C114">
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
       <c r="B115" s="5">
         <v>0</v>
@@ -8559,42 +8671,42 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>149</v>
+        <v>38</v>
       </c>
       <c r="B116" s="5">
-        <v>0</v>
+        <v>0.63639999999999997</v>
       </c>
       <c r="C116">
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="B117" s="5">
         <v>0</v>
       </c>
       <c r="C117">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B118" s="5">
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="B118" s="5">
-        <v>0</v>
-      </c>
-      <c r="C118">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="B119" s="5">
         <v>0</v>
@@ -8603,20 +8715,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B120" s="5">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="B120" s="5">
-        <v>0</v>
-      </c>
-      <c r="C120">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="B121" s="5">
         <v>0</v>
@@ -8625,9 +8737,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B122" s="5">
         <v>0</v>
@@ -8636,9 +8748,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B123" s="5">
         <v>0</v>
@@ -8647,7 +8759,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>32</v>
       </c>
@@ -8658,7 +8770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>58</v>
       </c>
@@ -8669,7 +8781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>89</v>
       </c>
@@ -8680,7 +8792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>164</v>
       </c>
@@ -8691,7 +8803,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>22</v>
       </c>
@@ -8702,7 +8814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>43</v>
       </c>
@@ -8713,7 +8825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>90</v>
       </c>
@@ -8724,7 +8836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>91</v>
       </c>
@@ -8735,7 +8847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>124</v>
       </c>
@@ -8746,7 +8858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>65</v>
       </c>
@@ -8757,7 +8869,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>73</v>
       </c>
@@ -8768,7 +8880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>85</v>
       </c>
@@ -8779,7 +8891,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>86</v>
       </c>
@@ -8790,7 +8902,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>109</v>
       </c>
@@ -8801,7 +8913,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>114</v>
       </c>
@@ -8812,7 +8924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>144</v>
       </c>
@@ -8823,7 +8935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>145</v>
       </c>
@@ -8834,7 +8946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>147</v>
       </c>
@@ -8845,7 +8957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>50</v>
       </c>
@@ -8856,7 +8968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>110</v>
       </c>
@@ -8867,7 +8979,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>150</v>
       </c>
@@ -8878,7 +8990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>84</v>
       </c>
@@ -8889,7 +9001,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>113</v>
       </c>
@@ -8900,7 +9012,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>126</v>
       </c>
@@ -8911,7 +9023,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>31</v>
       </c>
@@ -8922,7 +9034,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>117</v>
       </c>
@@ -8933,7 +9045,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>121</v>
       </c>
@@ -8944,7 +9056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>142</v>
       </c>
@@ -8955,7 +9067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>171</v>
       </c>
@@ -8966,7 +9078,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>68</v>
       </c>
@@ -8977,7 +9089,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>101</v>
       </c>
@@ -8988,7 +9100,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>76</v>
       </c>
@@ -8999,7 +9111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>111</v>
       </c>
@@ -9010,7 +9122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>105</v>
       </c>
@@ -9021,7 +9133,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>146</v>
       </c>
@@ -9032,7 +9144,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>72</v>
       </c>
@@ -9043,7 +9155,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>103</v>
       </c>
@@ -9054,7 +9166,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>69</v>
       </c>
@@ -9065,12 +9177,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" s="5"/>
-    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C161">
-    <sortCondition ref="C110:C161"/>
+    <sortCondition ref="C2:C161"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Started adding more descriptions to registration modules
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Java Projects\MIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E522C5-7FA5-42A5-9BEC-F0439CD20D7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAF36BE-2FF6-4983-B380-27275F5AB102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="480" yWindow="-108" windowWidth="22668" windowHeight="13176" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -683,10 +683,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$38</c:f>
+              <c:f>Sheet1!$B$2:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -797,16 +797,19 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$38</c:f>
+              <c:f>Sheet1!$N$2:$N$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -917,6 +920,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>77.108433734939766</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>76.92307692307692</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -956,10 +962,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$38</c:f>
+              <c:f>Sheet1!$B$2:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1070,16 +1076,19 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$38</c:f>
+              <c:f>Sheet1!$O$2:$O$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -1190,6 +1199,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>65.903141361256544</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>65.579014715291109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1229,10 +1241,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$38</c:f>
+              <c:f>Sheet1!$B$2:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1343,16 +1355,19 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$38</c:f>
+              <c:f>Sheet1!$P$2:$P$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -1463,6 +1478,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>65.662650602409641</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>64.49704142011835</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1502,10 +1520,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$38</c:f>
+              <c:f>Sheet1!$B$2:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1616,16 +1634,19 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$38</c:f>
+              <c:f>Sheet1!$Q$2:$Q$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1736,6 +1757,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>53.846153846153847</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1775,10 +1799,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$38</c:f>
+              <c:f>Sheet1!$B$2:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1889,16 +1913,19 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$38</c:f>
+              <c:f>Sheet1!$R$2:$R$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -2008,6 +2035,9 @@
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>40.375586854460096</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
@@ -2263,10 +2293,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$38</c:f>
+              <c:f>Sheet1!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2377,16 +2407,19 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>44132</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$38</c:f>
+              <c:f>Sheet1!$N$2:$N$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -2497,6 +2530,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>77.108433734939766</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>76.92307692307692</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2525,10 +2561,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$38</c:f>
+              <c:f>Sheet1!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2639,16 +2675,19 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>44132</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$38</c:f>
+              <c:f>Sheet1!$O$2:$O$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -2759,6 +2798,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>65.903141361256544</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>65.579014715291109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2787,10 +2829,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$38</c:f>
+              <c:f>Sheet1!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2901,16 +2943,19 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>44132</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$38</c:f>
+              <c:f>Sheet1!$P$2:$P$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -3021,6 +3066,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>65.662650602409641</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>64.49704142011835</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3049,10 +3097,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$38</c:f>
+              <c:f>Sheet1!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3163,16 +3211,19 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>44132</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$38</c:f>
+              <c:f>Sheet1!$Q$2:$Q$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -3283,6 +3334,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>53.846153846153847</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3311,10 +3365,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$38</c:f>
+              <c:f>Sheet1!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3425,16 +3479,19 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>44132</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$38</c:f>
+              <c:f>Sheet1!$R$2:$R$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -3544,6 +3601,9 @@
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>40.375586854460096</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
@@ -5264,31 +5324,31 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5335,7 +5395,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44054</v>
       </c>
@@ -5391,7 +5451,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44055</v>
       </c>
@@ -5447,7 +5507,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44056</v>
       </c>
@@ -5503,7 +5563,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44057</v>
       </c>
@@ -5558,7 +5618,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44058</v>
       </c>
@@ -5613,7 +5673,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>44064</v>
       </c>
@@ -5668,7 +5728,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>44069</v>
       </c>
@@ -5723,7 +5783,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>44070</v>
       </c>
@@ -5778,7 +5838,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44081</v>
       </c>
@@ -5833,7 +5893,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44082</v>
       </c>
@@ -5888,7 +5948,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44083</v>
       </c>
@@ -5943,7 +6003,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44084</v>
       </c>
@@ -5998,7 +6058,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44085</v>
       </c>
@@ -6053,7 +6113,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44089</v>
       </c>
@@ -6108,7 +6168,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>44090</v>
       </c>
@@ -6163,7 +6223,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44091</v>
       </c>
@@ -6218,7 +6278,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>44097</v>
       </c>
@@ -6273,7 +6333,7 @@
         <v>38.967136150234744</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>44098</v>
       </c>
@@ -6328,7 +6388,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>44099</v>
       </c>
@@ -6383,7 +6443,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>44102</v>
       </c>
@@ -6438,7 +6498,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>44103</v>
       </c>
@@ -6493,7 +6553,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>44104</v>
       </c>
@@ -6548,7 +6608,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>44110</v>
       </c>
@@ -6603,7 +6663,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>44113</v>
       </c>
@@ -6658,7 +6718,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>44116</v>
       </c>
@@ -6713,7 +6773,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>44117</v>
       </c>
@@ -6768,7 +6828,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>44118</v>
       </c>
@@ -6823,7 +6883,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>44119</v>
       </c>
@@ -6878,7 +6938,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>44120</v>
       </c>
@@ -6933,7 +6993,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>44123</v>
       </c>
@@ -6988,7 +7048,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>44124</v>
       </c>
@@ -7043,7 +7103,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>44125</v>
       </c>
@@ -7098,7 +7158,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>44126</v>
       </c>
@@ -7153,7 +7213,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>44127</v>
       </c>
@@ -7208,7 +7268,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>44130</v>
       </c>
@@ -7263,7 +7323,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>44131</v>
       </c>
@@ -7318,7 +7378,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>44132</v>
       </c>
@@ -7373,14 +7433,65 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="4"/>
-      <c r="P39" s="3"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>44134</v>
+      </c>
+      <c r="B39" s="4">
+        <v>38</v>
+      </c>
+      <c r="D39">
+        <v>169</v>
+      </c>
+      <c r="E39">
+        <v>130</v>
+      </c>
+      <c r="F39">
+        <v>1563</v>
+      </c>
+      <c r="G39">
+        <v>1025</v>
+      </c>
+      <c r="H39">
+        <v>109</v>
+      </c>
+      <c r="I39">
+        <v>26</v>
+      </c>
+      <c r="J39">
+        <v>14</v>
+      </c>
+      <c r="K39">
+        <v>213</v>
+      </c>
+      <c r="L39">
+        <v>86</v>
+      </c>
+      <c r="N39" s="3">
+        <f t="shared" ref="N39" si="159">100*E39/D39</f>
+        <v>76.92307692307692</v>
+      </c>
+      <c r="O39" s="3">
+        <f t="shared" ref="O39" si="160">100*G39/F39</f>
+        <v>65.579014715291109</v>
+      </c>
+      <c r="P39" s="3">
+        <f t="shared" ref="P39" si="161">100*H39/D39</f>
+        <v>64.49704142011835</v>
+      </c>
+      <c r="Q39" s="3">
+        <f t="shared" ref="Q39" si="162">100*J39/I39</f>
+        <v>53.846153846153847</v>
+      </c>
+      <c r="R39" s="3">
+        <f t="shared" ref="R39" si="163">100*L39/K39</f>
+        <v>40.375586854460096</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B41" s="4"/>
     </row>
   </sheetData>
@@ -7399,14 +7510,14 @@
       <selection activeCell="A109" sqref="A109:XFD109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
@@ -7417,7 +7528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -7428,7 +7539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -7439,7 +7550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -7450,7 +7561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -7461,7 +7572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -7472,7 +7583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
@@ -7483,7 +7594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
@@ -7494,7 +7605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
@@ -7505,7 +7616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
@@ -7516,7 +7627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -7527,7 +7638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -7538,7 +7649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
@@ -7549,7 +7660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
@@ -7560,7 +7671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>34</v>
       </c>
@@ -7571,7 +7682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
@@ -7582,7 +7693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
@@ -7593,7 +7704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
@@ -7604,7 +7715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>40</v>
       </c>
@@ -7615,7 +7726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>41</v>
       </c>
@@ -7626,7 +7737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>44</v>
       </c>
@@ -7637,7 +7748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>45</v>
       </c>
@@ -7648,7 +7759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>46</v>
       </c>
@@ -7659,7 +7770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>47</v>
       </c>
@@ -7670,7 +7781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>48</v>
       </c>
@@ -7681,7 +7792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>49</v>
       </c>
@@ -7692,7 +7803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>52</v>
       </c>
@@ -7703,7 +7814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>53</v>
       </c>
@@ -7714,7 +7825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>54</v>
       </c>
@@ -7725,7 +7836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>55</v>
       </c>
@@ -7736,7 +7847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>56</v>
       </c>
@@ -7747,7 +7858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>57</v>
       </c>
@@ -7758,7 +7869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>59</v>
       </c>
@@ -7769,7 +7880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>60</v>
       </c>
@@ -7780,7 +7891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>61</v>
       </c>
@@ -7791,7 +7902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>62</v>
       </c>
@@ -7802,7 +7913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>63</v>
       </c>
@@ -7813,7 +7924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>64</v>
       </c>
@@ -7824,7 +7935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>66</v>
       </c>
@@ -7835,7 +7946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>67</v>
       </c>
@@ -7846,7 +7957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>70</v>
       </c>
@@ -7857,7 +7968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>71</v>
       </c>
@@ -7868,7 +7979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>74</v>
       </c>
@@ -7879,7 +7990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>75</v>
       </c>
@@ -7890,7 +8001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>77</v>
       </c>
@@ -7901,7 +8012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>78</v>
       </c>
@@ -7912,7 +8023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>79</v>
       </c>
@@ -7923,7 +8034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>80</v>
       </c>
@@ -7934,7 +8045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>81</v>
       </c>
@@ -7945,7 +8056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>82</v>
       </c>
@@ -7956,7 +8067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>87</v>
       </c>
@@ -7967,7 +8078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>92</v>
       </c>
@@ -7978,7 +8089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>93</v>
       </c>
@@ -7989,7 +8100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>94</v>
       </c>
@@ -8000,7 +8111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>95</v>
       </c>
@@ -8011,7 +8122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>96</v>
       </c>
@@ -8022,7 +8133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>97</v>
       </c>
@@ -8033,7 +8144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>98</v>
       </c>
@@ -8044,7 +8155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>99</v>
       </c>
@@ -8055,7 +8166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>100</v>
       </c>
@@ -8066,7 +8177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>102</v>
       </c>
@@ -8077,7 +8188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>104</v>
       </c>
@@ -8088,7 +8199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>106</v>
       </c>
@@ -8099,7 +8210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>112</v>
       </c>
@@ -8110,7 +8221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>116</v>
       </c>
@@ -8121,7 +8232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>118</v>
       </c>
@@ -8132,7 +8243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>119</v>
       </c>
@@ -8143,7 +8254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>120</v>
       </c>
@@ -8154,7 +8265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>122</v>
       </c>
@@ -8165,7 +8276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>172</v>
       </c>
@@ -8176,7 +8287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>123</v>
       </c>
@@ -8187,7 +8298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>125</v>
       </c>
@@ -8198,7 +8309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>127</v>
       </c>
@@ -8209,7 +8320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>175</v>
       </c>
@@ -8220,7 +8331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>128</v>
       </c>
@@ -8231,7 +8342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>129</v>
       </c>
@@ -8242,7 +8353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>130</v>
       </c>
@@ -8253,7 +8364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>131</v>
       </c>
@@ -8264,7 +8375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>132</v>
       </c>
@@ -8275,7 +8386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>133</v>
       </c>
@@ -8286,7 +8397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>134</v>
       </c>
@@ -8297,7 +8408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>135</v>
       </c>
@@ -8308,7 +8419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>136</v>
       </c>
@@ -8319,7 +8430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>137</v>
       </c>
@@ -8330,7 +8441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>138</v>
       </c>
@@ -8341,7 +8452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>140</v>
       </c>
@@ -8352,7 +8463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>141</v>
       </c>
@@ -8363,7 +8474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>143</v>
       </c>
@@ -8374,7 +8485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>151</v>
       </c>
@@ -8385,7 +8496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>152</v>
       </c>
@@ -8396,7 +8507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>153</v>
       </c>
@@ -8407,7 +8518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>154</v>
       </c>
@@ -8418,7 +8529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>155</v>
       </c>
@@ -8429,7 +8540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>156</v>
       </c>
@@ -8440,7 +8551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>157</v>
       </c>
@@ -8451,7 +8562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>158</v>
       </c>
@@ -8462,7 +8573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>159</v>
       </c>
@@ -8473,7 +8584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>160</v>
       </c>
@@ -8484,7 +8595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>161</v>
       </c>
@@ -8495,7 +8606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>162</v>
       </c>
@@ -8506,7 +8617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>163</v>
       </c>
@@ -8517,7 +8628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>165</v>
       </c>
@@ -8528,7 +8639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>166</v>
       </c>
@@ -8539,7 +8650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>167</v>
       </c>
@@ -8550,7 +8661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>168</v>
       </c>
@@ -8561,7 +8672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>169</v>
       </c>
@@ -8572,7 +8683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>170</v>
       </c>
@@ -8583,7 +8694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>173</v>
       </c>
@@ -8594,7 +8705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>174</v>
       </c>
@@ -8605,7 +8716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>39</v>
       </c>
@@ -8616,7 +8727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>42</v>
       </c>
@@ -8627,7 +8738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>83</v>
       </c>
@@ -8638,7 +8749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>107</v>
       </c>
@@ -8649,7 +8760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>27</v>
       </c>
@@ -8660,7 +8771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>30</v>
       </c>
@@ -8671,7 +8782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>38</v>
       </c>
@@ -8682,7 +8793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>139</v>
       </c>
@@ -8693,7 +8804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>149</v>
       </c>
@@ -8704,7 +8815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>88</v>
       </c>
@@ -8715,7 +8826,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>148</v>
       </c>
@@ -8726,7 +8837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>51</v>
       </c>
@@ -8737,7 +8848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>108</v>
       </c>
@@ -8748,7 +8859,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>115</v>
       </c>
@@ -8759,7 +8870,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>32</v>
       </c>
@@ -8770,7 +8881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>58</v>
       </c>
@@ -8781,7 +8892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>89</v>
       </c>
@@ -8792,7 +8903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>164</v>
       </c>
@@ -8803,7 +8914,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>22</v>
       </c>
@@ -8814,7 +8925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>43</v>
       </c>
@@ -8825,7 +8936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>90</v>
       </c>
@@ -8836,7 +8947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>91</v>
       </c>
@@ -8847,7 +8958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>124</v>
       </c>
@@ -8858,7 +8969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>65</v>
       </c>
@@ -8869,7 +8980,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>73</v>
       </c>
@@ -8880,7 +8991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>85</v>
       </c>
@@ -8891,7 +9002,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>86</v>
       </c>
@@ -8902,7 +9013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>109</v>
       </c>
@@ -8913,7 +9024,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>114</v>
       </c>
@@ -8924,7 +9035,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>144</v>
       </c>
@@ -8935,7 +9046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>145</v>
       </c>
@@ -8946,7 +9057,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>147</v>
       </c>
@@ -8957,7 +9068,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>50</v>
       </c>
@@ -8968,7 +9079,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>110</v>
       </c>
@@ -8979,7 +9090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>150</v>
       </c>
@@ -8990,7 +9101,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>84</v>
       </c>
@@ -9001,7 +9112,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>113</v>
       </c>
@@ -9012,7 +9123,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>126</v>
       </c>
@@ -9023,7 +9134,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>31</v>
       </c>
@@ -9034,7 +9145,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>117</v>
       </c>
@@ -9045,7 +9156,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>121</v>
       </c>
@@ -9056,7 +9167,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>142</v>
       </c>
@@ -9067,7 +9178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>171</v>
       </c>
@@ -9078,7 +9189,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>68</v>
       </c>
@@ -9089,7 +9200,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>101</v>
       </c>
@@ -9100,7 +9211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>76</v>
       </c>
@@ -9111,7 +9222,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>111</v>
       </c>
@@ -9122,7 +9233,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>105</v>
       </c>
@@ -9133,7 +9244,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>146</v>
       </c>
@@ -9144,7 +9255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>72</v>
       </c>
@@ -9155,7 +9266,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>103</v>
       </c>
@@ -9166,7 +9277,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
Split automatic registration module and added block matching
Block matching uses another MPICBG feature extractor
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29054BB5-F118-459D-AF87-9092FD40CE88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BDF255-038C-4C92-84B8-668E27238EA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -689,10 +689,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$41</c:f>
+              <c:f>Sheet1!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -812,16 +812,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$41</c:f>
+              <c:f>Sheet1!$N$2:$N$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -941,6 +944,9 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>76.92307692307692</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>78.10650887573965</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -980,10 +986,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$41</c:f>
+              <c:f>Sheet1!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1103,16 +1109,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$41</c:f>
+              <c:f>Sheet1!$O$2:$O$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -1232,6 +1241,9 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>67.560664112388253</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>69.284802043422729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1271,10 +1283,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$41</c:f>
+              <c:f>Sheet1!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1394,16 +1406,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$41</c:f>
+              <c:f>Sheet1!$P$2:$P$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -1523,6 +1538,9 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>64.49704142011835</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>66.863905325443781</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1562,10 +1580,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$41</c:f>
+              <c:f>Sheet1!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1685,16 +1703,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$41</c:f>
+              <c:f>Sheet1!$Q$2:$Q$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1813,6 +1834,9 @@
                   <c:v>53.846153846153847</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>53.846153846153847</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>53.846153846153847</c:v>
                 </c:pt>
               </c:numCache>
@@ -1853,10 +1877,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$41</c:f>
+              <c:f>Sheet1!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1976,16 +2000,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$41</c:f>
+              <c:f>Sheet1!$R$2:$R$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -2104,6 +2131,9 @@
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>40.375586854460096</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
@@ -2359,10 +2389,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$41</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2482,16 +2512,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44138</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$41</c:f>
+              <c:f>Sheet1!$N$2:$N$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -2611,6 +2644,9 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>76.92307692307692</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>78.10650887573965</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2639,10 +2675,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$41</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2762,16 +2798,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44138</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$41</c:f>
+              <c:f>Sheet1!$O$2:$O$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -2891,6 +2930,9 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>67.560664112388253</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>69.284802043422729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2919,10 +2961,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$41</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3042,16 +3084,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44138</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$41</c:f>
+              <c:f>Sheet1!$P$2:$P$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -3171,6 +3216,9 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>64.49704142011835</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>66.863905325443781</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3199,10 +3247,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$41</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3322,16 +3370,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44138</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$41</c:f>
+              <c:f>Sheet1!$Q$2:$Q$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -3450,6 +3501,9 @@
                   <c:v>53.846153846153847</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>53.846153846153847</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>53.846153846153847</c:v>
                 </c:pt>
               </c:numCache>
@@ -3479,10 +3533,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$41</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3602,16 +3656,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44138</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$41</c:f>
+              <c:f>Sheet1!$R$2:$R$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -3730,6 +3787,9 @@
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>40.375586854460096</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
@@ -5447,10 +5507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7724,6 +7784,61 @@
         <v>40.375586854460096</v>
       </c>
     </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>44139</v>
+      </c>
+      <c r="B42" s="4">
+        <v>41</v>
+      </c>
+      <c r="D42">
+        <v>169</v>
+      </c>
+      <c r="E42">
+        <v>132</v>
+      </c>
+      <c r="F42">
+        <v>1566</v>
+      </c>
+      <c r="G42">
+        <v>1085</v>
+      </c>
+      <c r="H42">
+        <v>113</v>
+      </c>
+      <c r="I42">
+        <v>26</v>
+      </c>
+      <c r="J42">
+        <v>14</v>
+      </c>
+      <c r="K42">
+        <v>213</v>
+      </c>
+      <c r="L42">
+        <v>86</v>
+      </c>
+      <c r="N42" s="3">
+        <f t="shared" ref="N42" si="174">100*E42/D42</f>
+        <v>78.10650887573965</v>
+      </c>
+      <c r="O42" s="3">
+        <f t="shared" ref="O42" si="175">100*G42/F42</f>
+        <v>69.284802043422729</v>
+      </c>
+      <c r="P42" s="3">
+        <f t="shared" ref="P42" si="176">100*H42/D42</f>
+        <v>66.863905325443781</v>
+      </c>
+      <c r="Q42" s="3">
+        <f t="shared" ref="Q42" si="177">100*J42/I42</f>
+        <v>53.846153846153847</v>
+      </c>
+      <c r="R42" s="3">
+        <f t="shared" ref="R42" si="178">100*L42/K42</f>
+        <v>40.375586854460096</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7736,18 +7851,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60F2A9E-CB35-4818-B2AA-21716033EEE9}">
   <dimension ref="A1:C163"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T102" sqref="T102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" customWidth="1"/>
-    <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="6" max="8" width="8" customWidth="1"/>
-    <col min="10" max="17" width="8" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7818,7 +7930,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
@@ -7829,7 +7941,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -7840,7 +7952,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
@@ -7851,7 +7963,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
@@ -7862,7 +7974,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
@@ -7873,7 +7985,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="5">
         <v>1</v>
@@ -7884,7 +7996,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -7895,7 +8007,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
@@ -7906,7 +8018,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
@@ -7917,7 +8029,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="5">
         <v>1</v>
@@ -7928,7 +8040,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="5">
         <v>1</v>
@@ -7939,7 +8051,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
@@ -7950,7 +8062,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B19" s="5">
         <v>1</v>
@@ -7961,7 +8073,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
@@ -7972,7 +8084,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B21" s="5">
         <v>1</v>
@@ -7983,7 +8095,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B22" s="5">
         <v>1</v>
@@ -7994,7 +8106,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" s="5">
         <v>1</v>
@@ -8005,7 +8117,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" s="5">
         <v>1</v>
@@ -8016,7 +8128,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="5">
         <v>1</v>
@@ -8027,7 +8139,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
@@ -8038,7 +8150,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B27" s="5">
         <v>1</v>
@@ -8049,7 +8161,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B28" s="5">
         <v>1</v>
@@ -8060,7 +8172,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B29" s="5">
         <v>1</v>
@@ -8071,7 +8183,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B30" s="5">
         <v>1</v>
@@ -8082,7 +8194,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B31" s="5">
         <v>1</v>
@@ -8093,7 +8205,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B32" s="5">
         <v>1</v>
@@ -8104,7 +8216,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B33" s="5">
         <v>1</v>
@@ -8115,7 +8227,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B34" s="5">
         <v>1</v>
@@ -8126,7 +8238,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B35" s="5">
         <v>1</v>
@@ -8137,7 +8249,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" s="5">
         <v>1</v>
@@ -8148,7 +8260,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" s="5">
         <v>1</v>
@@ -8159,7 +8271,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B38" s="5">
         <v>1</v>
@@ -8170,7 +8282,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B39" s="5">
         <v>1</v>
@@ -8181,7 +8293,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B40" s="5">
         <v>1</v>
@@ -8192,7 +8304,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B41" s="5">
         <v>1</v>
@@ -8203,7 +8315,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B42" s="5">
         <v>1</v>
@@ -8214,7 +8326,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B43" s="5">
         <v>1</v>
@@ -8225,7 +8337,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B44" s="5">
         <v>1</v>
@@ -8236,7 +8348,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B45" s="5">
         <v>1</v>
@@ -8247,7 +8359,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B46" s="5">
         <v>1</v>
@@ -8258,7 +8370,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B47" s="5">
         <v>1</v>
@@ -8269,7 +8381,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B48" s="5">
         <v>1</v>
@@ -8280,7 +8392,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B49" s="5">
         <v>1</v>
@@ -8291,7 +8403,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B50" s="5">
         <v>1</v>
@@ -8302,7 +8414,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B51" s="5">
         <v>1</v>
@@ -8313,7 +8425,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B52" s="5">
         <v>1</v>
@@ -8324,7 +8436,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B53" s="5">
         <v>1</v>
@@ -8335,7 +8447,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B54" s="5">
         <v>1</v>
@@ -8346,7 +8458,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B55" s="5">
         <v>1</v>
@@ -8357,7 +8469,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B56" s="5">
         <v>1</v>
@@ -8368,7 +8480,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B57" s="5">
         <v>1</v>
@@ -8379,7 +8491,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B58" s="5">
         <v>1</v>
@@ -8390,7 +8502,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B59" s="5">
         <v>1</v>
@@ -8401,7 +8513,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B60" s="5">
         <v>1</v>
@@ -8412,7 +8524,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B61" s="5">
         <v>1</v>
@@ -8423,7 +8535,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B62" s="5">
         <v>1</v>
@@ -8434,7 +8546,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B63" s="5">
         <v>1</v>
@@ -8445,7 +8557,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B64" s="5">
         <v>1</v>
@@ -8456,7 +8568,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B65" s="5">
         <v>1</v>
@@ -8467,7 +8579,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B66" s="5">
         <v>1</v>
@@ -8478,7 +8590,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B67" s="5">
         <v>1</v>
@@ -8489,7 +8601,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B68" s="5">
         <v>1</v>
@@ -8500,7 +8612,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B69" s="5">
         <v>1</v>
@@ -8511,7 +8623,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>172</v>
+        <v>118</v>
       </c>
       <c r="B70" s="5">
         <v>1</v>
@@ -8522,7 +8634,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B71" s="5">
         <v>1</v>
@@ -8533,7 +8645,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B72" s="5">
         <v>1</v>
@@ -8544,7 +8656,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B73" s="5">
         <v>1</v>
@@ -8555,7 +8667,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B74" s="5">
         <v>1</v>
@@ -8566,7 +8678,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B75" s="5">
         <v>1</v>
@@ -8577,7 +8689,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B76" s="5">
         <v>1</v>
@@ -8588,7 +8700,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B77" s="5">
         <v>1</v>
@@ -8599,7 +8711,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>131</v>
+        <v>175</v>
       </c>
       <c r="B78" s="5">
         <v>1</v>
@@ -8610,7 +8722,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B79" s="5">
         <v>1</v>
@@ -8621,7 +8733,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B80" s="5">
         <v>1</v>
@@ -8632,7 +8744,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B81" s="5">
         <v>1</v>
@@ -8643,7 +8755,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B82" s="5">
         <v>1</v>
@@ -8654,7 +8766,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B83" s="5">
         <v>1</v>
@@ -8665,7 +8777,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B84" s="5">
         <v>1</v>
@@ -8676,7 +8788,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B85" s="5">
         <v>1</v>
@@ -8687,7 +8799,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B86" s="5">
         <v>1</v>
@@ -8698,7 +8810,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B87" s="5">
         <v>1</v>
@@ -8709,7 +8821,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B88" s="5">
         <v>1</v>
@@ -8720,7 +8832,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B89" s="5">
         <v>1</v>
@@ -8731,7 +8843,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B90" s="5">
         <v>1</v>
@@ -8742,7 +8854,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B91" s="5">
         <v>1</v>
@@ -8753,7 +8865,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B92" s="5">
         <v>1</v>
@@ -8764,7 +8876,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B93" s="5">
         <v>1</v>
@@ -8775,7 +8887,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B94" s="5">
         <v>1</v>
@@ -8786,7 +8898,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B95" s="5">
         <v>1</v>
@@ -8797,7 +8909,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B96" s="5">
         <v>1</v>
@@ -8808,7 +8920,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B97" s="5">
         <v>1</v>
@@ -8819,7 +8931,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B98" s="5">
         <v>1</v>
@@ -8830,7 +8942,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B99" s="5">
         <v>1</v>
@@ -8841,7 +8953,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B100" s="5">
         <v>1</v>
@@ -8852,7 +8964,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B101" s="5">
         <v>1</v>
@@ -8863,7 +8975,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B102" s="5">
         <v>1</v>
@@ -8874,7 +8986,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B103" s="5">
         <v>1</v>
@@ -8885,7 +8997,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B104" s="5">
         <v>1</v>
@@ -8896,7 +9008,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B105" s="5">
         <v>1</v>
@@ -8907,7 +9019,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B106" s="5">
         <v>1</v>
@@ -8918,7 +9030,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B107" s="5">
         <v>1</v>
@@ -8929,7 +9041,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B108" s="5">
         <v>1</v>
@@ -8939,8 +9051,8 @@
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>174</v>
+      <c r="A109" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="B109" s="5">
         <v>1</v>
@@ -8951,106 +9063,106 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B110" s="5">
-        <v>0.88890000000000002</v>
+        <v>1</v>
       </c>
       <c r="C110">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>42</v>
+        <v>170</v>
       </c>
       <c r="B111" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C111">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>83</v>
+        <v>173</v>
       </c>
       <c r="B112" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C112">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>107</v>
+        <v>174</v>
       </c>
       <c r="B113" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C113">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="B114" s="5">
-        <v>0.72729999999999995</v>
+        <v>0.96550000000000002</v>
       </c>
       <c r="C114">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
       <c r="B115" s="5">
-        <v>0.86960000000000004</v>
+        <v>0.88890000000000002</v>
       </c>
       <c r="C115">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B116" s="5">
-        <v>0</v>
+        <v>0.72729999999999995</v>
       </c>
       <c r="C116">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="B117" s="5">
         <v>0</v>
       </c>
       <c r="C117">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="B118" s="5">
         <v>0</v>
       </c>
       <c r="C118">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>149</v>
+        <v>27</v>
       </c>
       <c r="B119" s="5">
         <v>0</v>
@@ -9061,10 +9173,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B120" s="5">
-        <v>0.63639999999999997</v>
+        <v>0</v>
       </c>
       <c r="C120">
         <v>4</v>
@@ -9072,65 +9184,65 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="B121" s="5">
-        <v>0</v>
+        <v>0.63639999999999997</v>
       </c>
       <c r="C121">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B122" s="5">
         <v>0</v>
       </c>
       <c r="C122">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>51</v>
+        <v>149</v>
       </c>
       <c r="B123" s="5">
         <v>0</v>
       </c>
       <c r="C123">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="B124" s="5">
         <v>0</v>
       </c>
       <c r="C124">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="B125" s="5">
         <v>0</v>
       </c>
       <c r="C125">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>176</v>
+        <v>51</v>
       </c>
       <c r="B126" s="5">
-        <v>0.79310000000000003</v>
+        <v>0</v>
       </c>
       <c r="C126">
         <v>6</v>
@@ -9138,32 +9250,32 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="B127" s="5">
         <v>0</v>
       </c>
       <c r="C127">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="B128" s="5">
         <v>0</v>
       </c>
       <c r="C128">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>164</v>
+        <v>32</v>
       </c>
       <c r="B129" s="5">
-        <v>0</v>
+        <v>0.36359999999999998</v>
       </c>
       <c r="C129">
         <v>7</v>
@@ -9171,10 +9283,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B130" s="5">
-        <v>0.36359999999999998</v>
+        <v>0</v>
       </c>
       <c r="C130">
         <v>7</v>
@@ -9182,29 +9294,29 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="B131" s="5">
         <v>0</v>
       </c>
       <c r="C131">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>43</v>
+        <v>164</v>
       </c>
       <c r="B132" s="5">
         <v>0</v>
       </c>
       <c r="C132">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="B133" s="5">
         <v>0</v>
@@ -9215,7 +9327,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="B134" s="5">
         <v>0</v>
@@ -9445,7 +9557,7 @@
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+      <c r="A155" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B155" s="5">
@@ -9545,7 +9657,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C163">
-    <sortCondition ref="C2:C163"/>
+    <sortCondition ref="C1:C163"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added resolution as a parameter to block matching registration
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Java Projects\MIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C4C868-602D-4304-A937-0ADE642420B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EB38CC-CFF8-4601-91E9-AFF2709C0E7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="-108" windowWidth="22668" windowHeight="13176" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -695,10 +695,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$43</c:f>
+              <c:f>Sheet1!$B$2:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -824,16 +824,19 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$43</c:f>
+              <c:f>Sheet1!$N$2:$N$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -959,6 +962,9 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>78.488372093023258</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>79.069767441860463</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -998,10 +1004,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$43</c:f>
+              <c:f>Sheet1!$B$2:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1127,16 +1133,19 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$43</c:f>
+              <c:f>Sheet1!$O$2:$O$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -1262,6 +1271,9 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>70.243293824079856</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>70.6575682382134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1301,10 +1313,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$43</c:f>
+              <c:f>Sheet1!$B$2:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1430,16 +1442,19 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$43</c:f>
+              <c:f>Sheet1!$P$2:$P$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -1565,6 +1580,9 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>67.441860465116278</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>68.023255813953483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1604,10 +1622,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$43</c:f>
+              <c:f>Sheet1!$B$2:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1733,16 +1751,19 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$43</c:f>
+              <c:f>Sheet1!$Q$2:$Q$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1867,6 +1888,9 @@
                   <c:v>53.846153846153847</c:v>
                 </c:pt>
                 <c:pt idx="41">
+                  <c:v>53.846153846153847</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>53.846153846153847</c:v>
                 </c:pt>
               </c:numCache>
@@ -1907,10 +1931,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$43</c:f>
+              <c:f>Sheet1!$B$2:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2036,16 +2060,19 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$43</c:f>
+              <c:f>Sheet1!$R$2:$R$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -2170,6 +2197,9 @@
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
                 <c:pt idx="41">
+                  <c:v>40.375586854460096</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
@@ -2425,10 +2455,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$43</c:f>
+              <c:f>Sheet1!$A$2:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2554,16 +2584,19 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>44140</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44141</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$43</c:f>
+              <c:f>Sheet1!$N$2:$N$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -2689,6 +2722,9 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>78.488372093023258</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>79.069767441860463</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2717,10 +2753,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$43</c:f>
+              <c:f>Sheet1!$A$2:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2846,16 +2882,19 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>44140</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44141</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$43</c:f>
+              <c:f>Sheet1!$O$2:$O$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -2981,6 +3020,9 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>70.243293824079856</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>70.6575682382134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3009,10 +3051,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$43</c:f>
+              <c:f>Sheet1!$A$2:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3138,16 +3180,19 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>44140</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44141</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$43</c:f>
+              <c:f>Sheet1!$P$2:$P$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -3273,6 +3318,9 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>67.441860465116278</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>68.023255813953483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3301,10 +3349,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$43</c:f>
+              <c:f>Sheet1!$A$2:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3430,16 +3478,19 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>44140</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44141</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$43</c:f>
+              <c:f>Sheet1!$Q$2:$Q$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -3564,6 +3615,9 @@
                   <c:v>53.846153846153847</c:v>
                 </c:pt>
                 <c:pt idx="41">
+                  <c:v>53.846153846153847</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>53.846153846153847</c:v>
                 </c:pt>
               </c:numCache>
@@ -3593,10 +3647,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$43</c:f>
+              <c:f>Sheet1!$A$2:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3722,16 +3776,19 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>44140</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44141</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$43</c:f>
+              <c:f>Sheet1!$R$2:$R$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -3856,6 +3913,9 @@
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
                 <c:pt idx="41">
+                  <c:v>40.375586854460096</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>40.375586854460096</c:v>
                 </c:pt>
               </c:numCache>
@@ -5573,34 +5633,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:R43"/>
+  <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5647,7 +5707,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44054</v>
       </c>
@@ -5703,7 +5763,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44055</v>
       </c>
@@ -5759,7 +5819,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44056</v>
       </c>
@@ -5815,7 +5875,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44057</v>
       </c>
@@ -5870,7 +5930,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44058</v>
       </c>
@@ -5925,7 +5985,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44064</v>
       </c>
@@ -5980,7 +6040,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44069</v>
       </c>
@@ -6035,7 +6095,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44070</v>
       </c>
@@ -6090,7 +6150,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44081</v>
       </c>
@@ -6145,7 +6205,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44082</v>
       </c>
@@ -6200,7 +6260,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44083</v>
       </c>
@@ -6255,7 +6315,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44084</v>
       </c>
@@ -6310,7 +6370,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44085</v>
       </c>
@@ -6365,7 +6425,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44089</v>
       </c>
@@ -6420,7 +6480,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44090</v>
       </c>
@@ -6475,7 +6535,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44091</v>
       </c>
@@ -6530,7 +6590,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44097</v>
       </c>
@@ -6585,7 +6645,7 @@
         <v>38.967136150234744</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44098</v>
       </c>
@@ -6640,7 +6700,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44099</v>
       </c>
@@ -6695,7 +6755,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44102</v>
       </c>
@@ -6750,7 +6810,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44103</v>
       </c>
@@ -6805,7 +6865,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44104</v>
       </c>
@@ -6860,7 +6920,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44110</v>
       </c>
@@ -6915,7 +6975,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44113</v>
       </c>
@@ -6970,7 +7030,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44116</v>
       </c>
@@ -7025,7 +7085,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44117</v>
       </c>
@@ -7080,7 +7140,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44118</v>
       </c>
@@ -7135,7 +7195,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44119</v>
       </c>
@@ -7190,7 +7250,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44120</v>
       </c>
@@ -7245,7 +7305,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44123</v>
       </c>
@@ -7300,7 +7360,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44124</v>
       </c>
@@ -7355,7 +7415,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44125</v>
       </c>
@@ -7410,7 +7470,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44126</v>
       </c>
@@ -7465,7 +7525,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44127</v>
       </c>
@@ -7520,7 +7580,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44130</v>
       </c>
@@ -7575,7 +7635,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44131</v>
       </c>
@@ -7630,7 +7690,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44132</v>
       </c>
@@ -7685,7 +7745,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44134</v>
       </c>
@@ -7740,7 +7800,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44137</v>
       </c>
@@ -7795,7 +7855,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44138</v>
       </c>
@@ -7850,7 +7910,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44139</v>
       </c>
@@ -7905,7 +7965,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44140</v>
       </c>
@@ -7957,6 +8017,61 @@
       </c>
       <c r="R43" s="3">
         <f t="shared" ref="R43" si="183">100*L43/K43</f>
+        <v>40.375586854460096</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>44141</v>
+      </c>
+      <c r="B44" s="4">
+        <v>43</v>
+      </c>
+      <c r="D44">
+        <v>172</v>
+      </c>
+      <c r="E44">
+        <v>136</v>
+      </c>
+      <c r="F44">
+        <v>1612</v>
+      </c>
+      <c r="G44">
+        <v>1139</v>
+      </c>
+      <c r="H44">
+        <v>117</v>
+      </c>
+      <c r="I44">
+        <v>26</v>
+      </c>
+      <c r="J44">
+        <v>14</v>
+      </c>
+      <c r="K44">
+        <v>213</v>
+      </c>
+      <c r="L44">
+        <v>86</v>
+      </c>
+      <c r="N44" s="3">
+        <f t="shared" ref="N44" si="184">100*E44/D44</f>
+        <v>79.069767441860463</v>
+      </c>
+      <c r="O44" s="3">
+        <f t="shared" ref="O44" si="185">100*G44/F44</f>
+        <v>70.6575682382134</v>
+      </c>
+      <c r="P44" s="3">
+        <f t="shared" ref="P44" si="186">100*H44/D44</f>
+        <v>68.023255813953483</v>
+      </c>
+      <c r="Q44" s="3">
+        <f t="shared" ref="Q44" si="187">100*J44/I44</f>
+        <v>53.846153846153847</v>
+      </c>
+      <c r="R44" s="3">
+        <f t="shared" ref="R44" si="188">100*L44/K44</f>
         <v>40.375586854460096</v>
       </c>
     </row>
@@ -7976,14 +8091,14 @@
       <selection activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
@@ -7994,7 +8109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -8005,7 +8120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -8016,7 +8131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -8027,7 +8142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -8038,7 +8153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -8049,7 +8164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>69</v>
       </c>
@@ -8060,7 +8175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -8071,7 +8186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -8082,7 +8197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -8093,7 +8208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -8104,7 +8219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>26</v>
       </c>
@@ -8115,7 +8230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
@@ -8126,7 +8241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
@@ -8137,7 +8252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
@@ -8148,7 +8263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>34</v>
       </c>
@@ -8159,7 +8274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>35</v>
       </c>
@@ -8170,7 +8285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
@@ -8181,7 +8296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
@@ -8192,7 +8307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
@@ -8203,7 +8318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>41</v>
       </c>
@@ -8214,7 +8329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>42</v>
       </c>
@@ -8225,7 +8340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>44</v>
       </c>
@@ -8236,7 +8351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>45</v>
       </c>
@@ -8247,7 +8362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>46</v>
       </c>
@@ -8258,7 +8373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>47</v>
       </c>
@@ -8269,7 +8384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>48</v>
       </c>
@@ -8280,7 +8395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>49</v>
       </c>
@@ -8291,7 +8406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>52</v>
       </c>
@@ -8302,7 +8417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>53</v>
       </c>
@@ -8313,7 +8428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>54</v>
       </c>
@@ -8324,7 +8439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>55</v>
       </c>
@@ -8335,7 +8450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>56</v>
       </c>
@@ -8346,7 +8461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>57</v>
       </c>
@@ -8357,7 +8472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>59</v>
       </c>
@@ -8368,7 +8483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>60</v>
       </c>
@@ -8379,7 +8494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>61</v>
       </c>
@@ -8390,7 +8505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>62</v>
       </c>
@@ -8401,7 +8516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>63</v>
       </c>
@@ -8412,7 +8527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>64</v>
       </c>
@@ -8423,7 +8538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>66</v>
       </c>
@@ -8434,7 +8549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>67</v>
       </c>
@@ -8445,7 +8560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>178</v>
       </c>
@@ -8456,7 +8571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>179</v>
       </c>
@@ -8467,7 +8582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>70</v>
       </c>
@@ -8478,7 +8593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>71</v>
       </c>
@@ -8489,7 +8604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>74</v>
       </c>
@@ -8500,7 +8615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>75</v>
       </c>
@@ -8511,7 +8626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>77</v>
       </c>
@@ -8522,7 +8637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>78</v>
       </c>
@@ -8533,7 +8648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>79</v>
       </c>
@@ -8544,7 +8659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>80</v>
       </c>
@@ -8555,7 +8670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>81</v>
       </c>
@@ -8566,7 +8681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>82</v>
       </c>
@@ -8577,7 +8692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>87</v>
       </c>
@@ -8588,7 +8703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>90</v>
       </c>
@@ -8599,7 +8714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>91</v>
       </c>
@@ -8610,7 +8725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>92</v>
       </c>
@@ -8621,7 +8736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>93</v>
       </c>
@@ -8632,7 +8747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>94</v>
       </c>
@@ -8643,7 +8758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>95</v>
       </c>
@@ -8654,7 +8769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>96</v>
       </c>
@@ -8665,7 +8780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>97</v>
       </c>
@@ -8676,7 +8791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>98</v>
       </c>
@@ -8687,7 +8802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>99</v>
       </c>
@@ -8698,7 +8813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>100</v>
       </c>
@@ -8709,7 +8824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>102</v>
       </c>
@@ -8720,7 +8835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>104</v>
       </c>
@@ -8731,7 +8846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>106</v>
       </c>
@@ -8742,7 +8857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>112</v>
       </c>
@@ -8753,7 +8868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>116</v>
       </c>
@@ -8764,7 +8879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>118</v>
       </c>
@@ -8775,7 +8890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>119</v>
       </c>
@@ -8786,7 +8901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>120</v>
       </c>
@@ -8797,7 +8912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>122</v>
       </c>
@@ -8808,7 +8923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>172</v>
       </c>
@@ -8819,7 +8934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>123</v>
       </c>
@@ -8830,7 +8945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>125</v>
       </c>
@@ -8841,7 +8956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>127</v>
       </c>
@@ -8852,7 +8967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>175</v>
       </c>
@@ -8863,7 +8978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>128</v>
       </c>
@@ -8874,7 +8989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>129</v>
       </c>
@@ -8885,7 +9000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>130</v>
       </c>
@@ -8896,7 +9011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>131</v>
       </c>
@@ -8907,7 +9022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>132</v>
       </c>
@@ -8918,7 +9033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>133</v>
       </c>
@@ -8929,7 +9044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>134</v>
       </c>
@@ -8940,7 +9055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>135</v>
       </c>
@@ -8951,7 +9066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>136</v>
       </c>
@@ -8962,7 +9077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>137</v>
       </c>
@@ -8973,7 +9088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>138</v>
       </c>
@@ -8984,7 +9099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>140</v>
       </c>
@@ -8995,7 +9110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>141</v>
       </c>
@@ -9006,7 +9121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>143</v>
       </c>
@@ -9017,7 +9132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>149</v>
       </c>
@@ -9028,7 +9143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>151</v>
       </c>
@@ -9039,7 +9154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>152</v>
       </c>
@@ -9050,7 +9165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>153</v>
       </c>
@@ -9061,7 +9176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>154</v>
       </c>
@@ -9072,7 +9187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>155</v>
       </c>
@@ -9083,7 +9198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>156</v>
       </c>
@@ -9094,7 +9209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>157</v>
       </c>
@@ -9105,7 +9220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>158</v>
       </c>
@@ -9116,7 +9231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>159</v>
       </c>
@@ -9127,7 +9242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>160</v>
       </c>
@@ -9138,7 +9253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>161</v>
       </c>
@@ -9149,7 +9264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>162</v>
       </c>
@@ -9160,7 +9275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>163</v>
       </c>
@@ -9171,7 +9286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>165</v>
       </c>
@@ -9182,7 +9297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>166</v>
       </c>
@@ -9193,7 +9308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>167</v>
       </c>
@@ -9204,7 +9319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>168</v>
       </c>
@@ -9215,7 +9330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>169</v>
       </c>
@@ -9226,7 +9341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>170</v>
       </c>
@@ -9237,7 +9352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>173</v>
       </c>
@@ -9248,7 +9363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>174</v>
       </c>
@@ -9259,7 +9374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>176</v>
       </c>
@@ -9270,7 +9385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>39</v>
       </c>
@@ -9281,7 +9396,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>83</v>
       </c>
@@ -9292,7 +9407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>107</v>
       </c>
@@ -9303,7 +9418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>27</v>
       </c>
@@ -9314,7 +9429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>30</v>
       </c>
@@ -9325,7 +9440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>38</v>
       </c>
@@ -9336,7 +9451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>139</v>
       </c>
@@ -9347,7 +9462,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>88</v>
       </c>
@@ -9358,7 +9473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>148</v>
       </c>
@@ -9369,7 +9484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>51</v>
       </c>
@@ -9380,7 +9495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>108</v>
       </c>
@@ -9391,7 +9506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>115</v>
       </c>
@@ -9402,7 +9517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>32</v>
       </c>
@@ -9413,7 +9528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>58</v>
       </c>
@@ -9424,7 +9539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>89</v>
       </c>
@@ -9435,7 +9550,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>164</v>
       </c>
@@ -9446,7 +9561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>22</v>
       </c>
@@ -9457,7 +9572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>43</v>
       </c>
@@ -9468,7 +9583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>177</v>
       </c>
@@ -9479,7 +9594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>124</v>
       </c>
@@ -9490,7 +9605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>65</v>
       </c>
@@ -9501,7 +9616,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>73</v>
       </c>
@@ -9512,7 +9627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>85</v>
       </c>
@@ -9523,7 +9638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>86</v>
       </c>
@@ -9534,7 +9649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>109</v>
       </c>
@@ -9545,7 +9660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>114</v>
       </c>
@@ -9556,7 +9671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>144</v>
       </c>
@@ -9567,7 +9682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>145</v>
       </c>
@@ -9578,7 +9693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>147</v>
       </c>
@@ -9589,7 +9704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>50</v>
       </c>
@@ -9600,7 +9715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>110</v>
       </c>
@@ -9611,7 +9726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>150</v>
       </c>
@@ -9622,7 +9737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>84</v>
       </c>
@@ -9633,7 +9748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>113</v>
       </c>
@@ -9644,7 +9759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>126</v>
       </c>
@@ -9655,7 +9770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>31</v>
       </c>
@@ -9666,7 +9781,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>117</v>
       </c>
@@ -9677,7 +9792,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>121</v>
       </c>
@@ -9688,7 +9803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>142</v>
       </c>
@@ -9699,7 +9814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>171</v>
       </c>
@@ -9710,7 +9825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>68</v>
       </c>
@@ -9721,7 +9836,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>101</v>
       </c>
@@ -9732,7 +9847,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>76</v>
       </c>
@@ -9743,7 +9858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>111</v>
       </c>
@@ -9754,7 +9869,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>105</v>
       </c>
@@ -9765,7 +9880,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>146</v>
       </c>
@@ -9776,7 +9891,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>72</v>
       </c>
@@ -9787,7 +9902,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>103</v>
       </c>

</xml_diff>

<commit_message>
2D intensity histogram now outputs float
Also added more parameter descriptions.
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stephen\Programming\Java Projects\mia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C0DED8-EB0E-499C-A7E6-5104F29B856C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5C058E-6C30-49AA-A63F-A41A4F525471}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -207,10 +207,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$51</c:f>
+              <c:f>Sheet1!$B$2:$B$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -360,16 +360,19 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$51</c:f>
+              <c:f>Sheet1!$N$2:$N$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -519,6 +522,9 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>79.32960893854748</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>79.888268156424587</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -558,10 +564,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$51</c:f>
+              <c:f>Sheet1!$B$2:$B$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -711,16 +717,19 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$51</c:f>
+              <c:f>Sheet1!$O$2:$O$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -870,6 +879,9 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>71.66567871962063</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>72.274881516587683</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -909,10 +921,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$51</c:f>
+              <c:f>Sheet1!$B$2:$B$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1062,16 +1074,19 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$51</c:f>
+              <c:f>Sheet1!$P$2:$P$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -1221,6 +1236,9 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>64.245810055865917</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>64.80446927374301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1260,10 +1278,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$51</c:f>
+              <c:f>Sheet1!$B$2:$B$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1413,16 +1431,19 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$51</c:f>
+              <c:f>Sheet1!$Q$2:$Q$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1571,6 +1592,9 @@
                   <c:v>51.428571428571431</c:v>
                 </c:pt>
                 <c:pt idx="49">
+                  <c:v>51.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>51.428571428571431</c:v>
                 </c:pt>
               </c:numCache>
@@ -1611,10 +1635,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$51</c:f>
+              <c:f>Sheet1!$B$2:$B$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1764,16 +1788,19 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$51</c:f>
+              <c:f>Sheet1!$R$2:$R$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -1922,6 +1949,9 @@
                   <c:v>39.449541284403672</c:v>
                 </c:pt>
                 <c:pt idx="49">
+                  <c:v>39.449541284403672</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>39.449541284403672</c:v>
                 </c:pt>
               </c:numCache>
@@ -2177,10 +2207,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:f>Sheet1!$A$2:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2330,16 +2360,19 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>44302</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$51</c:f>
+              <c:f>Sheet1!$N$2:$N$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -2489,6 +2522,9 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>79.32960893854748</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>79.888268156424587</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2517,10 +2553,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:f>Sheet1!$A$2:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -2670,16 +2706,19 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>44302</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$51</c:f>
+              <c:f>Sheet1!$O$2:$O$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>15.016611295681063</c:v>
                 </c:pt>
@@ -2829,6 +2868,9 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>71.66567871962063</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>72.274881516587683</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2857,10 +2899,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:f>Sheet1!$A$2:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3010,16 +3052,19 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>44302</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$51</c:f>
+              <c:f>Sheet1!$P$2:$P$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -3169,6 +3214,9 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>64.245810055865917</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>64.80446927374301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3197,10 +3245,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:f>Sheet1!$A$2:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3350,16 +3398,19 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>44302</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$51</c:f>
+              <c:f>Sheet1!$Q$2:$Q$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -3508,6 +3559,9 @@
                   <c:v>51.428571428571431</c:v>
                 </c:pt>
                 <c:pt idx="49">
+                  <c:v>51.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>51.428571428571431</c:v>
                 </c:pt>
               </c:numCache>
@@ -3537,10 +3591,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:f>Sheet1!$A$2:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3690,16 +3744,19 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>44302</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$51</c:f>
+              <c:f>Sheet1!$R$2:$R$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -3848,6 +3905,9 @@
                   <c:v>39.449541284403672</c:v>
                 </c:pt>
                 <c:pt idx="49">
+                  <c:v>39.449541284403672</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>39.449541284403672</c:v>
                 </c:pt>
               </c:numCache>
@@ -5566,34 +5626,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:R51"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5640,7 +5700,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44054</v>
       </c>
@@ -5696,7 +5756,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44055</v>
       </c>
@@ -5752,7 +5812,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44056</v>
       </c>
@@ -5808,7 +5868,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44057</v>
       </c>
@@ -5863,7 +5923,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44058</v>
       </c>
@@ -5918,7 +5978,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>44064</v>
       </c>
@@ -5973,7 +6033,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>44069</v>
       </c>
@@ -6028,7 +6088,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>44070</v>
       </c>
@@ -6083,7 +6143,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44081</v>
       </c>
@@ -6138,7 +6198,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44082</v>
       </c>
@@ -6193,7 +6253,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44083</v>
       </c>
@@ -6248,7 +6308,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44084</v>
       </c>
@@ -6303,7 +6363,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44085</v>
       </c>
@@ -6358,7 +6418,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44089</v>
       </c>
@@ -6413,7 +6473,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>44090</v>
       </c>
@@ -6468,7 +6528,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44091</v>
       </c>
@@ -6523,7 +6583,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>44097</v>
       </c>
@@ -6578,7 +6638,7 @@
         <v>38.967136150234744</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>44098</v>
       </c>
@@ -6633,7 +6693,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>44099</v>
       </c>
@@ -6688,7 +6748,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>44102</v>
       </c>
@@ -6743,7 +6803,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>44103</v>
       </c>
@@ -6798,7 +6858,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>44104</v>
       </c>
@@ -6853,7 +6913,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>44110</v>
       </c>
@@ -6908,7 +6968,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>44113</v>
       </c>
@@ -6963,7 +7023,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>44116</v>
       </c>
@@ -7018,7 +7078,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>44117</v>
       </c>
@@ -7073,7 +7133,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>44118</v>
       </c>
@@ -7128,7 +7188,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>44119</v>
       </c>
@@ -7183,7 +7243,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>44120</v>
       </c>
@@ -7238,7 +7298,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>44123</v>
       </c>
@@ -7293,7 +7353,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>44124</v>
       </c>
@@ -7348,7 +7408,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>44125</v>
       </c>
@@ -7403,7 +7463,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>44126</v>
       </c>
@@ -7458,7 +7518,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>44127</v>
       </c>
@@ -7513,7 +7573,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>44130</v>
       </c>
@@ -7568,7 +7628,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>44131</v>
       </c>
@@ -7623,7 +7683,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>44132</v>
       </c>
@@ -7678,7 +7738,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>44134</v>
       </c>
@@ -7733,7 +7793,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>44137</v>
       </c>
@@ -7788,7 +7848,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>44138</v>
       </c>
@@ -7843,7 +7903,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>44139</v>
       </c>
@@ -7898,7 +7958,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>44140</v>
       </c>
@@ -7953,7 +8013,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>44141</v>
       </c>
@@ -8008,7 +8068,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44147</v>
       </c>
@@ -8063,7 +8123,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44148</v>
       </c>
@@ -8118,7 +8178,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>44151</v>
       </c>
@@ -8173,7 +8233,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>44152</v>
       </c>
@@ -8228,7 +8288,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>44300</v>
       </c>
@@ -8283,7 +8343,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>44301</v>
       </c>
@@ -8338,7 +8398,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>44302</v>
       </c>
@@ -8390,6 +8450,61 @@
       </c>
       <c r="R51" s="3">
         <f t="shared" ref="R51" si="223">100*L51/K51</f>
+        <v>39.449541284403672</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>44305</v>
+      </c>
+      <c r="B52" s="4">
+        <v>51</v>
+      </c>
+      <c r="D52">
+        <v>179</v>
+      </c>
+      <c r="E52">
+        <v>143</v>
+      </c>
+      <c r="F52">
+        <v>1688</v>
+      </c>
+      <c r="G52">
+        <v>1220</v>
+      </c>
+      <c r="H52">
+        <v>116</v>
+      </c>
+      <c r="I52">
+        <v>35</v>
+      </c>
+      <c r="J52">
+        <v>18</v>
+      </c>
+      <c r="K52">
+        <v>218</v>
+      </c>
+      <c r="L52">
+        <v>86</v>
+      </c>
+      <c r="N52" s="3">
+        <f t="shared" ref="N52" si="224">100*E52/D52</f>
+        <v>79.888268156424587</v>
+      </c>
+      <c r="O52" s="3">
+        <f t="shared" ref="O52" si="225">100*G52/F52</f>
+        <v>72.274881516587683</v>
+      </c>
+      <c r="P52" s="3">
+        <f t="shared" ref="P52" si="226">100*H52/D52</f>
+        <v>64.80446927374301</v>
+      </c>
+      <c r="Q52" s="3">
+        <f t="shared" ref="Q52" si="227">100*J52/I52</f>
+        <v>51.428571428571431</v>
+      </c>
+      <c r="R52" s="3">
+        <f t="shared" ref="R52" si="228">100*L52/K52</f>
         <v>39.449541284403672</v>
       </c>
     </row>
@@ -8409,1202 +8524,1202 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="6"/>
       <c r="C1" s="5"/>
       <c r="D1" s="6"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="6"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="6"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="6"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="6"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="6"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="6"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="6"/>
       <c r="C40" s="5"/>
       <c r="D40" s="6"/>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="6"/>
       <c r="C42" s="5"/>
       <c r="D42" s="6"/>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="6"/>
       <c r="C43" s="5"/>
       <c r="D43" s="6"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="6"/>
       <c r="C44" s="5"/>
       <c r="D44" s="6"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="6"/>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
       <c r="E45" s="5"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="6"/>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
       <c r="E46" s="5"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="6"/>
       <c r="C47" s="5"/>
       <c r="D47" s="6"/>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="6"/>
       <c r="C48" s="5"/>
       <c r="D48" s="6"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="6"/>
       <c r="C49" s="5"/>
       <c r="D49" s="6"/>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="6"/>
       <c r="C50" s="5"/>
       <c r="D50" s="6"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
       <c r="B51" s="6"/>
       <c r="C51" s="5"/>
       <c r="D51" s="6"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="6"/>
       <c r="C52" s="5"/>
       <c r="D52" s="6"/>
       <c r="E52" s="5"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="6"/>
       <c r="C53" s="5"/>
       <c r="D53" s="6"/>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="6"/>
       <c r="C54" s="5"/>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="6"/>
       <c r="C55" s="5"/>
       <c r="D55" s="6"/>
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="6"/>
       <c r="C56" s="5"/>
       <c r="D56" s="6"/>
       <c r="E56" s="5"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="6"/>
       <c r="C57" s="5"/>
       <c r="D57" s="6"/>
       <c r="E57" s="5"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="6"/>
       <c r="C58" s="5"/>
       <c r="D58" s="6"/>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="6"/>
       <c r="C59" s="5"/>
       <c r="D59" s="6"/>
       <c r="E59" s="5"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
       <c r="B60" s="6"/>
       <c r="C60" s="5"/>
       <c r="D60" s="6"/>
       <c r="E60" s="5"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
       <c r="B61" s="6"/>
       <c r="C61" s="5"/>
       <c r="D61" s="6"/>
       <c r="E61" s="5"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
       <c r="B62" s="6"/>
       <c r="C62" s="5"/>
       <c r="D62" s="6"/>
       <c r="E62" s="5"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="5"/>
       <c r="B63" s="6"/>
       <c r="C63" s="5"/>
       <c r="D63" s="6"/>
       <c r="E63" s="5"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
       <c r="B64" s="6"/>
       <c r="C64" s="5"/>
       <c r="D64" s="6"/>
       <c r="E64" s="5"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="5"/>
       <c r="B65" s="6"/>
       <c r="C65" s="5"/>
       <c r="D65" s="6"/>
       <c r="E65" s="5"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
       <c r="B66" s="6"/>
       <c r="C66" s="5"/>
       <c r="D66" s="6"/>
       <c r="E66" s="5"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="6"/>
       <c r="C67" s="5"/>
       <c r="D67" s="6"/>
       <c r="E67" s="5"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="6"/>
       <c r="C68" s="5"/>
       <c r="D68" s="6"/>
       <c r="E68" s="5"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="6"/>
       <c r="C69" s="5"/>
       <c r="D69" s="6"/>
       <c r="E69" s="5"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="6"/>
       <c r="C70" s="5"/>
       <c r="D70" s="6"/>
       <c r="E70" s="5"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
       <c r="B71" s="6"/>
       <c r="C71" s="5"/>
       <c r="D71" s="6"/>
       <c r="E71" s="5"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
       <c r="B72" s="6"/>
       <c r="C72" s="5"/>
       <c r="D72" s="6"/>
       <c r="E72" s="5"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="6"/>
       <c r="C73" s="5"/>
       <c r="D73" s="6"/>
       <c r="E73" s="5"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="6"/>
       <c r="C74" s="5"/>
       <c r="D74" s="6"/>
       <c r="E74" s="5"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
       <c r="B75" s="6"/>
       <c r="C75" s="5"/>
       <c r="D75" s="6"/>
       <c r="E75" s="5"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
       <c r="B76" s="6"/>
       <c r="C76" s="5"/>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
       <c r="B77" s="6"/>
       <c r="C77" s="5"/>
       <c r="D77" s="6"/>
       <c r="E77" s="5"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
       <c r="B78" s="6"/>
       <c r="C78" s="5"/>
       <c r="D78" s="6"/>
       <c r="E78" s="5"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
       <c r="B79" s="6"/>
       <c r="C79" s="5"/>
       <c r="D79" s="6"/>
       <c r="E79" s="5"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
       <c r="B80" s="6"/>
       <c r="C80" s="5"/>
       <c r="D80" s="6"/>
       <c r="E80" s="5"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="5"/>
       <c r="B81" s="6"/>
       <c r="C81" s="5"/>
       <c r="D81" s="6"/>
       <c r="E81" s="5"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="5"/>
       <c r="B82" s="6"/>
       <c r="C82" s="5"/>
       <c r="D82" s="6"/>
       <c r="E82" s="5"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="5"/>
       <c r="B83" s="6"/>
       <c r="C83" s="5"/>
       <c r="D83" s="6"/>
       <c r="E83" s="5"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="5"/>
       <c r="B84" s="6"/>
       <c r="C84" s="5"/>
       <c r="D84" s="6"/>
       <c r="E84" s="5"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="5"/>
       <c r="B85" s="6"/>
       <c r="C85" s="5"/>
       <c r="D85" s="6"/>
       <c r="E85" s="5"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="5"/>
       <c r="B86" s="6"/>
       <c r="C86" s="5"/>
       <c r="D86" s="6"/>
       <c r="E86" s="5"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="5"/>
       <c r="B87" s="6"/>
       <c r="C87" s="5"/>
       <c r="D87" s="6"/>
       <c r="E87" s="5"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="5"/>
       <c r="B88" s="6"/>
       <c r="C88" s="5"/>
       <c r="D88" s="6"/>
       <c r="E88" s="5"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="5"/>
       <c r="B89" s="6"/>
       <c r="C89" s="5"/>
       <c r="D89" s="6"/>
       <c r="E89" s="5"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="5"/>
       <c r="B90" s="6"/>
       <c r="C90" s="5"/>
       <c r="D90" s="6"/>
       <c r="E90" s="5"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="5"/>
       <c r="B91" s="6"/>
       <c r="C91" s="5"/>
       <c r="D91" s="6"/>
       <c r="E91" s="5"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="5"/>
       <c r="B92" s="6"/>
       <c r="C92" s="5"/>
       <c r="D92" s="6"/>
       <c r="E92" s="5"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="5"/>
       <c r="B93" s="6"/>
       <c r="C93" s="5"/>
       <c r="D93" s="6"/>
       <c r="E93" s="5"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="5"/>
       <c r="B94" s="6"/>
       <c r="C94" s="5"/>
       <c r="D94" s="6"/>
       <c r="E94" s="5"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="5"/>
       <c r="B95" s="6"/>
       <c r="C95" s="5"/>
       <c r="D95" s="6"/>
       <c r="E95" s="5"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="5"/>
       <c r="B96" s="6"/>
       <c r="C96" s="5"/>
       <c r="D96" s="6"/>
       <c r="E96" s="5"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="5"/>
       <c r="B97" s="6"/>
       <c r="C97" s="5"/>
       <c r="D97" s="6"/>
       <c r="E97" s="5"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="5"/>
       <c r="B98" s="6"/>
       <c r="C98" s="5"/>
       <c r="D98" s="6"/>
       <c r="E98" s="5"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
       <c r="B99" s="6"/>
       <c r="C99" s="5"/>
       <c r="D99" s="6"/>
       <c r="E99" s="5"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="5"/>
       <c r="B100" s="6"/>
       <c r="C100" s="5"/>
       <c r="D100" s="6"/>
       <c r="E100" s="5"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="5"/>
       <c r="B101" s="6"/>
       <c r="C101" s="5"/>
       <c r="D101" s="6"/>
       <c r="E101" s="5"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="5"/>
       <c r="B102" s="6"/>
       <c r="C102" s="5"/>
       <c r="D102" s="6"/>
       <c r="E102" s="5"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="5"/>
       <c r="B103" s="6"/>
       <c r="C103" s="5"/>
       <c r="D103" s="6"/>
       <c r="E103" s="5"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="5"/>
       <c r="B104" s="6"/>
       <c r="C104" s="5"/>
       <c r="D104" s="6"/>
       <c r="E104" s="5"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="5"/>
       <c r="B105" s="6"/>
       <c r="C105" s="5"/>
       <c r="D105" s="6"/>
       <c r="E105" s="5"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="5"/>
       <c r="B106" s="6"/>
       <c r="C106" s="5"/>
       <c r="D106" s="6"/>
       <c r="E106" s="5"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="5"/>
       <c r="B107" s="6"/>
       <c r="C107" s="5"/>
       <c r="D107" s="6"/>
       <c r="E107" s="5"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="5"/>
       <c r="B108" s="6"/>
       <c r="C108" s="5"/>
       <c r="D108" s="6"/>
       <c r="E108" s="5"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="5"/>
       <c r="B109" s="6"/>
       <c r="C109" s="5"/>
       <c r="D109" s="6"/>
       <c r="E109" s="5"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="5"/>
       <c r="B110" s="6"/>
       <c r="C110" s="5"/>
       <c r="D110" s="6"/>
       <c r="E110" s="5"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="5"/>
       <c r="B111" s="6"/>
       <c r="C111" s="5"/>
       <c r="D111" s="6"/>
       <c r="E111" s="5"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="5"/>
       <c r="B112" s="6"/>
       <c r="C112" s="5"/>
       <c r="D112" s="6"/>
       <c r="E112" s="5"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="5"/>
       <c r="B113" s="6"/>
       <c r="C113" s="5"/>
       <c r="D113" s="6"/>
       <c r="E113" s="5"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="5"/>
       <c r="B114" s="6"/>
       <c r="C114" s="5"/>
       <c r="D114" s="6"/>
       <c r="E114" s="5"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="5"/>
       <c r="B115" s="6"/>
       <c r="C115" s="5"/>
       <c r="D115" s="6"/>
       <c r="E115" s="5"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="5"/>
       <c r="B116" s="6"/>
       <c r="C116" s="5"/>
       <c r="D116" s="6"/>
       <c r="E116" s="5"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="5"/>
       <c r="B117" s="6"/>
       <c r="C117" s="5"/>
       <c r="D117" s="6"/>
       <c r="E117" s="5"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="5"/>
       <c r="B118" s="6"/>
       <c r="C118" s="5"/>
       <c r="D118" s="6"/>
       <c r="E118" s="5"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="5"/>
       <c r="B119" s="6"/>
       <c r="C119" s="5"/>
       <c r="D119" s="6"/>
       <c r="E119" s="5"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="5"/>
       <c r="B120" s="6"/>
       <c r="C120" s="5"/>
       <c r="D120" s="6"/>
       <c r="E120" s="5"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="5"/>
       <c r="B121" s="6"/>
       <c r="C121" s="5"/>
       <c r="D121" s="6"/>
       <c r="E121" s="5"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="5"/>
       <c r="B122" s="6"/>
       <c r="C122" s="5"/>
       <c r="D122" s="6"/>
       <c r="E122" s="5"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="5"/>
       <c r="B123" s="6"/>
       <c r="C123" s="5"/>
       <c r="D123" s="6"/>
       <c r="E123" s="5"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="5"/>
       <c r="B124" s="6"/>
       <c r="C124" s="5"/>
       <c r="D124" s="6"/>
       <c r="E124" s="5"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="5"/>
       <c r="B125" s="6"/>
       <c r="C125" s="5"/>
       <c r="D125" s="6"/>
       <c r="E125" s="5"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="5"/>
       <c r="B126" s="6"/>
       <c r="C126" s="5"/>
       <c r="D126" s="6"/>
       <c r="E126" s="5"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="5"/>
       <c r="B127" s="6"/>
       <c r="C127" s="5"/>
       <c r="D127" s="6"/>
       <c r="E127" s="5"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="5"/>
       <c r="B128" s="6"/>
       <c r="C128" s="5"/>
       <c r="D128" s="6"/>
       <c r="E128" s="5"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="5"/>
       <c r="B129" s="6"/>
       <c r="C129" s="5"/>
       <c r="D129" s="6"/>
       <c r="E129" s="5"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="5"/>
       <c r="B130" s="6"/>
       <c r="C130" s="5"/>
       <c r="D130" s="6"/>
       <c r="E130" s="5"/>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="5"/>
       <c r="B131" s="6"/>
       <c r="C131" s="5"/>
       <c r="D131" s="6"/>
       <c r="E131" s="5"/>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="5"/>
       <c r="B132" s="6"/>
       <c r="C132" s="5"/>
       <c r="D132" s="6"/>
       <c r="E132" s="5"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="5"/>
       <c r="B133" s="6"/>
       <c r="C133" s="5"/>
       <c r="D133" s="6"/>
       <c r="E133" s="5"/>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="5"/>
       <c r="B134" s="6"/>
       <c r="C134" s="5"/>
       <c r="D134" s="6"/>
       <c r="E134" s="5"/>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="5"/>
       <c r="B135" s="6"/>
       <c r="C135" s="5"/>
       <c r="D135" s="6"/>
       <c r="E135" s="5"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="5"/>
       <c r="B136" s="6"/>
       <c r="C136" s="5"/>
       <c r="D136" s="6"/>
       <c r="E136" s="5"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="5"/>
       <c r="B137" s="6"/>
       <c r="C137" s="5"/>
       <c r="D137" s="6"/>
       <c r="E137" s="5"/>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="5"/>
       <c r="B138" s="6"/>
       <c r="C138" s="5"/>
       <c r="D138" s="6"/>
       <c r="E138" s="5"/>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="5"/>
       <c r="B139" s="6"/>
       <c r="C139" s="5"/>
       <c r="D139" s="6"/>
       <c r="E139" s="5"/>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="5"/>
       <c r="B140" s="6"/>
       <c r="C140" s="5"/>
       <c r="D140" s="6"/>
       <c r="E140" s="5"/>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="5"/>
       <c r="B141" s="6"/>
       <c r="C141" s="5"/>
       <c r="D141" s="6"/>
       <c r="E141" s="5"/>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="5"/>
       <c r="B142" s="6"/>
       <c r="C142" s="5"/>
       <c r="D142" s="6"/>
       <c r="E142" s="5"/>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="5"/>
       <c r="B143" s="6"/>
       <c r="C143" s="5"/>
       <c r="D143" s="6"/>
       <c r="E143" s="5"/>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="5"/>
       <c r="B144" s="6"/>
       <c r="C144" s="5"/>
       <c r="D144" s="6"/>
       <c r="E144" s="5"/>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="5"/>
       <c r="B145" s="6"/>
       <c r="C145" s="5"/>
       <c r="D145" s="6"/>
       <c r="E145" s="5"/>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="5"/>
       <c r="B146" s="6"/>
       <c r="C146" s="5"/>
       <c r="D146" s="6"/>
       <c r="E146" s="5"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="5"/>
       <c r="B147" s="6"/>
       <c r="C147" s="5"/>
       <c r="D147" s="6"/>
       <c r="E147" s="5"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="5"/>
       <c r="B148" s="6"/>
       <c r="C148" s="5"/>
       <c r="D148" s="6"/>
       <c r="E148" s="5"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="5"/>
       <c r="B149" s="6"/>
       <c r="C149" s="5"/>
       <c r="D149" s="6"/>
       <c r="E149" s="5"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="5"/>
       <c r="B150" s="6"/>
       <c r="C150" s="5"/>
       <c r="D150" s="6"/>
       <c r="E150" s="5"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="5"/>
       <c r="B151" s="6"/>
       <c r="C151" s="5"/>
       <c r="D151" s="6"/>
       <c r="E151" s="5"/>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="5"/>
       <c r="B152" s="6"/>
       <c r="C152" s="5"/>
       <c r="D152" s="6"/>
       <c r="E152" s="5"/>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="5"/>
       <c r="B153" s="6"/>
       <c r="C153" s="5"/>
       <c r="D153" s="6"/>
       <c r="E153" s="5"/>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="5"/>
       <c r="B154" s="6"/>
       <c r="C154" s="5"/>
       <c r="D154" s="6"/>
       <c r="E154" s="5"/>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="5"/>
       <c r="B155" s="6"/>
       <c r="C155" s="5"/>
       <c r="D155" s="6"/>
       <c r="E155" s="5"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="5"/>
       <c r="B156" s="6"/>
       <c r="C156" s="5"/>
       <c r="D156" s="6"/>
       <c r="E156" s="5"/>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="5"/>
       <c r="B157" s="6"/>
       <c r="C157" s="5"/>
       <c r="D157" s="6"/>
       <c r="E157" s="5"/>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="5"/>
       <c r="B158" s="6"/>
       <c r="C158" s="5"/>
       <c r="D158" s="6"/>
       <c r="E158" s="5"/>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="5"/>
       <c r="B159" s="6"/>
       <c r="C159" s="5"/>
       <c r="D159" s="6"/>
       <c r="E159" s="5"/>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="5"/>
       <c r="B160" s="6"/>
       <c r="C160" s="5"/>
       <c r="D160" s="6"/>
       <c r="E160" s="5"/>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="5"/>
       <c r="B161" s="6"/>
       <c r="C161" s="5"/>
       <c r="D161" s="6"/>
       <c r="E161" s="5"/>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="5"/>
       <c r="B162" s="6"/>
       <c r="C162" s="5"/>
       <c r="D162" s="6"/>
       <c r="E162" s="5"/>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="5"/>
       <c r="B163" s="6"/>
       <c r="C163" s="5"/>
       <c r="D163" s="6"/>
       <c r="E163" s="5"/>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="5"/>
       <c r="B164" s="6"/>
       <c r="C164" s="5"/>
       <c r="D164" s="6"/>
       <c r="E164" s="5"/>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="5"/>
       <c r="B165" s="6"/>
       <c r="C165" s="5"/>
       <c r="D165" s="6"/>
       <c r="E165" s="5"/>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="5"/>
       <c r="B166" s="6"/>
       <c r="C166" s="5"/>
       <c r="D166" s="6"/>
       <c r="E166" s="5"/>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="5"/>
       <c r="B167" s="6"/>
       <c r="C167" s="5"/>
       <c r="D167" s="6"/>
       <c r="E167" s="5"/>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="5"/>
       <c r="B168" s="6"/>
       <c r="C168" s="5"/>
       <c r="D168" s="6"/>
       <c r="E168" s="5"/>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="5"/>
       <c r="B169" s="6"/>
       <c r="C169" s="5"/>
       <c r="D169" s="6"/>
       <c r="E169" s="5"/>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="5"/>
       <c r="B170" s="6"/>
       <c r="C170" s="5"/>
       <c r="D170" s="6"/>
       <c r="E170" s="5"/>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="5"/>
       <c r="B171" s="6"/>
       <c r="C171" s="5"/>

</xml_diff>

<commit_message>
Added module to measure intensity along an object path
The object path must be a single pixel-wide strip (skeletonisation is
performed first)
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stephen\Programming\Java Projects\mia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41707D00-A12D-42E7-B1DA-C870B9BAEA24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B69D4A-6480-4271-AC71-DA6C1BD3CB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
@@ -285,9 +285,6 @@
     <t>Run single command</t>
   </si>
   <si>
-    <t>Measure longest path texture</t>
-  </si>
-  <si>
     <t>Measure object colocalisation</t>
   </si>
   <si>
@@ -601,6 +598,9 @@
   </si>
   <si>
     <t>Track editor</t>
+  </si>
+  <si>
+    <t>Measure intensity along path</t>
   </si>
 </sst>
 </file>
@@ -722,10 +722,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$67</c:f>
+              <c:f>Sheet1!$B$2:$B$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -923,16 +923,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$67</c:f>
+              <c:f>Sheet1!$N$2:$N$68</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -1129,6 +1132,9 @@
                   <c:v>86.338797814207652</c:v>
                 </c:pt>
                 <c:pt idx="65">
+                  <c:v>86.338797814207652</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>86.338797814207652</c:v>
                 </c:pt>
               </c:numCache>
@@ -1169,10 +1175,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$67</c:f>
+              <c:f>Sheet1!$B$2:$B$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1370,18 +1376,21 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$67</c:f>
+              <c:f>Sheet1!$O$2:$O$68</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
-                  <c:v>14.045991298943443</c:v>
+                  <c:v>13.848039215686274</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -1577,6 +1586,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>86.645126548196018</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>87.600644122383258</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1616,10 +1628,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$67</c:f>
+              <c:f>Sheet1!$B$2:$B$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1817,16 +1829,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$67</c:f>
+              <c:f>Sheet1!$P$2:$P$68</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -2024,6 +2039,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>80.327868852459019</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>81.967213114754102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2063,10 +2081,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$67</c:f>
+              <c:f>Sheet1!$B$2:$B$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2264,16 +2282,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$67</c:f>
+              <c:f>Sheet1!$Q$2:$Q$68</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2470,6 +2491,9 @@
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="65">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
               </c:numCache>
@@ -2510,10 +2534,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$67</c:f>
+              <c:f>Sheet1!$B$2:$B$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2711,16 +2735,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$67</c:f>
+              <c:f>Sheet1!$R$2:$R$68</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -2918,6 +2945,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>36.324786324786324</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>36.956521739130437</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3172,10 +3202,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$67</c:f>
+              <c:f>Sheet1!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3373,16 +3403,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>44427</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>44431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$67</c:f>
+              <c:f>Sheet1!$N$2:$N$68</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -3579,6 +3612,9 @@
                   <c:v>86.338797814207652</c:v>
                 </c:pt>
                 <c:pt idx="65">
+                  <c:v>86.338797814207652</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>86.338797814207652</c:v>
                 </c:pt>
               </c:numCache>
@@ -3608,10 +3644,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$67</c:f>
+              <c:f>Sheet1!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3809,18 +3845,21 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>44427</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>44431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$67</c:f>
+              <c:f>Sheet1!$O$2:$O$68</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
-                  <c:v>14.045991298943443</c:v>
+                  <c:v>13.848039215686274</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -4016,6 +4055,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>86.645126548196018</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>87.600644122383258</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4044,10 +4086,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$67</c:f>
+              <c:f>Sheet1!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4245,16 +4287,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>44427</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>44431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$67</c:f>
+              <c:f>Sheet1!$P$2:$P$68</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -4452,6 +4497,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>80.327868852459019</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>81.967213114754102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4480,10 +4528,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$67</c:f>
+              <c:f>Sheet1!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4681,16 +4729,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>44427</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>44431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$67</c:f>
+              <c:f>Sheet1!$Q$2:$Q$68</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -4887,6 +4938,9 @@
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="65">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
               </c:numCache>
@@ -4916,10 +4970,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$67</c:f>
+              <c:f>Sheet1!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -5117,16 +5171,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>44427</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>44431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$67</c:f>
+              <c:f>Sheet1!$R$2:$R$68</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -5324,6 +5381,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>36.324786324786324</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>36.956521739130437</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7041,10 +7101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:R67"/>
+  <dimension ref="A1:R68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7156,7 +7216,7 @@
       </c>
       <c r="O2" s="3">
         <f>100*G2/MAX(G:G)</f>
-        <v>14.045991298943443</v>
+        <v>13.848039215686274</v>
       </c>
       <c r="P2" s="3">
         <f t="shared" ref="P2:P7" si="1">100*H2/D2</f>
@@ -10746,6 +10806,61 @@
       <c r="R67" s="3">
         <f t="shared" ref="R67" si="298">100*L67/K67</f>
         <v>36.324786324786324</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>44431</v>
+      </c>
+      <c r="B68" s="4">
+        <v>67</v>
+      </c>
+      <c r="D68">
+        <v>183</v>
+      </c>
+      <c r="E68">
+        <v>158</v>
+      </c>
+      <c r="F68">
+        <v>1863</v>
+      </c>
+      <c r="G68">
+        <v>1632</v>
+      </c>
+      <c r="H68">
+        <v>150</v>
+      </c>
+      <c r="I68">
+        <v>44</v>
+      </c>
+      <c r="J68">
+        <v>18</v>
+      </c>
+      <c r="K68">
+        <v>230</v>
+      </c>
+      <c r="L68">
+        <v>85</v>
+      </c>
+      <c r="N68" s="3">
+        <f t="shared" ref="N68" si="299">100*E68/D68</f>
+        <v>86.338797814207652</v>
+      </c>
+      <c r="O68" s="3">
+        <f t="shared" ref="O68" si="300">100*G68/F68</f>
+        <v>87.600644122383258</v>
+      </c>
+      <c r="P68" s="3">
+        <f t="shared" ref="P68" si="301">100*H68/D68</f>
+        <v>81.967213114754102</v>
+      </c>
+      <c r="Q68" s="3">
+        <f t="shared" ref="Q68" si="302">100*J68/I68</f>
+        <v>40.909090909090907</v>
+      </c>
+      <c r="R68" s="3">
+        <f t="shared" ref="R68" si="303">100*L68/K68</f>
+        <v>36.956521739130437</v>
       </c>
     </row>
   </sheetData>
@@ -10761,7 +10876,7 @@
   <dimension ref="A1:G175"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10777,7 +10892,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="5" t="b">
         <v>0</v>
@@ -10800,7 +10915,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="5" t="b">
         <v>0</v>
@@ -10823,7 +10938,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" s="5" t="b">
         <v>1</v>
@@ -10846,7 +10961,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="5" t="b">
         <v>1</v>
@@ -10869,7 +10984,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="5" t="b">
         <v>1</v>
@@ -10892,7 +11007,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="5" t="b">
         <v>0</v>
@@ -10961,7 +11076,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="5" t="b">
         <v>1</v>
@@ -10984,7 +11099,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="5" t="b">
         <v>1</v>
@@ -11007,7 +11122,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B11" s="5" t="b">
         <v>0</v>
@@ -11030,7 +11145,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B12" s="5" t="b">
         <v>1</v>
@@ -11053,7 +11168,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B13" s="5" t="b">
         <v>0</v>
@@ -11099,7 +11214,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B15" s="5" t="b">
         <v>0</v>
@@ -11122,36 +11237,36 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="B16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="5">
-        <v>0.625</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <v>6</v>
       </c>
       <c r="E16" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>100</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B17" s="5" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="5">
-        <v>0</v>
+        <v>0.1429</v>
       </c>
       <c r="D17">
         <v>6</v>
@@ -11168,13 +11283,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B18" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="5">
-        <v>0.1429</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -11183,21 +11298,21 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="B19" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="5">
-        <v>0.5</v>
+        <v>0.1429</v>
       </c>
       <c r="D19">
         <v>6</v>
@@ -11206,7 +11321,7 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -11214,10 +11329,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="B20" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="5">
         <v>0</v>
@@ -11229,7 +11344,7 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -11237,16 +11352,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="B21" s="5" t="b">
         <v>0</v>
       </c>
       <c r="C21" s="5">
-        <v>0.1429</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>
@@ -11260,16 +11375,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="B22" s="5" t="b">
         <v>0</v>
       </c>
       <c r="C22" s="5">
-        <v>0</v>
+        <v>0.28570000000000001</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
@@ -11283,13 +11398,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="B23" s="5" t="b">
         <v>0</v>
       </c>
       <c r="C23" s="5">
-        <v>0.58330000000000004</v>
+        <v>0.44440000000000002</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -11306,19 +11421,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>187</v>
+        <v>33</v>
       </c>
       <c r="B24" s="5" t="b">
         <v>0</v>
       </c>
       <c r="C24" s="5">
-        <v>0.28570000000000001</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E24" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>100</v>
@@ -11329,16 +11444,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>185</v>
+        <v>15</v>
       </c>
       <c r="B25" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="5">
-        <v>0.44440000000000002</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
@@ -11352,19 +11467,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B26" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26">
         <v>100</v>
@@ -11375,22 +11490,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="B27" s="5" t="b">
         <v>1</v>
       </c>
       <c r="C27" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E27" s="5">
         <v>1</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G27" t="b">
         <v>1</v>
@@ -11398,7 +11513,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B28" s="5" t="b">
         <v>1</v>
@@ -11416,12 +11531,12 @@
         <v>100</v>
       </c>
       <c r="G28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B29" s="5" t="b">
         <v>1</v>
@@ -11439,12 +11554,12 @@
         <v>100</v>
       </c>
       <c r="G29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B30" s="5" t="b">
         <v>1</v>
@@ -11462,12 +11577,12 @@
         <v>100</v>
       </c>
       <c r="G30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B31" s="5" t="b">
         <v>1</v>
@@ -11485,12 +11600,12 @@
         <v>100</v>
       </c>
       <c r="G31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B32" s="5" t="b">
         <v>1</v>
@@ -11508,12 +11623,12 @@
         <v>100</v>
       </c>
       <c r="G32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B33" s="5" t="b">
         <v>1</v>
@@ -11528,15 +11643,15 @@
         <v>1</v>
       </c>
       <c r="F33">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B34" s="5" t="b">
         <v>1</v>
@@ -11554,12 +11669,12 @@
         <v>100</v>
       </c>
       <c r="G34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B35" s="5" t="b">
         <v>1</v>
@@ -11582,7 +11697,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B36" s="5" t="b">
         <v>1</v>
@@ -11597,7 +11712,7 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>
@@ -11605,7 +11720,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B37" s="5" t="b">
         <v>1</v>
@@ -11623,12 +11738,12 @@
         <v>100</v>
       </c>
       <c r="G37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B38" s="5" t="b">
         <v>1</v>
@@ -11651,7 +11766,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B39" s="5" t="b">
         <v>1</v>
@@ -11663,7 +11778,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39">
         <v>100</v>
@@ -11674,7 +11789,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B40" s="5" t="b">
         <v>1</v>
@@ -11686,7 +11801,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40">
         <v>100</v>
@@ -11697,7 +11812,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B41" s="5" t="b">
         <v>1</v>
@@ -11720,7 +11835,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B42" s="5" t="b">
         <v>1</v>
@@ -11732,7 +11847,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42">
         <v>100</v>
@@ -11743,7 +11858,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>31</v>
+        <v>173</v>
       </c>
       <c r="B43" s="5" t="b">
         <v>1</v>
@@ -11766,7 +11881,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B44" s="5" t="b">
         <v>1</v>
@@ -11789,7 +11904,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>174</v>
+        <v>36</v>
       </c>
       <c r="B45" s="5" t="b">
         <v>1</v>
@@ -11812,7 +11927,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B46" s="5" t="b">
         <v>1</v>
@@ -11835,7 +11950,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B47" s="5" t="b">
         <v>1</v>
@@ -11858,7 +11973,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>37</v>
+        <v>185</v>
       </c>
       <c r="B48" s="5" t="b">
         <v>1</v>
@@ -11881,7 +11996,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B49" s="5" t="b">
         <v>1</v>
@@ -11904,7 +12019,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>186</v>
+        <v>41</v>
       </c>
       <c r="B50" s="5" t="b">
         <v>1</v>
@@ -11927,7 +12042,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B51" s="5" t="b">
         <v>1</v>
@@ -11950,7 +12065,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B52" s="5" t="b">
         <v>1</v>
@@ -11973,7 +12088,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B53" s="5" t="b">
         <v>1</v>
@@ -11996,7 +12111,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B54" s="5" t="b">
         <v>1</v>
@@ -12019,7 +12134,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B55" s="5" t="b">
         <v>1</v>
@@ -12037,12 +12152,12 @@
         <v>100</v>
       </c>
       <c r="G55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B56" s="5" t="b">
         <v>1</v>
@@ -12065,7 +12180,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B57" s="5" t="b">
         <v>1</v>
@@ -12083,12 +12198,12 @@
         <v>100</v>
       </c>
       <c r="G57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B58" s="5" t="b">
         <v>1</v>
@@ -12111,7 +12226,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B59" s="5" t="b">
         <v>1</v>
@@ -12134,7 +12249,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B60" s="5" t="b">
         <v>1</v>
@@ -12157,7 +12272,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B61" s="5" t="b">
         <v>1</v>
@@ -12180,7 +12295,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B62" s="5" t="b">
         <v>1</v>
@@ -12203,7 +12318,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B63" s="5" t="b">
         <v>1</v>
@@ -12226,7 +12341,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B64" s="5" t="b">
         <v>1</v>
@@ -12249,7 +12364,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B65" s="5" t="b">
         <v>1</v>
@@ -12272,7 +12387,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B66" s="5" t="b">
         <v>1</v>
@@ -12295,7 +12410,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B67" s="5" t="b">
         <v>1</v>
@@ -12318,7 +12433,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B68" s="5" t="b">
         <v>1</v>
@@ -12330,7 +12445,7 @@
         <v>0</v>
       </c>
       <c r="E68" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68">
         <v>100</v>
@@ -12341,7 +12456,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B69" s="5" t="b">
         <v>1</v>
@@ -12364,7 +12479,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B70" s="5" t="b">
         <v>1</v>
@@ -12376,7 +12491,7 @@
         <v>0</v>
       </c>
       <c r="E70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F70">
         <v>100</v>
@@ -12387,7 +12502,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B71" s="5" t="b">
         <v>1</v>
@@ -12410,7 +12525,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B72" s="5" t="b">
         <v>1</v>
@@ -12433,7 +12548,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B73" s="5" t="b">
         <v>1</v>
@@ -12456,7 +12571,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B74" s="5" t="b">
         <v>1</v>
@@ -12479,7 +12594,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B75" s="5" t="b">
         <v>1</v>
@@ -12502,7 +12617,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>68</v>
+        <v>174</v>
       </c>
       <c r="B76" s="5" t="b">
         <v>1</v>
@@ -12525,7 +12640,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>69</v>
+        <v>181</v>
       </c>
       <c r="B77" s="5" t="b">
         <v>1</v>
@@ -12571,7 +12686,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B79" s="5" t="b">
         <v>1</v>
@@ -12594,7 +12709,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B80" s="5" t="b">
         <v>1</v>
@@ -12617,7 +12732,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B81" s="5" t="b">
         <v>1</v>
@@ -12640,7 +12755,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B82" s="5" t="b">
         <v>1</v>
@@ -12663,7 +12778,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>179</v>
+        <v>70</v>
       </c>
       <c r="B83" s="5" t="b">
         <v>1</v>
@@ -12686,7 +12801,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>180</v>
+        <v>71</v>
       </c>
       <c r="B84" s="5" t="b">
         <v>1</v>
@@ -12704,12 +12819,12 @@
         <v>100</v>
       </c>
       <c r="G84" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B85" s="5" t="b">
         <v>1</v>
@@ -12732,7 +12847,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B86" s="5" t="b">
         <v>1</v>
@@ -12750,12 +12865,12 @@
         <v>100</v>
       </c>
       <c r="G86" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B87" s="5" t="b">
         <v>1</v>
@@ -12778,7 +12893,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B88" s="5" t="b">
         <v>1</v>
@@ -12801,7 +12916,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B89" s="5" t="b">
         <v>1</v>
@@ -12824,7 +12939,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B90" s="5" t="b">
         <v>1</v>
@@ -12847,7 +12962,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B91" s="5" t="b">
         <v>1</v>
@@ -12865,12 +12980,12 @@
         <v>100</v>
       </c>
       <c r="G91" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B92" s="5" t="b">
         <v>1</v>
@@ -12893,7 +13008,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B93" s="5" t="b">
         <v>1</v>
@@ -12911,12 +13026,12 @@
         <v>100</v>
       </c>
       <c r="G93" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="B94" s="5" t="b">
         <v>1</v>
@@ -12939,7 +13054,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B95" s="5" t="b">
         <v>1</v>
@@ -12962,7 +13077,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B96" s="5" t="b">
         <v>1</v>
@@ -12985,7 +13100,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B97" s="5" t="b">
         <v>1</v>
@@ -13000,7 +13115,7 @@
         <v>1</v>
       </c>
       <c r="F97">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G97" t="b">
         <v>1</v>
@@ -13008,7 +13123,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B98" s="5" t="b">
         <v>1</v>
@@ -13031,7 +13146,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B99" s="5" t="b">
         <v>1</v>
@@ -13054,7 +13169,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B100" s="5" t="b">
         <v>1</v>
@@ -13077,7 +13192,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B101" s="5" t="b">
         <v>1</v>
@@ -13100,7 +13215,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B102" s="5" t="b">
         <v>1</v>
@@ -13123,7 +13238,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B103" s="5" t="b">
         <v>1</v>
@@ -13146,7 +13261,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B104" s="5" t="b">
         <v>1</v>
@@ -13169,7 +13284,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B105" s="5" t="b">
         <v>1</v>
@@ -13192,7 +13307,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B106" s="5" t="b">
         <v>1</v>
@@ -13215,7 +13330,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B107" s="5" t="b">
         <v>1</v>
@@ -13238,7 +13353,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B108" s="5" t="b">
         <v>1</v>
@@ -13261,7 +13376,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B109" s="5" t="b">
         <v>1</v>
@@ -13284,7 +13399,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B110" s="5" t="b">
         <v>1</v>
@@ -13307,7 +13422,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B111" s="5" t="b">
         <v>1</v>
@@ -13330,7 +13445,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B112" s="5" t="b">
         <v>1</v>
@@ -13353,7 +13468,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B113" s="5" t="b">
         <v>1</v>
@@ -13376,7 +13491,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B114" s="5" t="b">
         <v>1</v>
@@ -13399,7 +13514,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B115" s="5" t="b">
         <v>1</v>
@@ -13422,7 +13537,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B116" s="5" t="b">
         <v>1</v>
@@ -13445,7 +13560,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B117" s="5" t="b">
         <v>1</v>
@@ -13468,7 +13583,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B118" s="5" t="b">
         <v>1</v>
@@ -13491,7 +13606,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B119" s="5" t="b">
         <v>1</v>
@@ -13514,7 +13629,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B120" s="5" t="b">
         <v>1</v>
@@ -13537,7 +13652,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B121" s="5" t="b">
         <v>1</v>
@@ -13560,7 +13675,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B122" s="5" t="b">
         <v>1</v>
@@ -13583,7 +13698,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B123" s="5" t="b">
         <v>1</v>
@@ -13606,7 +13721,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B124" s="5" t="b">
         <v>1</v>
@@ -13629,7 +13744,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B125" s="5" t="b">
         <v>1</v>
@@ -13652,7 +13767,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B126" s="5" t="b">
         <v>1</v>
@@ -13675,7 +13790,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B127" s="5" t="b">
         <v>1</v>
@@ -13698,7 +13813,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B128" s="5" t="b">
         <v>1</v>
@@ -13721,7 +13836,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B129" s="5" t="b">
         <v>1</v>
@@ -13744,7 +13859,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B130" s="5" t="b">
         <v>1</v>
@@ -13767,7 +13882,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B131" s="5" t="b">
         <v>1</v>
@@ -13790,7 +13905,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B132" s="5" t="b">
         <v>1</v>
@@ -13813,7 +13928,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B133" s="5" t="b">
         <v>1</v>
@@ -13836,7 +13951,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B134" s="5" t="b">
         <v>1</v>
@@ -13859,7 +13974,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B135" s="5" t="b">
         <v>1</v>
@@ -13882,7 +13997,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B136" s="5" t="b">
         <v>1</v>
@@ -13905,7 +14020,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B137" s="5" t="b">
         <v>1</v>
@@ -13928,7 +14043,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B138" s="5" t="b">
         <v>1</v>
@@ -13951,7 +14066,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B139" s="5" t="b">
         <v>1</v>
@@ -13974,7 +14089,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B140" s="5" t="b">
         <v>1</v>
@@ -13997,7 +14112,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B141" s="5" t="b">
         <v>1</v>
@@ -14020,7 +14135,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B142" s="5" t="b">
         <v>1</v>
@@ -14043,7 +14158,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B143" s="5" t="b">
         <v>1</v>
@@ -14066,7 +14181,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B144" s="5" t="b">
         <v>1</v>
@@ -14089,7 +14204,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B145" s="5" t="b">
         <v>1</v>
@@ -14112,7 +14227,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B146" s="5" t="b">
         <v>1</v>
@@ -14135,7 +14250,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B147" s="5" t="b">
         <v>1</v>
@@ -14158,7 +14273,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B148" s="5" t="b">
         <v>1</v>
@@ -14181,7 +14296,7 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B149" s="5" t="b">
         <v>1</v>
@@ -14204,7 +14319,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B150" s="5" t="b">
         <v>1</v>
@@ -14227,7 +14342,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B151" s="5" t="b">
         <v>1</v>
@@ -14250,7 +14365,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B152" s="5" t="b">
         <v>1</v>
@@ -14273,7 +14388,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B153" s="5" t="b">
         <v>1</v>
@@ -14296,7 +14411,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B154" s="5" t="b">
         <v>1</v>
@@ -14319,7 +14434,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B155" s="5" t="b">
         <v>1</v>
@@ -14342,7 +14457,7 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B156" s="5" t="b">
         <v>1</v>
@@ -14365,7 +14480,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B157" s="5" t="b">
         <v>1</v>
@@ -14388,7 +14503,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B158" s="5" t="b">
         <v>1</v>
@@ -14411,7 +14526,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B159" s="5" t="b">
         <v>1</v>
@@ -14434,7 +14549,7 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B160" s="5" t="b">
         <v>1</v>
@@ -14457,7 +14572,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B161" s="5" t="b">
         <v>1</v>
@@ -14480,7 +14595,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B162" s="5" t="b">
         <v>1</v>
@@ -14503,7 +14618,7 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B163" s="5" t="b">
         <v>1</v>
@@ -14526,7 +14641,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B164" s="5" t="b">
         <v>1</v>
@@ -14549,7 +14664,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B165" s="5" t="b">
         <v>1</v>
@@ -14572,7 +14687,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B166" s="5" t="b">
         <v>0</v>
@@ -14595,7 +14710,7 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B167" s="5" t="b">
         <v>1</v>
@@ -14618,7 +14733,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B168" s="5" t="b">
         <v>1</v>
@@ -14641,7 +14756,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B169" s="5" t="b">
         <v>1</v>
@@ -14664,7 +14779,7 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B170" s="5" t="b">
         <v>1</v>
@@ -14687,7 +14802,7 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B171" s="5" t="b">
         <v>1</v>
@@ -14710,7 +14825,7 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B172" s="5" t="b">
         <v>1</v>
@@ -14733,7 +14848,7 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B173" s="5" t="b">
         <v>1</v>
@@ -14756,7 +14871,7 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B174" s="5" t="b">
         <v>1</v>
@@ -14778,11 +14893,11 @@
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B175" s="5"/>
+      <c r="A175" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G174">
-    <sortCondition descending="1" ref="D6:D174"/>
+    <sortCondition descending="1" ref="D5:D174"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Simplified somme package names
Removed "Collection" name in favour of plurals
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stephen\Programming\Java Projects\mia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Java Projects\MIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C818E661-31D8-4279-BA38-9A7FB5B33B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B3C54C-72AB-44A7-820A-29E99D8522BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -719,212 +719,215 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$69</c:f>
+              <c:f>Sheet1!$B$2:$B$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>61</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>63</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>66</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
@@ -932,10 +935,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$69</c:f>
+              <c:f>Sheet1!$N$2:$N$70</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -1139,6 +1142,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>86.813186813186817</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>91.329479768786129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1178,212 +1184,215 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$69</c:f>
+              <c:f>Sheet1!$B$2:$B$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>61</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>63</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>66</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
@@ -1391,12 +1400,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$69</c:f>
+              <c:f>Sheet1!$O$2:$O$70</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
-                  <c:v>13.614457831325302</c:v>
+                  <c:v>13.573573573573574</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -1598,6 +1607,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>89.681253376553215</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>89.951377633711502</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1637,212 +1649,215 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$69</c:f>
+              <c:f>Sheet1!$B$2:$B$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>61</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>63</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>66</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
@@ -1850,10 +1865,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$69</c:f>
+              <c:f>Sheet1!$P$2:$P$70</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -2057,6 +2072,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>84.065934065934073</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>89.017341040462426</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2096,212 +2114,215 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$69</c:f>
+              <c:f>Sheet1!$B$2:$B$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>61</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>63</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>66</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
@@ -2309,10 +2330,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$69</c:f>
+              <c:f>Sheet1!$Q$2:$Q$70</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2515,6 +2536,9 @@
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="67">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="68">
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
               </c:numCache>
@@ -2555,212 +2579,215 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$69</c:f>
+              <c:f>Sheet1!$B$2:$B$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>61</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>63</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>66</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
@@ -2768,10 +2795,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$69</c:f>
+              <c:f>Sheet1!$R$2:$R$70</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -2974,6 +3001,9 @@
                   <c:v>36.956521739130437</c:v>
                 </c:pt>
                 <c:pt idx="67">
+                  <c:v>37.387387387387385</c:v>
+                </c:pt>
+                <c:pt idx="68">
                   <c:v>37.387387387387385</c:v>
                 </c:pt>
               </c:numCache>
@@ -3046,6 +3076,8 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="5"/>
+        <c:tickMarkSkip val="5"/>
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
@@ -3102,7 +3134,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1381721568"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -3229,10 +3261,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$69</c:f>
+              <c:f>Sheet1!$A$2:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3436,16 +3468,19 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>44433</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>44441</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$69</c:f>
+              <c:f>Sheet1!$N$2:$N$70</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -3649,6 +3684,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>86.813186813186817</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>91.329479768786129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3677,10 +3715,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$69</c:f>
+              <c:f>Sheet1!$A$2:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3884,18 +3922,21 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>44433</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>44441</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$69</c:f>
+              <c:f>Sheet1!$O$2:$O$70</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
-                  <c:v>13.614457831325302</c:v>
+                  <c:v>13.573573573573574</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -4097,6 +4138,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>89.681253376553215</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>89.951377633711502</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4125,10 +4169,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$69</c:f>
+              <c:f>Sheet1!$A$2:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4332,16 +4376,19 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>44433</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>44441</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$69</c:f>
+              <c:f>Sheet1!$P$2:$P$70</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -4545,6 +4592,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>84.065934065934073</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>89.017341040462426</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4573,10 +4623,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$69</c:f>
+              <c:f>Sheet1!$A$2:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4780,16 +4830,19 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>44433</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>44441</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$69</c:f>
+              <c:f>Sheet1!$Q$2:$Q$70</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -4992,6 +5045,9 @@
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="67">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="68">
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
               </c:numCache>
@@ -5021,10 +5077,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$69</c:f>
+              <c:f>Sheet1!$A$2:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -5228,16 +5284,19 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>44433</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>44441</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$69</c:f>
+              <c:f>Sheet1!$R$2:$R$70</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -5440,6 +5499,9 @@
                   <c:v>36.956521739130437</c:v>
                 </c:pt>
                 <c:pt idx="67">
+                  <c:v>37.387387387387385</c:v>
+                </c:pt>
+                <c:pt idx="68">
                   <c:v>37.387387387387385</c:v>
                 </c:pt>
               </c:numCache>
@@ -5467,6 +5529,7 @@
         <c:axId val="412970511"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="44454"/>
           <c:min val="44054"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -7158,34 +7221,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:R69"/>
+  <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7232,12 +7295,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44054</v>
       </c>
       <c r="B2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="4">
@@ -7273,7 +7336,7 @@
       </c>
       <c r="O2" s="3">
         <f>100*G2/MAX(G:G)</f>
-        <v>13.614457831325302</v>
+        <v>13.573573573573574</v>
       </c>
       <c r="P2" s="3">
         <f t="shared" ref="P2:P7" si="1">100*H2/D2</f>
@@ -7288,12 +7351,12 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44055</v>
       </c>
       <c r="B3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3">
@@ -7344,12 +7407,12 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44056</v>
       </c>
       <c r="B4" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4">
@@ -7400,12 +7463,12 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44057</v>
       </c>
       <c r="B5" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>161</v>
@@ -7455,12 +7518,12 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44058</v>
       </c>
       <c r="B6" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>161</v>
@@ -7510,12 +7573,12 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>44064</v>
       </c>
       <c r="B7" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>161</v>
@@ -7565,12 +7628,12 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>44069</v>
       </c>
       <c r="B8" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>161</v>
@@ -7620,12 +7683,12 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>44070</v>
       </c>
       <c r="B9" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <v>162</v>
@@ -7675,12 +7738,12 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44081</v>
       </c>
       <c r="B10" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>162</v>
@@ -7730,12 +7793,12 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44082</v>
       </c>
       <c r="B11" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>162</v>
@@ -7785,12 +7848,12 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44083</v>
       </c>
       <c r="B12" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12">
         <v>161</v>
@@ -7840,12 +7903,12 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44084</v>
       </c>
       <c r="B13" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13">
         <v>161</v>
@@ -7895,12 +7958,12 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44085</v>
       </c>
       <c r="B14" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14">
         <v>161</v>
@@ -7950,12 +8013,12 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44089</v>
       </c>
       <c r="B15" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15">
         <v>161</v>
@@ -8005,12 +8068,12 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>44090</v>
       </c>
       <c r="B16" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16">
         <v>161</v>
@@ -8060,12 +8123,12 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44091</v>
       </c>
       <c r="B17" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17">
         <v>161</v>
@@ -8115,12 +8178,12 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>44097</v>
       </c>
       <c r="B18" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>164</v>
@@ -8170,12 +8233,12 @@
         <v>38.967136150234744</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>44098</v>
       </c>
       <c r="B19" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19">
         <v>164</v>
@@ -8225,12 +8288,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>44099</v>
       </c>
       <c r="B20" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20">
         <v>164</v>
@@ -8280,12 +8343,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>44102</v>
       </c>
       <c r="B21" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21">
         <v>164</v>
@@ -8335,12 +8398,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>44103</v>
       </c>
       <c r="B22" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22">
         <v>164</v>
@@ -8390,12 +8453,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>44104</v>
       </c>
       <c r="B23" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23">
         <v>164</v>
@@ -8445,12 +8508,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>44110</v>
       </c>
       <c r="B24" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24">
         <v>164</v>
@@ -8500,12 +8563,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>44113</v>
       </c>
       <c r="B25" s="4">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25">
         <v>164</v>
@@ -8555,12 +8618,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>44116</v>
       </c>
       <c r="B26" s="4">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26">
         <v>164</v>
@@ -8610,12 +8673,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>44117</v>
       </c>
       <c r="B27" s="4">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27">
         <v>164</v>
@@ -8665,12 +8728,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>44118</v>
       </c>
       <c r="B28" s="4">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28">
         <v>165</v>
@@ -8720,12 +8783,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>44119</v>
       </c>
       <c r="B29" s="4">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29">
         <v>165</v>
@@ -8775,12 +8838,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>44120</v>
       </c>
       <c r="B30" s="4">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30">
         <v>165</v>
@@ -8830,12 +8893,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>44123</v>
       </c>
       <c r="B31" s="4">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31">
         <v>166</v>
@@ -8885,12 +8948,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>44124</v>
       </c>
       <c r="B32" s="4">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32">
         <v>166</v>
@@ -8940,12 +9003,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>44125</v>
       </c>
       <c r="B33" s="4">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33">
         <v>167</v>
@@ -8995,12 +9058,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>44126</v>
       </c>
       <c r="B34" s="4">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D34">
         <v>166</v>
@@ -9050,12 +9113,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>44127</v>
       </c>
       <c r="B35" s="4">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35">
         <v>166</v>
@@ -9105,12 +9168,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>44130</v>
       </c>
       <c r="B36" s="4">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36">
         <v>166</v>
@@ -9160,12 +9223,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>44131</v>
       </c>
       <c r="B37" s="4">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37">
         <v>166</v>
@@ -9215,12 +9278,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>44132</v>
       </c>
       <c r="B38" s="4">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38">
         <v>166</v>
@@ -9270,12 +9333,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>44134</v>
       </c>
       <c r="B39" s="4">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D39">
         <v>169</v>
@@ -9325,12 +9388,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>44137</v>
       </c>
       <c r="B40" s="4">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40">
         <v>169</v>
@@ -9380,12 +9443,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>44138</v>
       </c>
       <c r="B41" s="4">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D41">
         <v>169</v>
@@ -9435,12 +9498,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>44139</v>
       </c>
       <c r="B42" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D42">
         <v>169</v>
@@ -9490,12 +9553,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>44140</v>
       </c>
       <c r="B43" s="4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D43">
         <v>172</v>
@@ -9545,12 +9608,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>44141</v>
       </c>
       <c r="B44" s="4">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D44">
         <v>172</v>
@@ -9600,12 +9663,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44147</v>
       </c>
       <c r="B45" s="4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D45">
         <v>174</v>
@@ -9655,12 +9718,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44148</v>
       </c>
       <c r="B46" s="4">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D46">
         <v>174</v>
@@ -9710,12 +9773,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>44151</v>
       </c>
       <c r="B47" s="4">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D47">
         <v>174</v>
@@ -9765,12 +9828,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>44152</v>
       </c>
       <c r="B48" s="4">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48">
         <v>174</v>
@@ -9820,12 +9883,12 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>44300</v>
       </c>
       <c r="B49" s="4">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D49">
         <v>179</v>
@@ -9875,12 +9938,12 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>44301</v>
       </c>
       <c r="B50" s="4">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50">
         <v>179</v>
@@ -9930,12 +9993,12 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>44302</v>
       </c>
       <c r="B51" s="4">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D51">
         <v>179</v>
@@ -9985,12 +10048,12 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>44306</v>
       </c>
       <c r="B52" s="4">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D52">
         <v>179</v>
@@ -10040,12 +10103,12 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>44308</v>
       </c>
       <c r="B53" s="4">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D53">
         <v>179</v>
@@ -10095,12 +10158,12 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>44341</v>
       </c>
       <c r="B54" s="4">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D54">
         <v>182</v>
@@ -10150,12 +10213,12 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>44342</v>
       </c>
       <c r="B55" s="4">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D55">
         <v>182</v>
@@ -10205,12 +10268,12 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>44343</v>
       </c>
       <c r="B56" s="4">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D56">
         <v>182</v>
@@ -10260,12 +10323,12 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>44369</v>
       </c>
       <c r="B57" s="4">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D57">
         <v>185</v>
@@ -10315,12 +10378,12 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>44370</v>
       </c>
       <c r="B58" s="4">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D58">
         <v>185</v>
@@ -10370,12 +10433,12 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>44405</v>
       </c>
       <c r="B59" s="4">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D59">
         <v>185</v>
@@ -10425,12 +10488,12 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>44406</v>
       </c>
       <c r="B60" s="4">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D60">
         <v>185</v>
@@ -10480,12 +10543,12 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>44413</v>
       </c>
       <c r="B61" s="4">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D61">
         <v>183</v>
@@ -10535,12 +10598,12 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>44414</v>
       </c>
       <c r="B62" s="4">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D62">
         <v>183</v>
@@ -10590,12 +10653,12 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>44415</v>
       </c>
       <c r="B63" s="4">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D63">
         <v>183</v>
@@ -10645,12 +10708,12 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>44419</v>
       </c>
       <c r="B64" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D64">
         <v>183</v>
@@ -10700,12 +10763,12 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>44420</v>
       </c>
       <c r="B65" s="4">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D65">
         <v>183</v>
@@ -10755,12 +10818,12 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>44421</v>
       </c>
       <c r="B66" s="4">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D66">
         <v>183</v>
@@ -10810,12 +10873,12 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>44427</v>
       </c>
       <c r="B67" s="4">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D67">
         <v>183</v>
@@ -10865,12 +10928,12 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>44431</v>
       </c>
       <c r="B68" s="4">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D68">
         <v>183</v>
@@ -10920,12 +10983,12 @@
         <v>36.956521739130437</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>44433</v>
       </c>
       <c r="B69" s="4">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D69">
         <v>182</v>
@@ -10972,6 +11035,61 @@
       </c>
       <c r="R69" s="3">
         <f t="shared" ref="R69" si="308">100*L69/K69</f>
+        <v>37.387387387387385</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>44441</v>
+      </c>
+      <c r="B70" s="4">
+        <v>68</v>
+      </c>
+      <c r="D70">
+        <v>173</v>
+      </c>
+      <c r="E70">
+        <v>158</v>
+      </c>
+      <c r="F70">
+        <v>1851</v>
+      </c>
+      <c r="G70">
+        <v>1665</v>
+      </c>
+      <c r="H70">
+        <v>154</v>
+      </c>
+      <c r="I70">
+        <v>44</v>
+      </c>
+      <c r="J70">
+        <v>18</v>
+      </c>
+      <c r="K70">
+        <v>222</v>
+      </c>
+      <c r="L70">
+        <v>83</v>
+      </c>
+      <c r="N70" s="3">
+        <f t="shared" ref="N70" si="309">100*E70/D70</f>
+        <v>91.329479768786129</v>
+      </c>
+      <c r="O70" s="3">
+        <f t="shared" ref="O70" si="310">100*G70/F70</f>
+        <v>89.951377633711502</v>
+      </c>
+      <c r="P70" s="3">
+        <f t="shared" ref="P70" si="311">100*H70/D70</f>
+        <v>89.017341040462426</v>
+      </c>
+      <c r="Q70" s="3">
+        <f t="shared" ref="Q70" si="312">100*J70/I70</f>
+        <v>40.909090909090907</v>
+      </c>
+      <c r="R70" s="3">
+        <f t="shared" ref="R70" si="313">100*L70/K70</f>
         <v>37.387387387387385</v>
       </c>
     </row>
@@ -10988,21 +11106,21 @@
   <dimension ref="A1:G173"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="I170" sqref="I170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>101</v>
       </c>
@@ -11025,7 +11143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>103</v>
       </c>
@@ -11048,7 +11166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>109</v>
       </c>
@@ -11071,7 +11189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>99</v>
       </c>
@@ -11094,7 +11212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>111</v>
       </c>
@@ -11117,7 +11235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>66</v>
       </c>
@@ -11140,7 +11258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>71</v>
       </c>
@@ -11163,7 +11281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>107</v>
       </c>
@@ -11186,7 +11304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>112</v>
       </c>
@@ -11209,7 +11327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>143</v>
       </c>
@@ -11232,7 +11350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>145</v>
       </c>
@@ -11255,7 +11373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>52</v>
       </c>
@@ -11278,7 +11396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>59</v>
       </c>
@@ -11301,7 +11419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>84</v>
       </c>
@@ -11324,7 +11442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>122</v>
       </c>
@@ -11347,7 +11465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>146</v>
       </c>
@@ -11370,7 +11488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
@@ -11393,7 +11511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>184</v>
       </c>
@@ -11416,7 +11534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>182</v>
       </c>
@@ -11439,7 +11557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>32</v>
       </c>
@@ -11462,7 +11580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
@@ -11485,7 +11603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
@@ -11508,7 +11626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>33</v>
       </c>
@@ -11531,7 +11649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -11554,7 +11672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
@@ -11577,7 +11695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>30</v>
       </c>
@@ -11600,7 +11718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>31</v>
       </c>
@@ -11623,7 +11741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>171</v>
       </c>
@@ -11646,7 +11764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>34</v>
       </c>
@@ -11669,7 +11787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>19</v>
       </c>
@@ -11692,7 +11810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>35</v>
       </c>
@@ -11715,7 +11833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>36</v>
       </c>
@@ -11738,7 +11856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>37</v>
       </c>
@@ -11761,7 +11879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>183</v>
       </c>
@@ -11784,7 +11902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>38</v>
       </c>
@@ -11807,7 +11925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>40</v>
       </c>
@@ -11830,7 +11948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>41</v>
       </c>
@@ -11853,7 +11971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>42</v>
       </c>
@@ -11876,7 +11994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>43</v>
       </c>
@@ -11899,7 +12017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -11922,7 +12040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>45</v>
       </c>
@@ -11945,7 +12063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>46</v>
       </c>
@@ -11968,7 +12086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>47</v>
       </c>
@@ -11991,7 +12109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>48</v>
       </c>
@@ -12014,7 +12132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>49</v>
       </c>
@@ -12037,7 +12155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>50</v>
       </c>
@@ -12060,7 +12178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>51</v>
       </c>
@@ -12083,7 +12201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>53</v>
       </c>
@@ -12106,7 +12224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>54</v>
       </c>
@@ -12129,7 +12247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>55</v>
       </c>
@@ -12152,7 +12270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>56</v>
       </c>
@@ -12175,7 +12293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>27</v>
       </c>
@@ -12198,7 +12316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>57</v>
       </c>
@@ -12221,7 +12339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>58</v>
       </c>
@@ -12244,7 +12362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>60</v>
       </c>
@@ -12267,7 +12385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>20</v>
       </c>
@@ -12290,7 +12408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>61</v>
       </c>
@@ -12313,7 +12431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>62</v>
       </c>
@@ -12336,7 +12454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>63</v>
       </c>
@@ -12359,7 +12477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>64</v>
       </c>
@@ -12382,7 +12500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>65</v>
       </c>
@@ -12405,7 +12523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>67</v>
       </c>
@@ -12428,7 +12546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>68</v>
       </c>
@@ -12451,7 +12569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>24</v>
       </c>
@@ -12474,7 +12592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>25</v>
       </c>
@@ -12497,7 +12615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>172</v>
       </c>
@@ -12520,7 +12638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>179</v>
       </c>
@@ -12543,7 +12661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>173</v>
       </c>
@@ -12566,7 +12684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>174</v>
       </c>
@@ -12589,7 +12707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>175</v>
       </c>
@@ -12612,7 +12730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>176</v>
       </c>
@@ -12635,7 +12753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>177</v>
       </c>
@@ -12658,7 +12776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>69</v>
       </c>
@@ -12681,7 +12799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>70</v>
       </c>
@@ -12704,7 +12822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>72</v>
       </c>
@@ -12727,7 +12845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>73</v>
       </c>
@@ -12750,7 +12868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>74</v>
       </c>
@@ -12773,7 +12891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>75</v>
       </c>
@@ -12796,7 +12914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>76</v>
       </c>
@@ -12819,7 +12937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>17</v>
       </c>
@@ -12842,7 +12960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>77</v>
       </c>
@@ -12865,7 +12983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>78</v>
       </c>
@@ -12888,7 +13006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>79</v>
       </c>
@@ -12911,7 +13029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>80</v>
       </c>
@@ -12934,7 +13052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>178</v>
       </c>
@@ -12957,7 +13075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>81</v>
       </c>
@@ -12980,7 +13098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>186</v>
       </c>
@@ -13003,7 +13121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>82</v>
       </c>
@@ -13026,7 +13144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>83</v>
       </c>
@@ -13049,7 +13167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>23</v>
       </c>
@@ -13072,7 +13190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>85</v>
       </c>
@@ -13095,7 +13213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>86</v>
       </c>
@@ -13118,7 +13236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>87</v>
       </c>
@@ -13141,7 +13259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>88</v>
       </c>
@@ -13164,7 +13282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>89</v>
       </c>
@@ -13187,7 +13305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>90</v>
       </c>
@@ -13210,7 +13328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>91</v>
       </c>
@@ -13233,7 +13351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>92</v>
       </c>
@@ -13256,7 +13374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>93</v>
       </c>
@@ -13279,7 +13397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>94</v>
       </c>
@@ -13302,7 +13420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>95</v>
       </c>
@@ -13325,7 +13443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>96</v>
       </c>
@@ -13348,7 +13466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>97</v>
       </c>
@@ -13371,7 +13489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>98</v>
       </c>
@@ -13394,7 +13512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>100</v>
       </c>
@@ -13417,7 +13535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>102</v>
       </c>
@@ -13440,7 +13558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>104</v>
       </c>
@@ -13463,7 +13581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>105</v>
       </c>
@@ -13486,7 +13604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>106</v>
       </c>
@@ -13509,7 +13627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>108</v>
       </c>
@@ -13532,7 +13650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>110</v>
       </c>
@@ -13555,7 +13673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>180</v>
       </c>
@@ -13578,7 +13696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>113</v>
       </c>
@@ -13601,7 +13719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>114</v>
       </c>
@@ -13624,7 +13742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>115</v>
       </c>
@@ -13647,7 +13765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>116</v>
       </c>
@@ -13670,7 +13788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>117</v>
       </c>
@@ -13693,7 +13811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>118</v>
       </c>
@@ -13716,7 +13834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>119</v>
       </c>
@@ -13739,7 +13857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>181</v>
       </c>
@@ -13762,7 +13880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>120</v>
       </c>
@@ -13785,7 +13903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>121</v>
       </c>
@@ -13808,7 +13926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>124</v>
       </c>
@@ -13831,7 +13949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>123</v>
       </c>
@@ -13854,7 +13972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>125</v>
       </c>
@@ -13877,7 +13995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>126</v>
       </c>
@@ -13900,7 +14018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>127</v>
       </c>
@@ -13923,7 +14041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>128</v>
       </c>
@@ -13946,7 +14064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>129</v>
       </c>
@@ -13969,7 +14087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>130</v>
       </c>
@@ -13992,7 +14110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>21</v>
       </c>
@@ -14015,7 +14133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>131</v>
       </c>
@@ -14038,7 +14156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>132</v>
       </c>
@@ -14061,7 +14179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>133</v>
       </c>
@@ -14084,7 +14202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>134</v>
       </c>
@@ -14107,7 +14225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>135</v>
       </c>
@@ -14130,7 +14248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>136</v>
       </c>
@@ -14153,7 +14271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>137</v>
       </c>
@@ -14176,7 +14294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>138</v>
       </c>
@@ -14199,7 +14317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>139</v>
       </c>
@@ -14222,7 +14340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>185</v>
       </c>
@@ -14245,7 +14363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>140</v>
       </c>
@@ -14268,7 +14386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>141</v>
       </c>
@@ -14291,7 +14409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>26</v>
       </c>
@@ -14314,7 +14432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>142</v>
       </c>
@@ -14337,7 +14455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>144</v>
       </c>
@@ -14360,7 +14478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>147</v>
       </c>
@@ -14383,7 +14501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>148</v>
       </c>
@@ -14406,7 +14524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>149</v>
       </c>
@@ -14429,7 +14547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>150</v>
       </c>
@@ -14452,7 +14570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>151</v>
       </c>
@@ -14475,7 +14593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>152</v>
       </c>
@@ -14498,7 +14616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>153</v>
       </c>
@@ -14521,7 +14639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>154</v>
       </c>
@@ -14544,7 +14662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>155</v>
       </c>
@@ -14567,7 +14685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>156</v>
       </c>
@@ -14590,7 +14708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>157</v>
       </c>
@@ -14613,7 +14731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>158</v>
       </c>
@@ -14636,7 +14754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>18</v>
       </c>
@@ -14659,7 +14777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>159</v>
       </c>
@@ -14682,7 +14800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>160</v>
       </c>
@@ -14705,7 +14823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>161</v>
       </c>
@@ -14728,7 +14846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>162</v>
       </c>
@@ -14751,7 +14869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>163</v>
       </c>
@@ -14774,7 +14892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>164</v>
       </c>
@@ -14797,7 +14915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>165</v>
       </c>
@@ -14820,7 +14938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>166</v>
       </c>
@@ -14843,7 +14961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>167</v>
       </c>
@@ -14866,7 +14984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>168</v>
       </c>
@@ -14889,7 +15007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>22</v>
       </c>
@@ -14912,7 +15030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>169</v>
       </c>
@@ -14935,7 +15053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>170</v>
       </c>
@@ -14958,7 +15076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>187</v>
       </c>
@@ -14983,7 +15101,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G173">
-    <sortCondition descending="1" ref="D4:D173"/>
+    <sortCondition descending="1" ref="D12:D173"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Consolidated FitSpline and MeasureObjectCurvature modules
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Java Projects\MIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stephen\Programming\Java Projects\mia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AFD468-9F9B-46D3-BED5-AA14CEDECC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D178D4B1-1961-4843-B6F0-112B55FAB5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" activeTab="1" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
   <si>
     <t>Date</t>
   </si>
@@ -210,9 +210,6 @@
     <t>White balance correction</t>
   </si>
   <si>
-    <t>Apply offset correction</t>
-  </si>
-  <si>
     <t>Best focus stack</t>
   </si>
   <si>
@@ -336,9 +333,6 @@
     <t>Fit longest chord</t>
   </si>
   <si>
-    <t>Fit spline</t>
-  </si>
-  <si>
     <t>Measure object centroid</t>
   </si>
   <si>
@@ -595,6 +589,9 @@
   </si>
   <si>
     <t>Preferences</t>
+  </si>
+  <si>
+    <t>Spot detection</t>
   </si>
 </sst>
 </file>
@@ -716,10 +713,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$72</c:f>
+              <c:f>Sheet1!$B$2:$B$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -932,16 +929,19 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$72</c:f>
+              <c:f>Sheet1!$N$2:$N$73</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -1154,6 +1154,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>92.441860465116278</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>93.567251461988306</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1193,10 +1196,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$72</c:f>
+              <c:f>Sheet1!$B$2:$B$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1409,18 +1412,21 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$72</c:f>
+              <c:f>Sheet1!$O$2:$O$73</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
-                  <c:v>13.071139386928861</c:v>
+                  <c:v>12.85551763367463</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -1631,6 +1637,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>93.408968125337651</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>95.856052344601963</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1670,10 +1679,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$72</c:f>
+              <c:f>Sheet1!$B$2:$B$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1886,16 +1895,19 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$72</c:f>
+              <c:f>Sheet1!$P$2:$P$73</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -2108,6 +2120,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>93.023255813953483</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>94.736842105263165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2147,10 +2162,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$72</c:f>
+              <c:f>Sheet1!$B$2:$B$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2363,16 +2378,19 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$72</c:f>
+              <c:f>Sheet1!$Q$2:$Q$73</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2584,6 +2602,9 @@
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="70">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="71">
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
               </c:numCache>
@@ -2624,10 +2645,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$72</c:f>
+              <c:f>Sheet1!$B$2:$B$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2840,16 +2861,19 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$72</c:f>
+              <c:f>Sheet1!$R$2:$R$73</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -3062,6 +3086,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>36.403508771929822</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>37.053571428571431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3318,10 +3345,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$72</c:f>
+              <c:f>Sheet1!$A$2:$A$73</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3534,16 +3561,19 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>44452</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>44453</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$72</c:f>
+              <c:f>Sheet1!$N$2:$N$73</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -3756,6 +3786,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>92.441860465116278</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>93.567251461988306</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3784,10 +3817,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$72</c:f>
+              <c:f>Sheet1!$A$2:$A$73</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4000,18 +4033,21 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>44452</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>44453</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$72</c:f>
+              <c:f>Sheet1!$O$2:$O$73</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
-                  <c:v>13.071139386928861</c:v>
+                  <c:v>12.85551763367463</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -4222,6 +4258,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>93.408968125337651</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>95.856052344601963</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4250,10 +4289,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$72</c:f>
+              <c:f>Sheet1!$A$2:$A$73</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4466,16 +4505,19 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>44452</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>44453</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$72</c:f>
+              <c:f>Sheet1!$P$2:$P$73</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -4688,6 +4730,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>93.023255813953483</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>94.736842105263165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4716,10 +4761,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$72</c:f>
+              <c:f>Sheet1!$A$2:$A$73</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4932,16 +4977,19 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>44452</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>44453</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$72</c:f>
+              <c:f>Sheet1!$Q$2:$Q$73</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -5153,6 +5201,9 @@
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="70">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="71">
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
               </c:numCache>
@@ -5182,10 +5233,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$72</c:f>
+              <c:f>Sheet1!$A$2:$A$73</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -5398,16 +5449,19 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>44452</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>44453</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$72</c:f>
+              <c:f>Sheet1!$R$2:$R$73</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -5620,6 +5674,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>36.403508771929822</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>37.053571428571431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7338,34 +7395,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:R72"/>
+  <dimension ref="A1:R73"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72:L72"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N73" sqref="N73:P73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7412,7 +7469,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44054</v>
       </c>
@@ -7453,7 +7510,7 @@
       </c>
       <c r="O2" s="3">
         <f>100*G2/MAX(G:G)</f>
-        <v>13.071139386928861</v>
+        <v>12.85551763367463</v>
       </c>
       <c r="P2" s="3">
         <f t="shared" ref="P2:P7" si="1">100*H2/D2</f>
@@ -7468,7 +7525,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44055</v>
       </c>
@@ -7524,7 +7581,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44056</v>
       </c>
@@ -7580,7 +7637,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44057</v>
       </c>
@@ -7635,7 +7692,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44058</v>
       </c>
@@ -7690,7 +7747,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44064</v>
       </c>
@@ -7745,7 +7802,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44069</v>
       </c>
@@ -7800,7 +7857,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44070</v>
       </c>
@@ -7855,7 +7912,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44081</v>
       </c>
@@ -7910,7 +7967,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44082</v>
       </c>
@@ -7965,7 +8022,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44083</v>
       </c>
@@ -8020,7 +8077,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44084</v>
       </c>
@@ -8075,7 +8132,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44085</v>
       </c>
@@ -8130,7 +8187,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44089</v>
       </c>
@@ -8185,7 +8242,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44090</v>
       </c>
@@ -8240,7 +8297,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44091</v>
       </c>
@@ -8295,7 +8352,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44097</v>
       </c>
@@ -8350,7 +8407,7 @@
         <v>38.967136150234744</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44098</v>
       </c>
@@ -8405,7 +8462,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44099</v>
       </c>
@@ -8460,7 +8517,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44102</v>
       </c>
@@ -8515,7 +8572,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44103</v>
       </c>
@@ -8570,7 +8627,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44104</v>
       </c>
@@ -8625,7 +8682,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44110</v>
       </c>
@@ -8680,7 +8737,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44113</v>
       </c>
@@ -8735,7 +8792,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44116</v>
       </c>
@@ -8790,7 +8847,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44117</v>
       </c>
@@ -8845,7 +8902,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44118</v>
       </c>
@@ -8900,7 +8957,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44119</v>
       </c>
@@ -8955,7 +9012,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44120</v>
       </c>
@@ -9010,7 +9067,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44123</v>
       </c>
@@ -9065,7 +9122,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44124</v>
       </c>
@@ -9120,7 +9177,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44125</v>
       </c>
@@ -9175,7 +9232,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44126</v>
       </c>
@@ -9230,7 +9287,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44127</v>
       </c>
@@ -9285,7 +9342,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44130</v>
       </c>
@@ -9340,7 +9397,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44131</v>
       </c>
@@ -9395,7 +9452,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44132</v>
       </c>
@@ -9450,7 +9507,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44134</v>
       </c>
@@ -9505,7 +9562,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44137</v>
       </c>
@@ -9560,7 +9617,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44138</v>
       </c>
@@ -9615,7 +9672,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44139</v>
       </c>
@@ -9670,7 +9727,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44140</v>
       </c>
@@ -9725,7 +9782,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44141</v>
       </c>
@@ -9780,7 +9837,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44147</v>
       </c>
@@ -9835,7 +9892,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44148</v>
       </c>
@@ -9890,7 +9947,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44151</v>
       </c>
@@ -9945,7 +10002,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44152</v>
       </c>
@@ -10000,7 +10057,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>44300</v>
       </c>
@@ -10055,7 +10112,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>44301</v>
       </c>
@@ -10110,7 +10167,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>44302</v>
       </c>
@@ -10165,7 +10222,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44306</v>
       </c>
@@ -10220,7 +10277,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>44308</v>
       </c>
@@ -10275,7 +10332,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>44341</v>
       </c>
@@ -10330,7 +10387,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>44342</v>
       </c>
@@ -10385,7 +10442,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>44343</v>
       </c>
@@ -10440,7 +10497,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>44369</v>
       </c>
@@ -10495,7 +10552,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>44370</v>
       </c>
@@ -10550,7 +10607,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>44405</v>
       </c>
@@ -10605,7 +10662,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>44406</v>
       </c>
@@ -10660,7 +10717,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>44413</v>
       </c>
@@ -10715,7 +10772,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>44414</v>
       </c>
@@ -10770,7 +10827,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>44415</v>
       </c>
@@ -10825,7 +10882,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>44419</v>
       </c>
@@ -10880,7 +10937,7 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>44420</v>
       </c>
@@ -10935,7 +10992,7 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>44421</v>
       </c>
@@ -10990,7 +11047,7 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>44427</v>
       </c>
@@ -11045,7 +11102,7 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>44431</v>
       </c>
@@ -11100,7 +11157,7 @@
         <v>36.956521739130437</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>44433</v>
       </c>
@@ -11155,7 +11212,7 @@
         <v>37.387387387387385</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>44441</v>
       </c>
@@ -11210,7 +11267,7 @@
         <v>37.387387387387385</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>44449</v>
       </c>
@@ -11265,7 +11322,7 @@
         <v>36.403508771929822</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>44452</v>
       </c>
@@ -11318,6 +11375,61 @@
       <c r="R72" s="3">
         <f t="shared" ref="R72" si="323">100*L72/K72</f>
         <v>36.403508771929822</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>44453</v>
+      </c>
+      <c r="B73" s="4">
+        <v>71</v>
+      </c>
+      <c r="D73">
+        <v>171</v>
+      </c>
+      <c r="E73">
+        <v>160</v>
+      </c>
+      <c r="F73">
+        <v>1834</v>
+      </c>
+      <c r="G73">
+        <v>1758</v>
+      </c>
+      <c r="H73">
+        <v>162</v>
+      </c>
+      <c r="I73">
+        <v>44</v>
+      </c>
+      <c r="J73">
+        <v>18</v>
+      </c>
+      <c r="K73">
+        <v>224</v>
+      </c>
+      <c r="L73">
+        <v>83</v>
+      </c>
+      <c r="N73" s="3">
+        <f t="shared" ref="N73" si="324">100*E73/D73</f>
+        <v>93.567251461988306</v>
+      </c>
+      <c r="O73" s="3">
+        <f t="shared" ref="O73" si="325">100*G73/F73</f>
+        <v>95.856052344601963</v>
+      </c>
+      <c r="P73" s="3">
+        <f t="shared" ref="P73" si="326">100*H73/D73</f>
+        <v>94.736842105263165</v>
+      </c>
+      <c r="Q73" s="3">
+        <f t="shared" ref="Q73" si="327">100*J73/I73</f>
+        <v>40.909090909090907</v>
+      </c>
+      <c r="R73" s="3">
+        <f t="shared" ref="R73" si="328">100*L73/K73</f>
+        <v>37.053571428571431</v>
       </c>
     </row>
   </sheetData>
@@ -11332,47 +11444,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60F2A9E-CB35-4818-B2AA-21716033EEE9}">
   <dimension ref="A1:G172"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1">
         <v>100</v>
       </c>
-      <c r="B1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>21</v>
-      </c>
-      <c r="E1" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
       <c r="G1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -11381,30 +11493,30 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -11416,9 +11528,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -11439,9 +11551,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -11459,12 +11571,12 @@
         <v>100</v>
       </c>
       <c r="G5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -11482,21 +11594,21 @@
         <v>100</v>
       </c>
       <c r="G6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="B7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5">
-        <v>0</v>
+        <v>0.1429</v>
       </c>
       <c r="D7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
@@ -11508,9 +11620,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -11519,7 +11631,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
@@ -11528,21 +11640,21 @@
         <v>100</v>
       </c>
       <c r="G8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
       <c r="C9" s="5">
-        <v>0.1429</v>
+        <v>0.44440000000000002</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="5">
         <v>1</v>
@@ -11551,21 +11663,21 @@
         <v>100</v>
       </c>
       <c r="G9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>121</v>
+        <v>15</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="5">
-        <v>0.1429</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
@@ -11577,18 +11689,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>145</v>
+        <v>16</v>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E11" s="5">
         <v>1</v>
@@ -11600,18 +11712,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>179</v>
+        <v>33</v>
       </c>
       <c r="B12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="5">
-        <v>0.44440000000000002</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E12" s="5">
         <v>1</v>
@@ -11623,9 +11735,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -11637,7 +11749,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>100</v>
@@ -11646,9 +11758,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -11660,7 +11772,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>100</v>
@@ -11669,9 +11781,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -11692,9 +11804,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -11715,9 +11827,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -11738,9 +11850,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>29</v>
+        <v>166</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -11752,7 +11864,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>100</v>
@@ -11761,9 +11873,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -11784,9 +11896,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -11807,9 +11919,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -11821,7 +11933,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
         <v>100</v>
@@ -11830,9 +11942,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>168</v>
+        <v>45</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -11853,9 +11965,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -11876,9 +11988,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -11899,9 +12011,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -11922,9 +12034,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
@@ -11945,9 +12057,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
@@ -11968,9 +12080,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
@@ -11991,9 +12103,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -12014,9 +12126,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
@@ -12037,9 +12149,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -12060,9 +12172,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -12080,12 +12192,12 @@
         <v>100</v>
       </c>
       <c r="G32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
@@ -12106,9 +12218,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
@@ -12129,9 +12241,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B35" t="b">
         <v>1</v>
@@ -12152,9 +12264,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="B36" t="b">
         <v>1</v>
@@ -12172,12 +12284,12 @@
         <v>100</v>
       </c>
       <c r="G36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -12198,12 +12310,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38" s="5">
         <v>1</v>
@@ -12221,9 +12333,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -12244,9 +12356,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>180</v>
+        <v>41</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -12267,9 +12379,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B41" t="b">
         <v>1</v>
@@ -12290,12 +12402,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" s="5">
         <v>1</v>
@@ -12313,9 +12425,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B43" t="b">
         <v>1</v>
@@ -12336,9 +12448,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B44" t="b">
         <v>1</v>
@@ -12359,9 +12471,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B45" t="b">
         <v>1</v>
@@ -12382,9 +12494,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B46" t="b">
         <v>1</v>
@@ -12396,7 +12508,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46">
         <v>100</v>
@@ -12405,9 +12517,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B47" t="b">
         <v>1</v>
@@ -12425,12 +12537,12 @@
         <v>100</v>
       </c>
       <c r="G47" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B48" t="b">
         <v>1</v>
@@ -12451,9 +12563,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B49" t="b">
         <v>1</v>
@@ -12474,9 +12586,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B50" t="b">
         <v>1</v>
@@ -12488,7 +12600,7 @@
         <v>0</v>
       </c>
       <c r="E50" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50">
         <v>100</v>
@@ -12497,9 +12609,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="B51" t="b">
         <v>1</v>
@@ -12517,12 +12629,12 @@
         <v>100</v>
       </c>
       <c r="G51" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B52" t="b">
         <v>1</v>
@@ -12543,9 +12655,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B53" t="b">
         <v>1</v>
@@ -12566,9 +12678,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B54" t="b">
         <v>1</v>
@@ -12589,9 +12701,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B55" t="b">
         <v>1</v>
@@ -12612,9 +12724,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B56" t="b">
         <v>1</v>
@@ -12632,12 +12744,12 @@
         <v>100</v>
       </c>
       <c r="G56" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="B57" t="b">
         <v>1</v>
@@ -12658,9 +12770,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B58" t="b">
         <v>1</v>
@@ -12681,9 +12793,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B59" t="b">
         <v>1</v>
@@ -12701,12 +12813,12 @@
         <v>100</v>
       </c>
       <c r="G59" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>24</v>
+        <v>167</v>
       </c>
       <c r="B60" t="b">
         <v>1</v>
@@ -12724,12 +12836,12 @@
         <v>100</v>
       </c>
       <c r="G60" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>25</v>
+        <v>174</v>
       </c>
       <c r="B61" t="b">
         <v>1</v>
@@ -12750,9 +12862,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>68</v>
+        <v>168</v>
       </c>
       <c r="B62" t="b">
         <v>1</v>
@@ -12773,9 +12885,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>69</v>
+        <v>169</v>
       </c>
       <c r="B63" t="b">
         <v>1</v>
@@ -12793,12 +12905,12 @@
         <v>100</v>
       </c>
       <c r="G63" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B64" t="b">
         <v>1</v>
@@ -12819,11 +12931,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B65" s="5" t="b">
+        <v>171</v>
+      </c>
+      <c r="B65" t="b">
         <v>1</v>
       </c>
       <c r="C65" s="5">
@@ -12842,9 +12954,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B66" t="b">
         <v>1</v>
@@ -12865,9 +12977,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>171</v>
+        <v>70</v>
       </c>
       <c r="B67" t="b">
         <v>1</v>
@@ -12888,9 +13000,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>172</v>
+        <v>71</v>
       </c>
       <c r="B68" t="b">
         <v>1</v>
@@ -12911,9 +13023,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>173</v>
+        <v>72</v>
       </c>
       <c r="B69" t="b">
         <v>1</v>
@@ -12934,9 +13046,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>174</v>
+        <v>73</v>
       </c>
       <c r="B70" t="b">
         <v>1</v>
@@ -12957,9 +13069,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B71" t="b">
         <v>1</v>
@@ -12980,9 +13092,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="B72" t="b">
         <v>1</v>
@@ -13003,9 +13115,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B73" t="b">
         <v>1</v>
@@ -13026,9 +13138,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B74" t="b">
         <v>1</v>
@@ -13046,12 +13158,12 @@
         <v>100</v>
       </c>
       <c r="G74" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B75" t="b">
         <v>1</v>
@@ -13072,9 +13184,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="B76" t="b">
         <v>1</v>
@@ -13095,9 +13207,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>76</v>
+        <v>173</v>
       </c>
       <c r="B77" t="b">
         <v>1</v>
@@ -13118,9 +13230,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B78" t="b">
         <v>1</v>
@@ -13138,12 +13250,12 @@
         <v>100</v>
       </c>
       <c r="G78" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="B79" t="b">
         <v>1</v>
@@ -13164,9 +13276,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B80" t="b">
         <v>1</v>
@@ -13181,15 +13293,15 @@
         <v>1</v>
       </c>
       <c r="F80">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G80" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>175</v>
+        <v>81</v>
       </c>
       <c r="B81" t="b">
         <v>1</v>
@@ -13210,9 +13322,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B82" t="b">
         <v>1</v>
@@ -13227,130 +13339,130 @@
         <v>1</v>
       </c>
       <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" t="b">
+        <v>1</v>
+      </c>
+      <c r="C83" s="5">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83" s="5">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" t="b">
+        <v>1</v>
+      </c>
+      <c r="C84" s="5">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84" s="5">
+        <v>1</v>
+      </c>
+      <c r="F84">
         <v>100</v>
       </c>
-      <c r="G82" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B83" t="b">
-        <v>1</v>
-      </c>
-      <c r="C83" s="5">
-        <v>1</v>
-      </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
-      <c r="E83" s="5">
-        <v>1</v>
-      </c>
-      <c r="F83">
+      <c r="G84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" t="b">
+        <v>1</v>
+      </c>
+      <c r="C85" s="5">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85" s="5">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" t="b">
+        <v>1</v>
+      </c>
+      <c r="C86" s="5">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86" s="5">
+        <v>1</v>
+      </c>
+      <c r="F86">
         <v>100</v>
       </c>
-      <c r="G83" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A84" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B84" t="b">
-        <v>1</v>
-      </c>
-      <c r="C84" s="5">
-        <v>1</v>
-      </c>
-      <c r="D84">
-        <v>0</v>
-      </c>
-      <c r="E84" s="5">
-        <v>1</v>
-      </c>
-      <c r="F84">
-        <v>0</v>
-      </c>
-      <c r="G84" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B85" t="b">
-        <v>1</v>
-      </c>
-      <c r="C85" s="5">
-        <v>1</v>
-      </c>
-      <c r="D85">
-        <v>0</v>
-      </c>
-      <c r="E85" s="5">
-        <v>1</v>
-      </c>
-      <c r="F85">
+      <c r="G86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" t="b">
+        <v>1</v>
+      </c>
+      <c r="C87" s="5">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87" s="5">
+        <v>1</v>
+      </c>
+      <c r="F87">
         <v>100</v>
       </c>
-      <c r="G85" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B86" t="b">
-        <v>1</v>
-      </c>
-      <c r="C86" s="5">
-        <v>1</v>
-      </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
-      <c r="E86" s="5">
-        <v>1</v>
-      </c>
-      <c r="F86">
-        <v>0</v>
-      </c>
-      <c r="G86" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B87" t="b">
-        <v>1</v>
-      </c>
-      <c r="C87" s="5">
-        <v>1</v>
-      </c>
-      <c r="D87">
-        <v>0</v>
-      </c>
-      <c r="E87" s="5">
-        <v>1</v>
-      </c>
-      <c r="F87">
-        <v>0</v>
-      </c>
       <c r="G87" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B88" t="b">
         <v>1</v>
@@ -13371,9 +13483,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B89" t="b">
         <v>1</v>
@@ -13394,9 +13506,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B90" t="b">
         <v>1</v>
@@ -13411,15 +13523,15 @@
         <v>1</v>
       </c>
       <c r="F90">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G90" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B91" t="b">
         <v>1</v>
@@ -13440,9 +13552,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B92" t="b">
         <v>1</v>
@@ -13463,9 +13575,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B93" t="b">
         <v>1</v>
@@ -13480,15 +13592,15 @@
         <v>1</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G93" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B94" t="b">
         <v>1</v>
@@ -13509,9 +13621,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B95" t="b">
         <v>1</v>
@@ -13532,9 +13644,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B96" t="b">
         <v>1</v>
@@ -13555,9 +13667,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B97" t="b">
         <v>1</v>
@@ -13572,15 +13684,15 @@
         <v>1</v>
       </c>
       <c r="F97">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G97" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B98" t="b">
         <v>1</v>
@@ -13601,9 +13713,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B99" t="b">
         <v>1</v>
@@ -13624,9 +13736,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B100" t="b">
         <v>1</v>
@@ -13647,12 +13759,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B101" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" s="5">
         <v>1</v>
@@ -13670,9 +13782,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B102" t="b">
         <v>1</v>
@@ -13687,15 +13799,15 @@
         <v>1</v>
       </c>
       <c r="F102">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G102" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B103" t="b">
         <v>1</v>
@@ -13710,15 +13822,15 @@
         <v>1</v>
       </c>
       <c r="F103">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G103" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B104" t="b">
         <v>1</v>
@@ -13739,9 +13851,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B105" t="b">
         <v>1</v>
@@ -13756,130 +13868,130 @@
         <v>1</v>
       </c>
       <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" t="b">
+        <v>1</v>
+      </c>
+      <c r="C106" s="5">
+        <v>1</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106" s="5">
+        <v>1</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="G106" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107" t="b">
+        <v>1</v>
+      </c>
+      <c r="C107" s="5">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107" s="5">
+        <v>1</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B108" t="b">
+        <v>1</v>
+      </c>
+      <c r="C108" s="5">
+        <v>1</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108" s="5">
+        <v>1</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B109" t="b">
+        <v>0</v>
+      </c>
+      <c r="C109" s="5">
+        <v>1</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109" s="5">
+        <v>1</v>
+      </c>
+      <c r="F109">
         <v>100</v>
       </c>
-      <c r="G105" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B106" t="b">
-        <v>1</v>
-      </c>
-      <c r="C106" s="5">
-        <v>1</v>
-      </c>
-      <c r="D106">
-        <v>0</v>
-      </c>
-      <c r="E106" s="5">
-        <v>1</v>
-      </c>
-      <c r="F106">
-        <v>0</v>
-      </c>
-      <c r="G106" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A107" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B107" t="b">
-        <v>1</v>
-      </c>
-      <c r="C107" s="5">
-        <v>1</v>
-      </c>
-      <c r="D107">
-        <v>0</v>
-      </c>
-      <c r="E107" s="5">
-        <v>1</v>
-      </c>
-      <c r="F107">
+      <c r="G109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B110" t="b">
+        <v>1</v>
+      </c>
+      <c r="C110" s="5">
+        <v>1</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110" s="5">
+        <v>1</v>
+      </c>
+      <c r="F110">
         <v>100</v>
       </c>
-      <c r="G107" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A108" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B108" t="b">
-        <v>1</v>
-      </c>
-      <c r="C108" s="5">
-        <v>1</v>
-      </c>
-      <c r="D108">
-        <v>0</v>
-      </c>
-      <c r="E108" s="5">
-        <v>1</v>
-      </c>
-      <c r="F108">
-        <v>0</v>
-      </c>
-      <c r="G108" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A109" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B109" t="b">
-        <v>1</v>
-      </c>
-      <c r="C109" s="5">
-        <v>1</v>
-      </c>
-      <c r="D109">
-        <v>0</v>
-      </c>
-      <c r="E109" s="5">
-        <v>1</v>
-      </c>
-      <c r="F109">
-        <v>0</v>
-      </c>
-      <c r="G109" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A110" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B110" t="b">
-        <v>1</v>
-      </c>
-      <c r="C110" s="5">
-        <v>1</v>
-      </c>
-      <c r="D110">
-        <v>0</v>
-      </c>
-      <c r="E110" s="5">
-        <v>1</v>
-      </c>
-      <c r="F110">
-        <v>0</v>
-      </c>
       <c r="G110" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>177</v>
+        <v>111</v>
       </c>
       <c r="B111" t="b">
         <v>1</v>
@@ -13894,18 +14006,18 @@
         <v>1</v>
       </c>
       <c r="F111">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G111" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>181</v>
+        <v>112</v>
       </c>
       <c r="B112" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C112" s="5">
         <v>1</v>
@@ -13923,9 +14035,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B113" t="b">
         <v>1</v>
@@ -13946,9 +14058,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B114" t="b">
         <v>1</v>
@@ -13969,9 +14081,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B115" t="b">
         <v>1</v>
@@ -13992,9 +14104,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B116" t="b">
         <v>1</v>
@@ -14009,107 +14121,107 @@
         <v>1</v>
       </c>
       <c r="F116">
+        <v>22.22</v>
+      </c>
+      <c r="G116" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B117" t="b">
+        <v>1</v>
+      </c>
+      <c r="C117" s="5">
+        <v>1</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117" s="5">
+        <v>1</v>
+      </c>
+      <c r="F117">
+        <v>0</v>
+      </c>
+      <c r="G117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B118" t="b">
+        <v>1</v>
+      </c>
+      <c r="C118" s="5">
+        <v>1</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+      <c r="E118" s="5">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <v>22.22</v>
+      </c>
+      <c r="G118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B119" t="b">
+        <v>1</v>
+      </c>
+      <c r="C119" s="5">
+        <v>1</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119" s="5">
+        <v>1</v>
+      </c>
+      <c r="F119">
         <v>100</v>
       </c>
-      <c r="G116" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A117" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B117" t="b">
-        <v>1</v>
-      </c>
-      <c r="C117" s="5">
-        <v>1</v>
-      </c>
-      <c r="D117">
-        <v>0</v>
-      </c>
-      <c r="E117" s="5">
-        <v>1</v>
-      </c>
-      <c r="F117">
+      <c r="G119" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B120" t="b">
+        <v>1</v>
+      </c>
+      <c r="C120" s="5">
+        <v>1</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+      <c r="E120" s="5">
+        <v>1</v>
+      </c>
+      <c r="F120">
         <v>100</v>
       </c>
-      <c r="G117" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A118" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B118" t="b">
-        <v>1</v>
-      </c>
-      <c r="C118" s="5">
-        <v>1</v>
-      </c>
-      <c r="D118">
-        <v>0</v>
-      </c>
-      <c r="E118" s="5">
-        <v>1</v>
-      </c>
-      <c r="F118">
-        <v>100</v>
-      </c>
-      <c r="G118" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A119" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B119" t="b">
-        <v>1</v>
-      </c>
-      <c r="C119" s="5">
-        <v>1</v>
-      </c>
-      <c r="D119">
-        <v>0</v>
-      </c>
-      <c r="E119" s="5">
-        <v>1</v>
-      </c>
-      <c r="F119">
-        <v>36.36</v>
-      </c>
-      <c r="G119" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A120" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B120" t="b">
-        <v>1</v>
-      </c>
-      <c r="C120" s="5">
-        <v>1</v>
-      </c>
-      <c r="D120">
-        <v>0</v>
-      </c>
-      <c r="E120" s="5">
-        <v>1</v>
-      </c>
-      <c r="F120">
-        <v>0</v>
-      </c>
       <c r="G120" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B121" t="b">
         <v>1</v>
@@ -14130,9 +14242,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B122" t="b">
         <v>1</v>
@@ -14153,7 +14265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>122</v>
       </c>
@@ -14176,9 +14288,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B124" t="b">
         <v>1</v>
@@ -14199,9 +14311,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B125" t="b">
         <v>1</v>
@@ -14222,9 +14334,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B126" t="b">
         <v>1</v>
@@ -14242,12 +14354,12 @@
         <v>100</v>
       </c>
       <c r="G126" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B127" t="b">
         <v>1</v>
@@ -14265,12 +14377,12 @@
         <v>100</v>
       </c>
       <c r="G127" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>138</v>
+        <v>180</v>
       </c>
       <c r="B128" t="b">
         <v>1</v>
@@ -14291,9 +14403,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>182</v>
+        <v>124</v>
       </c>
       <c r="B129" t="b">
         <v>1</v>
@@ -14314,9 +14426,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B130" t="b">
         <v>1</v>
@@ -14337,9 +14449,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B131" t="b">
         <v>1</v>
@@ -14360,9 +14472,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B132" t="b">
         <v>1</v>
@@ -14383,9 +14495,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>129</v>
+        <v>21</v>
       </c>
       <c r="B133" t="b">
         <v>1</v>
@@ -14406,9 +14518,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="B134" t="b">
         <v>1</v>
@@ -14429,9 +14541,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B135" t="b">
         <v>1</v>
@@ -14452,9 +14564,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B136" t="b">
         <v>1</v>
@@ -14475,9 +14587,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B137" t="b">
         <v>1</v>
@@ -14498,7 +14610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>133</v>
       </c>
@@ -14521,9 +14633,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B139" t="b">
         <v>1</v>
@@ -14544,9 +14656,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B140" t="b">
         <v>1</v>
@@ -14567,9 +14679,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B141" t="b">
         <v>1</v>
@@ -14590,9 +14702,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>140</v>
+        <v>26</v>
       </c>
       <c r="B142" t="b">
         <v>1</v>
@@ -14613,9 +14725,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>26</v>
+        <v>139</v>
       </c>
       <c r="B143" t="b">
         <v>1</v>
@@ -14636,7 +14748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>141</v>
       </c>
@@ -14653,41 +14765,41 @@
         <v>1</v>
       </c>
       <c r="F144">
+        <v>0</v>
+      </c>
+      <c r="G144" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B145" t="b">
+        <v>1</v>
+      </c>
+      <c r="C145" s="5">
+        <v>1</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+      <c r="E145" s="5">
+        <v>1</v>
+      </c>
+      <c r="F145">
         <v>100</v>
       </c>
-      <c r="G144" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A145" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B145" t="b">
-        <v>1</v>
-      </c>
-      <c r="C145" s="5">
-        <v>1</v>
-      </c>
-      <c r="D145">
-        <v>0</v>
-      </c>
-      <c r="E145" s="5">
-        <v>1</v>
-      </c>
-      <c r="F145">
-        <v>0</v>
-      </c>
       <c r="G145" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="B146" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C146" s="5">
         <v>1</v>
@@ -14705,12 +14817,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B147" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C147" s="5">
         <v>1</v>
@@ -14728,9 +14840,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B148" t="b">
         <v>1</v>
@@ -14751,9 +14863,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B149" t="b">
         <v>1</v>
@@ -14771,12 +14883,12 @@
         <v>100</v>
       </c>
       <c r="G149" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B150" t="b">
         <v>1</v>
@@ -14794,12 +14906,12 @@
         <v>100</v>
       </c>
       <c r="G150" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="B151" t="b">
         <v>1</v>
@@ -14820,9 +14932,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B152" t="b">
         <v>1</v>
@@ -14843,9 +14955,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B153" t="b">
         <v>1</v>
@@ -14866,9 +14978,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B154" t="b">
         <v>1</v>
@@ -14889,9 +15001,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B155" t="b">
         <v>1</v>
@@ -14912,9 +15024,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B156" t="b">
         <v>1</v>
@@ -14935,9 +15047,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B157" t="b">
         <v>1</v>
@@ -14958,9 +15070,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B158" t="b">
         <v>1</v>
@@ -14981,9 +15093,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B159" t="b">
         <v>1</v>
@@ -15004,9 +15116,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B160" t="b">
         <v>1</v>
@@ -15027,9 +15139,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B161" t="b">
         <v>1</v>
@@ -15050,9 +15162,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>157</v>
+        <v>18</v>
       </c>
       <c r="B162" t="b">
         <v>1</v>
@@ -15070,12 +15182,12 @@
         <v>100</v>
       </c>
       <c r="G162" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>18</v>
+        <v>156</v>
       </c>
       <c r="B163" t="b">
         <v>1</v>
@@ -15093,12 +15205,12 @@
         <v>100</v>
       </c>
       <c r="G163" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B164" t="b">
         <v>1</v>
@@ -15119,9 +15231,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B165" t="b">
         <v>1</v>
@@ -15142,9 +15254,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B166" t="b">
         <v>1</v>
@@ -15165,9 +15277,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B167" t="b">
         <v>1</v>
@@ -15188,9 +15300,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>167</v>
+        <v>22</v>
       </c>
       <c r="B168" t="b">
         <v>1</v>
@@ -15211,9 +15323,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>22</v>
+        <v>182</v>
       </c>
       <c r="B169" t="b">
         <v>1</v>
@@ -15234,9 +15346,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B170" t="b">
         <v>1</v>
@@ -15257,9 +15369,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B171" t="b">
         <v>1</v>
@@ -15280,32 +15392,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A172" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="B172" t="b">
-        <v>1</v>
-      </c>
-      <c r="C172" s="5">
-        <v>1</v>
-      </c>
-      <c r="D172">
-        <v>0</v>
-      </c>
-      <c r="E172" s="5">
-        <v>1</v>
-      </c>
-      <c r="F172">
-        <v>100</v>
-      </c>
-      <c r="G172" t="b">
-        <v>1</v>
-      </c>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G172">
-    <sortCondition descending="1" ref="D4:D172"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G171">
+    <sortCondition descending="1" ref="D2:D171"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Module list icons orange when inaccessible
If using workflow handling, inaccessible modules will be shown in orange
to distinguish them from erroring modules.
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stephen\Programming\Java Projects\mia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D178D4B1-1961-4843-B6F0-112B55FAB5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88324A9E-3781-4A69-9517-222598C699F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7397,7 +7397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
   <dimension ref="A1:R73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N73" sqref="N73:P73"/>
     </sheetView>
   </sheetViews>
@@ -11444,8 +11444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60F2A9E-CB35-4818-B2AA-21716033EEE9}">
   <dimension ref="A1:G172"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated description coverage document
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Java Projects\MIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stephen\Programming\Java Projects\mia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0944FAD3-DCED-4021-9A15-B9AF2AB984F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB88BC39-79A1-4FA9-BAE1-0EAFC4CD03CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="1" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28095" windowHeight="16440" activeTab="1" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
   <si>
     <t>Date</t>
   </si>
@@ -360,9 +360,6 @@
     <t>Measure track motion</t>
   </si>
   <si>
-    <t>Active contour-based detection</t>
-  </si>
-  <si>
     <t>Extract object edges</t>
   </si>
   <si>
@@ -588,10 +585,10 @@
     <t>Workflow handling</t>
   </si>
   <si>
-    <t>Preferences</t>
-  </si>
-  <si>
     <t>Spot detection</t>
+  </si>
+  <si>
+    <t>Fit active contours</t>
   </si>
 </sst>
 </file>
@@ -713,10 +710,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$73</c:f>
+              <c:f>Sheet1!$B$2:$B$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -932,16 +929,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$73</c:f>
+              <c:f>Sheet1!$N$2:$N$74</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -1157,6 +1157,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>93.567251461988306</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>95.294117647058826</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1196,10 +1199,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$73</c:f>
+              <c:f>Sheet1!$B$2:$B$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1415,18 +1418,21 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$73</c:f>
+              <c:f>Sheet1!$O$2:$O$74</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
-                  <c:v>12.85551763367463</c:v>
+                  <c:v>12.661064425770308</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -1640,6 +1646,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>95.856052344601963</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>97.43449781659389</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1679,10 +1688,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$73</c:f>
+              <c:f>Sheet1!$B$2:$B$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1898,16 +1907,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$73</c:f>
+              <c:f>Sheet1!$P$2:$P$74</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -2123,6 +2135,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>94.736842105263165</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>96.470588235294116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2162,10 +2177,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$73</c:f>
+              <c:f>Sheet1!$B$2:$B$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2381,16 +2396,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$73</c:f>
+              <c:f>Sheet1!$Q$2:$Q$74</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2605,6 +2623,9 @@
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="71">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="72">
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
               </c:numCache>
@@ -2645,10 +2666,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$73</c:f>
+              <c:f>Sheet1!$B$2:$B$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2864,16 +2885,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$73</c:f>
+              <c:f>Sheet1!$R$2:$R$74</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -3088,6 +3112,9 @@
                   <c:v>36.403508771929822</c:v>
                 </c:pt>
                 <c:pt idx="71">
+                  <c:v>37.053571428571431</c:v>
+                </c:pt>
+                <c:pt idx="72">
                   <c:v>37.053571428571431</c:v>
                 </c:pt>
               </c:numCache>
@@ -3324,7 +3351,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.9962033397686165E-2"/>
+          <c:y val="2.3206751054852322E-2"/>
+          <c:w val="0.89896897099610062"/>
+          <c:h val="0.8795920130236885"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -3345,10 +3382,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$73</c:f>
+              <c:f>Sheet1!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3564,16 +3601,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>44453</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>44466</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$73</c:f>
+              <c:f>Sheet1!$N$2:$N$74</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -3789,6 +3829,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>93.567251461988306</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>95.294117647058826</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3817,10 +3860,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$73</c:f>
+              <c:f>Sheet1!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4036,18 +4079,21 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>44453</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>44466</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$73</c:f>
+              <c:f>Sheet1!$O$2:$O$74</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
-                  <c:v>12.85551763367463</c:v>
+                  <c:v>12.661064425770308</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -4261,6 +4307,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>95.856052344601963</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>97.43449781659389</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4289,10 +4338,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$73</c:f>
+              <c:f>Sheet1!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4508,16 +4557,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>44453</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>44466</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$73</c:f>
+              <c:f>Sheet1!$P$2:$P$74</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -4733,6 +4785,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>94.736842105263165</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>96.470588235294116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4761,10 +4816,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$73</c:f>
+              <c:f>Sheet1!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4980,16 +5035,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>44453</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>44466</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$73</c:f>
+              <c:f>Sheet1!$Q$2:$Q$74</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -5204,6 +5262,9 @@
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="71">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="72">
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
               </c:numCache>
@@ -5233,10 +5294,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$73</c:f>
+              <c:f>Sheet1!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -5452,16 +5513,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>44453</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>44466</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$73</c:f>
+              <c:f>Sheet1!$R$2:$R$74</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -5676,6 +5740,9 @@
                   <c:v>36.403508771929822</c:v>
                 </c:pt>
                 <c:pt idx="71">
+                  <c:v>37.053571428571431</c:v>
+                </c:pt>
+                <c:pt idx="72">
                   <c:v>37.053571428571431</c:v>
                 </c:pt>
               </c:numCache>
@@ -7395,34 +7462,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:R73"/>
+  <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N73" sqref="N73:P73"/>
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7469,7 +7536,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44054</v>
       </c>
@@ -7510,7 +7577,7 @@
       </c>
       <c r="O2" s="3">
         <f>100*G2/MAX(G:G)</f>
-        <v>12.85551763367463</v>
+        <v>12.661064425770308</v>
       </c>
       <c r="P2" s="3">
         <f t="shared" ref="P2:P7" si="1">100*H2/D2</f>
@@ -7525,7 +7592,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44055</v>
       </c>
@@ -7581,7 +7648,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44056</v>
       </c>
@@ -7637,7 +7704,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44057</v>
       </c>
@@ -7692,7 +7759,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44058</v>
       </c>
@@ -7747,7 +7814,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44064</v>
       </c>
@@ -7802,7 +7869,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44069</v>
       </c>
@@ -7857,7 +7924,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44070</v>
       </c>
@@ -7912,7 +7979,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44081</v>
       </c>
@@ -7967,7 +8034,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44082</v>
       </c>
@@ -8022,7 +8089,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44083</v>
       </c>
@@ -8077,7 +8144,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44084</v>
       </c>
@@ -8132,7 +8199,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44085</v>
       </c>
@@ -8187,7 +8254,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44089</v>
       </c>
@@ -8242,7 +8309,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44090</v>
       </c>
@@ -8297,7 +8364,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44091</v>
       </c>
@@ -8352,7 +8419,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44097</v>
       </c>
@@ -8407,7 +8474,7 @@
         <v>38.967136150234744</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44098</v>
       </c>
@@ -8462,7 +8529,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44099</v>
       </c>
@@ -8517,7 +8584,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44102</v>
       </c>
@@ -8572,7 +8639,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44103</v>
       </c>
@@ -8627,7 +8694,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44104</v>
       </c>
@@ -8682,7 +8749,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44110</v>
       </c>
@@ -8737,7 +8804,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44113</v>
       </c>
@@ -8792,7 +8859,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44116</v>
       </c>
@@ -8847,7 +8914,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44117</v>
       </c>
@@ -8902,7 +8969,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44118</v>
       </c>
@@ -8957,7 +9024,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44119</v>
       </c>
@@ -9012,7 +9079,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44120</v>
       </c>
@@ -9067,7 +9134,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44123</v>
       </c>
@@ -9122,7 +9189,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44124</v>
       </c>
@@ -9177,7 +9244,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44125</v>
       </c>
@@ -9232,7 +9299,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44126</v>
       </c>
@@ -9287,7 +9354,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44127</v>
       </c>
@@ -9342,7 +9409,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44130</v>
       </c>
@@ -9397,7 +9464,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44131</v>
       </c>
@@ -9452,7 +9519,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44132</v>
       </c>
@@ -9507,7 +9574,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44134</v>
       </c>
@@ -9562,7 +9629,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44137</v>
       </c>
@@ -9617,7 +9684,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44138</v>
       </c>
@@ -9672,7 +9739,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44139</v>
       </c>
@@ -9727,7 +9794,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44140</v>
       </c>
@@ -9782,7 +9849,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44141</v>
       </c>
@@ -9837,7 +9904,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44147</v>
       </c>
@@ -9892,7 +9959,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44148</v>
       </c>
@@ -9947,7 +10014,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44151</v>
       </c>
@@ -10002,7 +10069,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44152</v>
       </c>
@@ -10057,7 +10124,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>44300</v>
       </c>
@@ -10112,7 +10179,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>44301</v>
       </c>
@@ -10167,7 +10234,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>44302</v>
       </c>
@@ -10222,7 +10289,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44306</v>
       </c>
@@ -10277,7 +10344,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>44308</v>
       </c>
@@ -10332,7 +10399,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>44341</v>
       </c>
@@ -10387,7 +10454,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>44342</v>
       </c>
@@ -10442,7 +10509,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>44343</v>
       </c>
@@ -10497,7 +10564,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>44369</v>
       </c>
@@ -10552,7 +10619,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>44370</v>
       </c>
@@ -10607,7 +10674,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>44405</v>
       </c>
@@ -10662,7 +10729,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>44406</v>
       </c>
@@ -10717,7 +10784,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>44413</v>
       </c>
@@ -10772,7 +10839,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>44414</v>
       </c>
@@ -10827,7 +10894,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>44415</v>
       </c>
@@ -10882,7 +10949,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>44419</v>
       </c>
@@ -10937,7 +11004,7 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>44420</v>
       </c>
@@ -10992,7 +11059,7 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>44421</v>
       </c>
@@ -11047,7 +11114,7 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>44427</v>
       </c>
@@ -11102,7 +11169,7 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>44431</v>
       </c>
@@ -11157,7 +11224,7 @@
         <v>36.956521739130437</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>44433</v>
       </c>
@@ -11212,7 +11279,7 @@
         <v>37.387387387387385</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>44441</v>
       </c>
@@ -11267,7 +11334,7 @@
         <v>37.387387387387385</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>44449</v>
       </c>
@@ -11322,7 +11389,7 @@
         <v>36.403508771929822</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>44452</v>
       </c>
@@ -11377,7 +11444,7 @@
         <v>36.403508771929822</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>44453</v>
       </c>
@@ -11429,6 +11496,61 @@
       </c>
       <c r="R73" s="3">
         <f t="shared" ref="R73" si="328">100*L73/K73</f>
+        <v>37.053571428571431</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>44466</v>
+      </c>
+      <c r="B74" s="4">
+        <v>72</v>
+      </c>
+      <c r="D74">
+        <v>170</v>
+      </c>
+      <c r="E74">
+        <v>162</v>
+      </c>
+      <c r="F74">
+        <v>1832</v>
+      </c>
+      <c r="G74">
+        <v>1785</v>
+      </c>
+      <c r="H74">
+        <v>164</v>
+      </c>
+      <c r="I74">
+        <v>44</v>
+      </c>
+      <c r="J74">
+        <v>18</v>
+      </c>
+      <c r="K74">
+        <v>224</v>
+      </c>
+      <c r="L74">
+        <v>83</v>
+      </c>
+      <c r="N74" s="3">
+        <f t="shared" ref="N74" si="329">100*E74/D74</f>
+        <v>95.294117647058826</v>
+      </c>
+      <c r="O74" s="3">
+        <f t="shared" ref="O74" si="330">100*G74/F74</f>
+        <v>97.43449781659389</v>
+      </c>
+      <c r="P74" s="3">
+        <f t="shared" ref="P74" si="331">100*H74/D74</f>
+        <v>96.470588235294116</v>
+      </c>
+      <c r="Q74" s="3">
+        <f t="shared" ref="Q74" si="332">100*J74/I74</f>
+        <v>40.909090909090907</v>
+      </c>
+      <c r="R74" s="3">
+        <f t="shared" ref="R74" si="333">100*L74/K74</f>
         <v>37.053571428571431</v>
       </c>
     </row>
@@ -11442,24 +11564,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60F2A9E-CB35-4818-B2AA-21716033EEE9}">
-  <dimension ref="A1:G172"/>
+  <dimension ref="A1:G171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>69</v>
       </c>
@@ -11482,7 +11604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>104</v>
       </c>
@@ -11505,9 +11627,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -11528,9 +11650,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -11551,9 +11673,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -11574,9 +11696,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -11597,9 +11719,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -11617,12 +11739,12 @@
         <v>100</v>
       </c>
       <c r="G7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>109</v>
+        <v>16</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -11643,9 +11765,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>119</v>
+        <v>33</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -11666,9 +11788,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -11680,7 +11802,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>100</v>
@@ -11689,9 +11811,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -11703,7 +11825,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>100</v>
@@ -11712,9 +11834,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -11735,9 +11857,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -11749,7 +11871,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>100</v>
@@ -11758,9 +11880,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -11781,9 +11903,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>30</v>
+        <v>165</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -11804,9 +11926,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -11827,9 +11949,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -11841,7 +11963,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>100</v>
@@ -11850,9 +11972,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>166</v>
+        <v>44</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -11873,9 +11995,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -11896,9 +12018,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -11919,9 +12041,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -11942,9 +12064,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -11965,9 +12087,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -11988,9 +12110,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -12011,9 +12133,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -12034,9 +12156,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
@@ -12057,9 +12179,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
@@ -12080,9 +12202,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
@@ -12103,9 +12225,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -12123,12 +12245,12 @@
         <v>100</v>
       </c>
       <c r="G29" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
@@ -12149,9 +12271,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -12172,9 +12294,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -12192,12 +12314,12 @@
         <v>100</v>
       </c>
       <c r="G32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>35</v>
+        <v>177</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
@@ -12218,9 +12340,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
@@ -12241,12 +12363,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" s="5">
         <v>1</v>
@@ -12264,9 +12386,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>178</v>
+        <v>40</v>
       </c>
       <c r="B36" t="b">
         <v>1</v>
@@ -12287,9 +12409,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -12310,12 +12432,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" s="5">
         <v>1</v>
@@ -12333,9 +12455,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -12356,9 +12478,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -12379,9 +12501,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B41" t="b">
         <v>1</v>
@@ -12402,9 +12524,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="B42" t="b">
         <v>1</v>
@@ -12425,9 +12547,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B43" t="b">
         <v>1</v>
@@ -12439,7 +12561,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43">
         <v>100</v>
@@ -12448,9 +12570,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="B44" t="b">
         <v>1</v>
@@ -12468,12 +12590,12 @@
         <v>100</v>
       </c>
       <c r="G44" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="B45" t="b">
         <v>1</v>
@@ -12494,9 +12616,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B46" t="b">
         <v>1</v>
@@ -12508,7 +12630,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46">
         <v>100</v>
@@ -12517,9 +12639,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="B47" t="b">
         <v>1</v>
@@ -12537,12 +12659,12 @@
         <v>100</v>
       </c>
       <c r="G47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B48" t="b">
         <v>1</v>
@@ -12563,9 +12685,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B49" t="b">
         <v>1</v>
@@ -12586,9 +12708,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B50" t="b">
         <v>1</v>
@@ -12609,9 +12731,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B51" t="b">
         <v>1</v>
@@ -12632,9 +12754,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B52" t="b">
         <v>1</v>
@@ -12655,9 +12777,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B53" t="b">
         <v>1</v>
@@ -12675,12 +12797,12 @@
         <v>100</v>
       </c>
       <c r="G53" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="B54" t="b">
         <v>1</v>
@@ -12701,9 +12823,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B55" t="b">
         <v>1</v>
@@ -12724,9 +12846,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B56" t="b">
         <v>1</v>
@@ -12747,9 +12869,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>25</v>
+        <v>166</v>
       </c>
       <c r="B57" t="b">
         <v>1</v>
@@ -12770,9 +12892,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="B58" t="b">
         <v>1</v>
@@ -12793,9 +12915,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="B59" t="b">
         <v>1</v>
@@ -12813,12 +12935,12 @@
         <v>100</v>
       </c>
       <c r="G59" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B60" t="b">
         <v>1</v>
@@ -12839,9 +12961,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B61" t="b">
         <v>1</v>
@@ -12862,9 +12984,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B62" t="b">
         <v>1</v>
@@ -12885,9 +13007,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B63" t="b">
         <v>1</v>
@@ -12908,9 +13030,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="B64" t="b">
         <v>1</v>
@@ -12931,9 +13053,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>171</v>
+        <v>71</v>
       </c>
       <c r="B65" t="b">
         <v>1</v>
@@ -12954,9 +13076,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>172</v>
+        <v>72</v>
       </c>
       <c r="B66" t="b">
         <v>1</v>
@@ -12977,9 +13099,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B67" t="b">
         <v>1</v>
@@ -13000,9 +13122,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B68" t="b">
         <v>1</v>
@@ -13023,9 +13145,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="B69" t="b">
         <v>1</v>
@@ -13046,9 +13168,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B70" t="b">
         <v>1</v>
@@ -13069,9 +13191,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B71" t="b">
         <v>1</v>
@@ -13089,12 +13211,12 @@
         <v>100</v>
       </c>
       <c r="G71" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="B72" t="b">
         <v>1</v>
@@ -13115,9 +13237,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B73" t="b">
         <v>1</v>
@@ -13138,9 +13260,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>76</v>
+        <v>172</v>
       </c>
       <c r="B74" t="b">
         <v>1</v>
@@ -13158,12 +13280,12 @@
         <v>100</v>
       </c>
       <c r="G74" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B75" t="b">
         <v>1</v>
@@ -13184,9 +13306,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>78</v>
+        <v>180</v>
       </c>
       <c r="B76" t="b">
         <v>1</v>
@@ -13207,9 +13329,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>173</v>
+        <v>80</v>
       </c>
       <c r="B77" t="b">
         <v>1</v>
@@ -13224,15 +13346,15 @@
         <v>1</v>
       </c>
       <c r="F77">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G77" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B78" t="b">
         <v>1</v>
@@ -13253,9 +13375,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>181</v>
+        <v>82</v>
       </c>
       <c r="B79" t="b">
         <v>1</v>
@@ -13270,15 +13392,15 @@
         <v>1</v>
       </c>
       <c r="F79">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G79" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="B80" t="b">
         <v>1</v>
@@ -13299,9 +13421,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B81" t="b">
         <v>1</v>
@@ -13322,9 +13444,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B82" t="b">
         <v>1</v>
@@ -13345,9 +13467,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="B83" t="b">
         <v>1</v>
@@ -13362,15 +13484,15 @@
         <v>1</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G83" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B84" t="b">
         <v>1</v>
@@ -13391,9 +13513,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B85" t="b">
         <v>1</v>
@@ -13408,15 +13530,15 @@
         <v>1</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G85" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B86" t="b">
         <v>1</v>
@@ -13431,15 +13553,15 @@
         <v>1</v>
       </c>
       <c r="F86">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G86" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B87" t="b">
         <v>1</v>
@@ -13454,15 +13576,15 @@
         <v>1</v>
       </c>
       <c r="F87">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G87" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B88" t="b">
         <v>1</v>
@@ -13483,9 +13605,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B89" t="b">
         <v>1</v>
@@ -13500,15 +13622,15 @@
         <v>1</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G89" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B90" t="b">
         <v>1</v>
@@ -13523,15 +13645,15 @@
         <v>1</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G90" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B91" t="b">
         <v>1</v>
@@ -13546,15 +13668,15 @@
         <v>1</v>
       </c>
       <c r="F91">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G91" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B92" t="b">
         <v>1</v>
@@ -13575,9 +13697,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B93" t="b">
         <v>1</v>
@@ -13598,9 +13720,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B94" t="b">
         <v>1</v>
@@ -13621,9 +13743,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B95" t="b">
         <v>1</v>
@@ -13638,15 +13760,15 @@
         <v>1</v>
       </c>
       <c r="F95">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G95" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B96" t="b">
         <v>1</v>
@@ -13667,9 +13789,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B97" t="b">
         <v>1</v>
@@ -13684,18 +13806,18 @@
         <v>1</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G97" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C98" s="5">
         <v>1</v>
@@ -13713,9 +13835,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B99" t="b">
         <v>1</v>
@@ -13736,9 +13858,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B100" t="b">
         <v>1</v>
@@ -13753,202 +13875,202 @@
         <v>1</v>
       </c>
       <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" t="b">
+        <v>1</v>
+      </c>
+      <c r="C101" s="5">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101" s="5">
+        <v>1</v>
+      </c>
+      <c r="F101">
         <v>100</v>
       </c>
-      <c r="G100" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A101" s="5" t="s">
+      <c r="G101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B102" t="b">
+        <v>1</v>
+      </c>
+      <c r="C102" s="5">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102" s="5">
+        <v>1</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B103" t="b">
+        <v>1</v>
+      </c>
+      <c r="C103" s="5">
+        <v>1</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103" s="5">
+        <v>1</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B104" t="b">
+        <v>1</v>
+      </c>
+      <c r="C104" s="5">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104" s="5">
+        <v>1</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B105" t="b">
+        <v>1</v>
+      </c>
+      <c r="C105" s="5">
+        <v>1</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105" s="5">
+        <v>1</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B106" t="b">
+        <v>0</v>
+      </c>
+      <c r="C106" s="5">
+        <v>1</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106" s="5">
+        <v>1</v>
+      </c>
+      <c r="F106">
         <v>100</v>
       </c>
-      <c r="B101" t="b">
-        <v>0</v>
-      </c>
-      <c r="C101" s="5">
-        <v>1</v>
-      </c>
-      <c r="D101">
-        <v>0</v>
-      </c>
-      <c r="E101" s="5">
-        <v>1</v>
-      </c>
-      <c r="F101">
-        <v>0</v>
-      </c>
-      <c r="G101" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B102" t="b">
-        <v>1</v>
-      </c>
-      <c r="C102" s="5">
-        <v>1</v>
-      </c>
-      <c r="D102">
-        <v>0</v>
-      </c>
-      <c r="E102" s="5">
-        <v>1</v>
-      </c>
-      <c r="F102">
+      <c r="G106" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B107" t="b">
+        <v>1</v>
+      </c>
+      <c r="C107" s="5">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107" s="5">
+        <v>1</v>
+      </c>
+      <c r="F107">
         <v>100</v>
       </c>
-      <c r="G102" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A103" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B103" t="b">
-        <v>1</v>
-      </c>
-      <c r="C103" s="5">
-        <v>1</v>
-      </c>
-      <c r="D103">
-        <v>0</v>
-      </c>
-      <c r="E103" s="5">
-        <v>1</v>
-      </c>
-      <c r="F103">
-        <v>0</v>
-      </c>
-      <c r="G103" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A104" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B104" t="b">
-        <v>1</v>
-      </c>
-      <c r="C104" s="5">
-        <v>1</v>
-      </c>
-      <c r="D104">
-        <v>0</v>
-      </c>
-      <c r="E104" s="5">
-        <v>1</v>
-      </c>
-      <c r="F104">
+      <c r="G107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B108" t="b">
+        <v>1</v>
+      </c>
+      <c r="C108" s="5">
+        <v>1</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108" s="5">
+        <v>1</v>
+      </c>
+      <c r="F108">
         <v>100</v>
       </c>
-      <c r="G104" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A105" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B105" t="b">
-        <v>1</v>
-      </c>
-      <c r="C105" s="5">
-        <v>1</v>
-      </c>
-      <c r="D105">
-        <v>0</v>
-      </c>
-      <c r="E105" s="5">
-        <v>1</v>
-      </c>
-      <c r="F105">
-        <v>0</v>
-      </c>
-      <c r="G105" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B106" t="b">
-        <v>1</v>
-      </c>
-      <c r="C106" s="5">
-        <v>1</v>
-      </c>
-      <c r="D106">
-        <v>0</v>
-      </c>
-      <c r="E106" s="5">
-        <v>1</v>
-      </c>
-      <c r="F106">
-        <v>0</v>
-      </c>
-      <c r="G106" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A107" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B107" t="b">
-        <v>1</v>
-      </c>
-      <c r="C107" s="5">
-        <v>1</v>
-      </c>
-      <c r="D107">
-        <v>0</v>
-      </c>
-      <c r="E107" s="5">
-        <v>1</v>
-      </c>
-      <c r="F107">
-        <v>0</v>
-      </c>
-      <c r="G107" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A108" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B108" t="b">
-        <v>1</v>
-      </c>
-      <c r="C108" s="5">
-        <v>1</v>
-      </c>
-      <c r="D108">
-        <v>0</v>
-      </c>
-      <c r="E108" s="5">
-        <v>1</v>
-      </c>
-      <c r="F108">
-        <v>0</v>
-      </c>
       <c r="G108" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>179</v>
+        <v>109</v>
       </c>
       <c r="B109" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C109" s="5">
         <v>1</v>
@@ -13966,7 +14088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>110</v>
       </c>
@@ -13989,7 +14111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>111</v>
       </c>
@@ -14012,7 +14134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>112</v>
       </c>
@@ -14035,7 +14157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>113</v>
       </c>
@@ -14058,7 +14180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>114</v>
       </c>
@@ -14081,7 +14203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>115</v>
       </c>
@@ -14098,82 +14220,82 @@
         <v>1</v>
       </c>
       <c r="F115">
+        <v>22.22</v>
+      </c>
+      <c r="G115" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B116" t="b">
+        <v>1</v>
+      </c>
+      <c r="C116" s="5">
+        <v>1</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116" s="5">
+        <v>1</v>
+      </c>
+      <c r="F116">
+        <v>0</v>
+      </c>
+      <c r="G116" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B117" t="b">
+        <v>1</v>
+      </c>
+      <c r="C117" s="5">
+        <v>1</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117" s="5">
+        <v>1</v>
+      </c>
+      <c r="F117">
+        <v>22.22</v>
+      </c>
+      <c r="G117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B118" t="b">
+        <v>1</v>
+      </c>
+      <c r="C118" s="5">
+        <v>1</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+      <c r="E118" s="5">
+        <v>1</v>
+      </c>
+      <c r="F118">
         <v>100</v>
       </c>
-      <c r="G115" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A116" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B116" t="b">
-        <v>1</v>
-      </c>
-      <c r="C116" s="5">
-        <v>1</v>
-      </c>
-      <c r="D116">
-        <v>0</v>
-      </c>
-      <c r="E116" s="5">
-        <v>1</v>
-      </c>
-      <c r="F116">
-        <v>22.22</v>
-      </c>
-      <c r="G116" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A117" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B117" t="b">
-        <v>1</v>
-      </c>
-      <c r="C117" s="5">
-        <v>1</v>
-      </c>
-      <c r="D117">
-        <v>0</v>
-      </c>
-      <c r="E117" s="5">
-        <v>1</v>
-      </c>
-      <c r="F117">
-        <v>0</v>
-      </c>
-      <c r="G117" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A118" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B118" t="b">
-        <v>1</v>
-      </c>
-      <c r="C118" s="5">
-        <v>1</v>
-      </c>
-      <c r="D118">
-        <v>0</v>
-      </c>
-      <c r="E118" s="5">
-        <v>1</v>
-      </c>
-      <c r="F118">
-        <v>22.22</v>
-      </c>
       <c r="G118" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>117</v>
       </c>
@@ -14196,7 +14318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>118</v>
       </c>
@@ -14219,9 +14341,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B121" t="b">
         <v>1</v>
@@ -14242,9 +14364,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B122" t="b">
         <v>1</v>
@@ -14265,9 +14387,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B123" t="b">
         <v>1</v>
@@ -14288,9 +14410,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B124" t="b">
         <v>1</v>
@@ -14311,9 +14433,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B125" t="b">
         <v>1</v>
@@ -14334,9 +14456,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B126" t="b">
         <v>1</v>
@@ -14357,9 +14479,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B127" t="b">
         <v>1</v>
@@ -14380,9 +14502,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B128" t="b">
         <v>1</v>
@@ -14403,9 +14525,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B129" t="b">
         <v>1</v>
@@ -14426,9 +14548,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B130" t="b">
         <v>1</v>
@@ -14449,9 +14571,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B131" t="b">
         <v>1</v>
@@ -14472,9 +14594,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B132" t="b">
         <v>1</v>
@@ -14495,7 +14617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>21</v>
       </c>
@@ -14518,9 +14640,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B134" t="b">
         <v>1</v>
@@ -14541,9 +14663,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B135" t="b">
         <v>1</v>
@@ -14564,9 +14686,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B136" t="b">
         <v>1</v>
@@ -14587,9 +14709,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B137" t="b">
         <v>1</v>
@@ -14610,9 +14732,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B138" t="b">
         <v>1</v>
@@ -14633,9 +14755,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B139" t="b">
         <v>1</v>
@@ -14656,9 +14778,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B140" t="b">
         <v>1</v>
@@ -14679,9 +14801,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B141" t="b">
         <v>1</v>
@@ -14702,7 +14824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>26</v>
       </c>
@@ -14725,9 +14847,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B143" t="b">
         <v>1</v>
@@ -14748,9 +14870,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B144" t="b">
         <v>1</v>
@@ -14771,9 +14893,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B145" t="b">
         <v>1</v>
@@ -14794,9 +14916,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B146" t="b">
         <v>0</v>
@@ -14817,9 +14939,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B147" t="b">
         <v>1</v>
@@ -14840,9 +14962,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B148" t="b">
         <v>1</v>
@@ -14863,9 +14985,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B149" t="b">
         <v>1</v>
@@ -14886,9 +15008,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B150" t="b">
         <v>1</v>
@@ -14909,9 +15031,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B151" t="b">
         <v>1</v>
@@ -14932,9 +15054,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B152" t="b">
         <v>1</v>
@@ -14955,9 +15077,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B153" t="b">
         <v>1</v>
@@ -14978,9 +15100,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B154" t="b">
         <v>1</v>
@@ -15001,9 +15123,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B155" t="b">
         <v>1</v>
@@ -15024,9 +15146,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B156" t="b">
         <v>1</v>
@@ -15047,9 +15169,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B157" t="b">
         <v>1</v>
@@ -15070,9 +15192,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B158" t="b">
         <v>1</v>
@@ -15093,9 +15215,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B159" t="b">
         <v>1</v>
@@ -15116,9 +15238,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B160" t="b">
         <v>1</v>
@@ -15139,9 +15261,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B161" t="b">
         <v>1</v>
@@ -15162,7 +15284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>18</v>
       </c>
@@ -15185,9 +15307,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B163" t="b">
         <v>1</v>
@@ -15208,9 +15330,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B164" t="b">
         <v>1</v>
@@ -15231,9 +15353,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B165" t="b">
         <v>1</v>
@@ -15254,9 +15376,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B166" t="b">
         <v>1</v>
@@ -15277,9 +15399,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B167" t="b">
         <v>1</v>
@@ -15300,7 +15422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>22</v>
       </c>
@@ -15323,9 +15445,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B169" t="b">
         <v>1</v>
@@ -15346,9 +15468,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B170" t="b">
         <v>1</v>
@@ -15369,35 +15491,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A171" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="B171" t="b">
-        <v>1</v>
-      </c>
-      <c r="C171" s="5">
-        <v>1</v>
-      </c>
-      <c r="D171">
-        <v>0</v>
-      </c>
-      <c r="E171" s="5">
-        <v>1</v>
-      </c>
-      <c r="F171">
-        <v>100</v>
-      </c>
-      <c r="G171" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A172" s="5"/>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G171">
-    <sortCondition descending="1" ref="D8:D171"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G170">
+    <sortCondition descending="1" ref="D2:D170"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished standardising Hough based modules
These can now export the N highest scoring objects. They also have
parameter ranges with increments
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stephen\Programming\Java Projects\mia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB88BC39-79A1-4FA9-BAE1-0EAFC4CD03CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E74F877-0035-4638-BFC3-0E69733C2EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28095" windowHeight="16440" activeTab="1" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
   <si>
     <t>Date</t>
   </si>
@@ -589,6 +589,9 @@
   </si>
   <si>
     <t>Fit active contours</t>
+  </si>
+  <si>
+    <t>Rectangle detection</t>
   </si>
 </sst>
 </file>
@@ -710,10 +713,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$74</c:f>
+              <c:f>Sheet1!$B$2:$B$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -932,16 +935,19 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$74</c:f>
+              <c:f>Sheet1!$N$2:$N$75</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -1160,6 +1166,9 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>95.294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>95.32163742690058</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1199,10 +1208,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$74</c:f>
+              <c:f>Sheet1!$B$2:$B$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1421,18 +1430,21 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$74</c:f>
+              <c:f>Sheet1!$O$2:$O$75</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
-                  <c:v>12.661064425770308</c:v>
+                  <c:v>12.458654906284455</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -1649,6 +1661,9 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>97.43449781659389</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>97.474476088124661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1688,10 +1703,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$74</c:f>
+              <c:f>Sheet1!$B$2:$B$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1910,16 +1925,19 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$74</c:f>
+              <c:f>Sheet1!$P$2:$P$75</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -2138,6 +2156,9 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>96.470588235294116</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>96.491228070175438</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2177,10 +2198,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$74</c:f>
+              <c:f>Sheet1!$B$2:$B$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2399,16 +2420,19 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$74</c:f>
+              <c:f>Sheet1!$Q$2:$Q$75</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2626,6 +2650,9 @@
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="72">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="73">
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
               </c:numCache>
@@ -2666,10 +2693,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$74</c:f>
+              <c:f>Sheet1!$B$2:$B$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2888,16 +2915,19 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$74</c:f>
+              <c:f>Sheet1!$R$2:$R$75</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -3116,6 +3146,9 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>37.053571428571431</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>36.888888888888886</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3382,10 +3415,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$74</c:f>
+              <c:f>Sheet1!$A$2:$A$75</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3604,16 +3637,19 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>44466</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>44469</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$74</c:f>
+              <c:f>Sheet1!$N$2:$N$75</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -3832,6 +3868,9 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>95.294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>95.32163742690058</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3860,10 +3899,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$74</c:f>
+              <c:f>Sheet1!$A$2:$A$75</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4082,18 +4121,21 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>44466</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>44469</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$74</c:f>
+              <c:f>Sheet1!$O$2:$O$75</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
-                  <c:v>12.661064425770308</c:v>
+                  <c:v>12.458654906284455</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -4310,6 +4352,9 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>97.43449781659389</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>97.474476088124661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4338,10 +4383,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$74</c:f>
+              <c:f>Sheet1!$A$2:$A$75</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4560,16 +4605,19 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>44466</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>44469</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$74</c:f>
+              <c:f>Sheet1!$P$2:$P$75</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -4788,6 +4836,9 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>96.470588235294116</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>96.491228070175438</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4816,10 +4867,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$74</c:f>
+              <c:f>Sheet1!$A$2:$A$75</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -5038,16 +5089,19 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>44466</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>44469</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$74</c:f>
+              <c:f>Sheet1!$Q$2:$Q$75</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -5265,6 +5319,9 @@
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="72">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="73">
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
               </c:numCache>
@@ -5294,10 +5351,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$74</c:f>
+              <c:f>Sheet1!$A$2:$A$75</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -5516,16 +5573,19 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>44466</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>44469</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$74</c:f>
+              <c:f>Sheet1!$R$2:$R$75</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -5744,6 +5804,9 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>37.053571428571431</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>36.888888888888886</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7462,10 +7525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:R74"/>
+  <dimension ref="A1:R75"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T36" sqref="T36"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W64" sqref="W64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7577,7 +7640,7 @@
       </c>
       <c r="O2" s="3">
         <f>100*G2/MAX(G:G)</f>
-        <v>12.661064425770308</v>
+        <v>12.458654906284455</v>
       </c>
       <c r="P2" s="3">
         <f t="shared" ref="P2:P7" si="1">100*H2/D2</f>
@@ -11552,6 +11615,61 @@
       <c r="R74" s="3">
         <f t="shared" ref="R74" si="333">100*L74/K74</f>
         <v>37.053571428571431</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>44469</v>
+      </c>
+      <c r="B75" s="4">
+        <v>73</v>
+      </c>
+      <c r="D75">
+        <v>171</v>
+      </c>
+      <c r="E75">
+        <v>163</v>
+      </c>
+      <c r="F75">
+        <v>1861</v>
+      </c>
+      <c r="G75">
+        <v>1814</v>
+      </c>
+      <c r="H75">
+        <v>165</v>
+      </c>
+      <c r="I75">
+        <v>44</v>
+      </c>
+      <c r="J75">
+        <v>18</v>
+      </c>
+      <c r="K75">
+        <v>225</v>
+      </c>
+      <c r="L75">
+        <v>83</v>
+      </c>
+      <c r="N75" s="3">
+        <f t="shared" ref="N75" si="334">100*E75/D75</f>
+        <v>95.32163742690058</v>
+      </c>
+      <c r="O75" s="3">
+        <f t="shared" ref="O75" si="335">100*G75/F75</f>
+        <v>97.474476088124661</v>
+      </c>
+      <c r="P75" s="3">
+        <f t="shared" ref="P75" si="336">100*H75/D75</f>
+        <v>96.491228070175438</v>
+      </c>
+      <c r="Q75" s="3">
+        <f t="shared" ref="Q75" si="337">100*J75/I75</f>
+        <v>40.909090909090907</v>
+      </c>
+      <c r="R75" s="3">
+        <f t="shared" ref="R75" si="338">100*L75/K75</f>
+        <v>36.888888888888886</v>
       </c>
     </row>
   </sheetData>
@@ -11566,8 +11684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60F2A9E-CB35-4818-B2AA-21716033EEE9}">
   <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J105" sqref="J105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11583,16 +11701,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="B1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E1" s="5">
         <v>1</v>
@@ -11606,16 +11724,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -11624,21 +11742,21 @@
         <v>100</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -11652,16 +11770,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
@@ -11670,21 +11788,21 @@
         <v>100</v>
       </c>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
@@ -11698,16 +11816,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="B6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="5">
-        <v>0.44440000000000002</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
@@ -11721,7 +11839,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>15</v>
+        <v>151</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -11744,7 +11862,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>16</v>
+        <v>152</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -11767,7 +11885,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>33</v>
+        <v>153</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -11790,7 +11908,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>28</v>
+        <v>154</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -11802,7 +11920,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>100</v>
@@ -11813,7 +11931,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -11825,18 +11943,18 @@
         <v>0</v>
       </c>
       <c r="E11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>100</v>
       </c>
       <c r="G11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>30</v>
+        <v>163</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -11859,7 +11977,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>31</v>
+        <v>155</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -11882,7 +12000,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>32</v>
+        <v>156</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -11894,7 +12012,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>100</v>
@@ -11905,7 +12023,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -11928,7 +12046,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -11951,7 +12069,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>43</v>
+        <v>168</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -11974,7 +12092,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>44</v>
+        <v>167</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -11997,7 +12115,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>45</v>
+        <v>173</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -12020,7 +12138,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>46</v>
+        <v>169</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -12043,7 +12161,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -12066,7 +12184,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -12089,7 +12207,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>49</v>
+        <v>124</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -12112,7 +12230,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -12124,7 +12242,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>100</v>
@@ -12135,7 +12253,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -12150,7 +12268,7 @@
         <v>1</v>
       </c>
       <c r="F25">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G25" t="b">
         <v>1</v>
@@ -12158,7 +12276,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
@@ -12176,12 +12294,12 @@
         <v>100</v>
       </c>
       <c r="G26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
@@ -12204,7 +12322,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
@@ -12227,7 +12345,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -12245,12 +12363,12 @@
         <v>100</v>
       </c>
       <c r="G29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
@@ -12265,7 +12383,7 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
@@ -12273,7 +12391,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -12296,7 +12414,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -12319,7 +12437,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>177</v>
+        <v>20</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
@@ -12337,12 +12455,12 @@
         <v>100</v>
       </c>
       <c r="G33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
@@ -12365,10 +12483,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="B35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="5">
         <v>1</v>
@@ -12380,7 +12498,7 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G35" t="b">
         <v>1</v>
@@ -12388,7 +12506,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B36" t="b">
         <v>1</v>
@@ -12411,7 +12529,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -12434,7 +12552,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -12457,7 +12575,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -12480,7 +12598,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -12503,7 +12621,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="B41" t="b">
         <v>1</v>
@@ -12526,7 +12644,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="B42" t="b">
         <v>1</v>
@@ -12549,7 +12667,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="B43" t="b">
         <v>1</v>
@@ -12561,7 +12679,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43">
         <v>100</v>
@@ -12572,7 +12690,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B44" t="b">
         <v>1</v>
@@ -12590,12 +12708,12 @@
         <v>100</v>
       </c>
       <c r="G44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="B45" t="b">
         <v>1</v>
@@ -12618,16 +12736,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>60</v>
+        <v>141</v>
       </c>
       <c r="B46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E46" s="5">
         <v>1</v>
@@ -12636,21 +12754,21 @@
         <v>100</v>
       </c>
       <c r="G46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>61</v>
+        <v>142</v>
       </c>
       <c r="B47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E47" s="5">
         <v>1</v>
@@ -12664,7 +12782,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>62</v>
+        <v>143</v>
       </c>
       <c r="B48" t="b">
         <v>1</v>
@@ -12687,7 +12805,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B49" t="b">
         <v>1</v>
@@ -12710,7 +12828,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B50" t="b">
         <v>1</v>
@@ -12733,7 +12851,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="B51" t="b">
         <v>1</v>
@@ -12756,7 +12874,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="B52" t="b">
         <v>1</v>
@@ -12779,16 +12897,16 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="B53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E53" s="5">
         <v>1</v>
@@ -12797,12 +12915,12 @@
         <v>100</v>
       </c>
       <c r="G53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>25</v>
+        <v>177</v>
       </c>
       <c r="B54" t="b">
         <v>1</v>
@@ -12825,7 +12943,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B55" t="b">
         <v>1</v>
@@ -12848,10 +12966,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>68</v>
+        <v>178</v>
       </c>
       <c r="B56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56" s="5">
         <v>1</v>
@@ -12866,12 +12984,12 @@
         <v>100</v>
       </c>
       <c r="G56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>166</v>
+        <v>108</v>
       </c>
       <c r="B57" t="b">
         <v>1</v>
@@ -12894,7 +13012,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>173</v>
+        <v>62</v>
       </c>
       <c r="B58" t="b">
         <v>1</v>
@@ -12917,7 +13035,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>167</v>
+        <v>38</v>
       </c>
       <c r="B59" t="b">
         <v>1</v>
@@ -12940,10 +13058,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>168</v>
+        <v>39</v>
       </c>
       <c r="B60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C60" s="5">
         <v>1</v>
@@ -12963,7 +13081,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="B61" t="b">
         <v>1</v>
@@ -12986,7 +13104,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>170</v>
+        <v>46</v>
       </c>
       <c r="B62" t="b">
         <v>1</v>
@@ -13009,7 +13127,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>171</v>
+        <v>21</v>
       </c>
       <c r="B63" t="b">
         <v>1</v>
@@ -13032,7 +13150,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>70</v>
+        <v>184</v>
       </c>
       <c r="B64" t="b">
         <v>1</v>
@@ -13055,7 +13173,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B65" t="b">
         <v>1</v>
@@ -13078,7 +13196,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="B66" t="b">
         <v>1</v>
@@ -13093,7 +13211,7 @@
         <v>1</v>
       </c>
       <c r="F66">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G66" t="b">
         <v>1</v>
@@ -13101,7 +13219,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B67" t="b">
         <v>1</v>
@@ -13116,7 +13234,7 @@
         <v>1</v>
       </c>
       <c r="F67">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G67" t="b">
         <v>1</v>
@@ -13124,7 +13242,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="B68" t="b">
         <v>1</v>
@@ -13147,7 +13265,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B69" t="b">
         <v>1</v>
@@ -13170,7 +13288,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>75</v>
+        <v>164</v>
       </c>
       <c r="B70" t="b">
         <v>1</v>
@@ -13193,7 +13311,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B71" t="b">
         <v>1</v>
@@ -13211,12 +13329,12 @@
         <v>100</v>
       </c>
       <c r="G71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B72" t="b">
         <v>1</v>
@@ -13239,7 +13357,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="B73" t="b">
         <v>1</v>
@@ -13262,7 +13380,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>172</v>
+        <v>110</v>
       </c>
       <c r="B74" t="b">
         <v>1</v>
@@ -13285,7 +13403,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="B75" t="b">
         <v>1</v>
@@ -13308,7 +13426,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>180</v>
+        <v>76</v>
       </c>
       <c r="B76" t="b">
         <v>1</v>
@@ -13326,12 +13444,12 @@
         <v>100</v>
       </c>
       <c r="G76" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="B77" t="b">
         <v>1</v>
@@ -13346,7 +13464,7 @@
         <v>1</v>
       </c>
       <c r="F77">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G77" t="b">
         <v>1</v>
@@ -13354,7 +13472,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B78" t="b">
         <v>1</v>
@@ -13377,7 +13495,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="B79" t="b">
         <v>1</v>
@@ -13392,7 +13510,7 @@
         <v>1</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G79" t="b">
         <v>1</v>
@@ -13400,7 +13518,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B80" t="b">
         <v>1</v>
@@ -13415,7 +13533,7 @@
         <v>1</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G80" t="b">
         <v>1</v>
@@ -13423,7 +13541,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B81" t="b">
         <v>1</v>
@@ -13446,7 +13564,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="B82" t="b">
         <v>1</v>
@@ -13458,10 +13576,10 @@
         <v>0</v>
       </c>
       <c r="E82" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G82" t="b">
         <v>1</v>
@@ -13469,7 +13587,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B83" t="b">
         <v>1</v>
@@ -13492,7 +13610,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="B84" t="b">
         <v>1</v>
@@ -13515,7 +13633,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="B85" t="b">
         <v>1</v>
@@ -13538,7 +13656,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="B86" t="b">
         <v>1</v>
@@ -13553,7 +13671,7 @@
         <v>1</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G86" t="b">
         <v>1</v>
@@ -13561,7 +13679,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B87" t="b">
         <v>1</v>
@@ -13576,7 +13694,7 @@
         <v>1</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G87" t="b">
         <v>1</v>
@@ -13584,7 +13702,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B88" t="b">
         <v>1</v>
@@ -13607,7 +13725,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="B89" t="b">
         <v>1</v>
@@ -13630,7 +13748,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="B90" t="b">
         <v>1</v>
@@ -13653,7 +13771,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="B91" t="b">
         <v>1</v>
@@ -13668,7 +13786,7 @@
         <v>1</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G91" t="b">
         <v>1</v>
@@ -13676,7 +13794,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="B92" t="b">
         <v>1</v>
@@ -13699,7 +13817,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="B93" t="b">
         <v>1</v>
@@ -13722,7 +13840,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="B94" t="b">
         <v>1</v>
@@ -13734,10 +13852,10 @@
         <v>0</v>
       </c>
       <c r="E94" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G94" t="b">
         <v>1</v>
@@ -13745,7 +13863,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="B95" t="b">
         <v>1</v>
@@ -13760,7 +13878,7 @@
         <v>1</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G95" t="b">
         <v>1</v>
@@ -13768,7 +13886,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
       <c r="B96" t="b">
         <v>1</v>
@@ -13791,7 +13909,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="B97" t="b">
         <v>1</v>
@@ -13803,7 +13921,7 @@
         <v>0</v>
       </c>
       <c r="E97" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F97">
         <v>100</v>
@@ -13814,22 +13932,22 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B98" t="b">
+        <v>1</v>
+      </c>
+      <c r="C98" s="5">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98" s="5">
+        <v>1</v>
+      </c>
+      <c r="F98">
         <v>100</v>
-      </c>
-      <c r="B98" t="b">
-        <v>0</v>
-      </c>
-      <c r="C98" s="5">
-        <v>1</v>
-      </c>
-      <c r="D98">
-        <v>0</v>
-      </c>
-      <c r="E98" s="5">
-        <v>1</v>
-      </c>
-      <c r="F98">
-        <v>0</v>
       </c>
       <c r="G98" t="b">
         <v>1</v>
@@ -13837,7 +13955,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B99" t="b">
         <v>1</v>
@@ -13860,7 +13978,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="B100" t="b">
         <v>1</v>
@@ -13883,10 +14001,10 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B101" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" s="5">
         <v>1</v>
@@ -13898,7 +14016,7 @@
         <v>1</v>
       </c>
       <c r="F101">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G101" t="b">
         <v>1</v>
@@ -13906,7 +14024,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="B102" t="b">
         <v>1</v>
@@ -13921,7 +14039,7 @@
         <v>1</v>
       </c>
       <c r="F102">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G102" t="b">
         <v>1</v>
@@ -13929,7 +14047,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B103" t="b">
         <v>1</v>
@@ -13944,7 +14062,7 @@
         <v>1</v>
       </c>
       <c r="F103">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G103" t="b">
         <v>1</v>
@@ -13952,7 +14070,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B104" t="b">
         <v>1</v>
@@ -13975,7 +14093,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="B105" t="b">
         <v>1</v>
@@ -13990,7 +14108,7 @@
         <v>1</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G105" t="b">
         <v>1</v>
@@ -13998,10 +14116,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>178</v>
+        <v>82</v>
       </c>
       <c r="B106" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C106" s="5">
         <v>1</v>
@@ -14013,7 +14131,7 @@
         <v>1</v>
       </c>
       <c r="F106">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G106" t="b">
         <v>1</v>
@@ -14021,16 +14139,16 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B107" t="b">
         <v>1</v>
       </c>
       <c r="C107" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D107">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E107" s="5">
         <v>1</v>
@@ -14039,12 +14157,12 @@
         <v>100</v>
       </c>
       <c r="G107" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>184</v>
+        <v>105</v>
       </c>
       <c r="B108" t="b">
         <v>1</v>
@@ -14059,7 +14177,7 @@
         <v>1</v>
       </c>
       <c r="F108">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G108" t="b">
         <v>1</v>
@@ -14067,7 +14185,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B109" t="b">
         <v>1</v>
@@ -14082,7 +14200,7 @@
         <v>1</v>
       </c>
       <c r="F109">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G109" t="b">
         <v>1</v>
@@ -14090,7 +14208,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="B110" t="b">
         <v>1</v>
@@ -14105,7 +14223,7 @@
         <v>1</v>
       </c>
       <c r="F110">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G110" t="b">
         <v>1</v>
@@ -14113,7 +14231,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B111" t="b">
         <v>1</v>
@@ -14128,7 +14246,7 @@
         <v>1</v>
       </c>
       <c r="F111">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G111" t="b">
         <v>1</v>
@@ -14136,7 +14254,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="B112" t="b">
         <v>1</v>
@@ -14159,7 +14277,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="B113" t="b">
         <v>1</v>
@@ -14177,12 +14295,12 @@
         <v>100</v>
       </c>
       <c r="G113" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="B114" t="b">
         <v>1</v>
@@ -14205,7 +14323,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="B115" t="b">
         <v>1</v>
@@ -14220,7 +14338,7 @@
         <v>1</v>
       </c>
       <c r="F115">
-        <v>22.22</v>
+        <v>100</v>
       </c>
       <c r="G115" t="b">
         <v>1</v>
@@ -14228,7 +14346,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B116" t="b">
         <v>1</v>
@@ -14243,7 +14361,7 @@
         <v>1</v>
       </c>
       <c r="F116">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G116" t="b">
         <v>1</v>
@@ -14251,7 +14369,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>183</v>
+        <v>51</v>
       </c>
       <c r="B117" t="b">
         <v>1</v>
@@ -14266,7 +14384,7 @@
         <v>1</v>
       </c>
       <c r="F117">
-        <v>22.22</v>
+        <v>100</v>
       </c>
       <c r="G117" t="b">
         <v>1</v>
@@ -14274,7 +14392,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B118" t="b">
         <v>1</v>
@@ -14297,7 +14415,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B119" t="b">
         <v>1</v>
@@ -14320,7 +14438,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="B120" t="b">
         <v>1</v>
@@ -14335,7 +14453,7 @@
         <v>1</v>
       </c>
       <c r="F120">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G120" t="b">
         <v>1</v>
@@ -14343,16 +14461,16 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>120</v>
+        <v>176</v>
       </c>
       <c r="B121" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C121" s="5">
-        <v>1</v>
+        <v>0.44440000000000002</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E121" s="5">
         <v>1</v>
@@ -14366,7 +14484,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="B122" t="b">
         <v>1</v>
@@ -14381,7 +14499,7 @@
         <v>1</v>
       </c>
       <c r="F122">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G122" t="b">
         <v>1</v>
@@ -14389,7 +14507,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B123" t="b">
         <v>1</v>
@@ -14412,7 +14530,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>122</v>
+        <v>16</v>
       </c>
       <c r="B124" t="b">
         <v>1</v>
@@ -14435,7 +14553,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="B125" t="b">
         <v>1</v>
@@ -14458,7 +14576,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="B126" t="b">
         <v>1</v>
@@ -14476,15 +14594,15 @@
         <v>100</v>
       </c>
       <c r="G126" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="B127" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C127" s="5">
         <v>1</v>
@@ -14504,7 +14622,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>179</v>
+        <v>52</v>
       </c>
       <c r="B128" t="b">
         <v>1</v>
@@ -14527,7 +14645,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B129" t="b">
         <v>1</v>
@@ -14550,7 +14668,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="B130" t="b">
         <v>1</v>
@@ -14568,12 +14686,12 @@
         <v>100</v>
       </c>
       <c r="G130" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>125</v>
+        <v>185</v>
       </c>
       <c r="B131" t="b">
         <v>1</v>
@@ -14588,7 +14706,7 @@
         <v>1</v>
       </c>
       <c r="F131">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G131" t="b">
         <v>1</v>
@@ -14596,7 +14714,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>126</v>
+        <v>25</v>
       </c>
       <c r="B132" t="b">
         <v>1</v>
@@ -14619,7 +14737,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="B133" t="b">
         <v>1</v>
@@ -14642,7 +14760,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="B134" t="b">
         <v>1</v>
@@ -14665,7 +14783,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>128</v>
+        <v>26</v>
       </c>
       <c r="B135" t="b">
         <v>1</v>
@@ -14688,7 +14806,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B136" t="b">
         <v>1</v>
@@ -14711,7 +14829,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>130</v>
+        <v>67</v>
       </c>
       <c r="B137" t="b">
         <v>1</v>
@@ -14734,7 +14852,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B138" t="b">
         <v>1</v>
@@ -14757,7 +14875,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B139" t="b">
         <v>1</v>
@@ -14780,7 +14898,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="B140" t="b">
         <v>1</v>
@@ -14798,12 +14916,12 @@
         <v>100</v>
       </c>
       <c r="G140" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="B141" t="b">
         <v>1</v>
@@ -14826,7 +14944,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="B142" t="b">
         <v>1</v>
@@ -14849,7 +14967,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>138</v>
+        <v>77</v>
       </c>
       <c r="B143" t="b">
         <v>1</v>
@@ -14872,7 +14990,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>140</v>
+        <v>78</v>
       </c>
       <c r="B144" t="b">
         <v>1</v>
@@ -14887,7 +15005,7 @@
         <v>1</v>
       </c>
       <c r="F144">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G144" t="b">
         <v>1</v>
@@ -14895,7 +15013,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="B145" t="b">
         <v>1</v>
@@ -14918,10 +15036,10 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>158</v>
+        <v>79</v>
       </c>
       <c r="B146" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C146" s="5">
         <v>1</v>
@@ -14941,7 +15059,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>159</v>
+        <v>115</v>
       </c>
       <c r="B147" t="b">
         <v>1</v>
@@ -14956,7 +15074,7 @@
         <v>1</v>
       </c>
       <c r="F147">
-        <v>100</v>
+        <v>22.22</v>
       </c>
       <c r="G147" t="b">
         <v>1</v>
@@ -14964,7 +15082,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>160</v>
+        <v>72</v>
       </c>
       <c r="B148" t="b">
         <v>1</v>
@@ -14987,7 +15105,7 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>161</v>
+        <v>70</v>
       </c>
       <c r="B149" t="b">
         <v>1</v>
@@ -15005,12 +15123,12 @@
         <v>100</v>
       </c>
       <c r="G149" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="B150" t="b">
         <v>1</v>
@@ -15033,7 +15151,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B151" t="b">
         <v>1</v>
@@ -15056,7 +15174,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="B152" t="b">
         <v>1</v>
@@ -15079,7 +15197,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="B153" t="b">
         <v>1</v>
@@ -15102,7 +15220,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="B154" t="b">
         <v>1</v>
@@ -15125,7 +15243,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="B155" t="b">
         <v>1</v>
@@ -15143,12 +15261,12 @@
         <v>100</v>
       </c>
       <c r="G155" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B156" t="b">
         <v>1</v>
@@ -15171,16 +15289,16 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B157" t="b">
         <v>1</v>
       </c>
       <c r="C157" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D157">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E157" s="5">
         <v>1</v>
@@ -15194,7 +15312,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="B158" t="b">
         <v>1</v>
@@ -15217,7 +15335,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="B159" t="b">
         <v>1</v>
@@ -15232,7 +15350,7 @@
         <v>1</v>
       </c>
       <c r="F159">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G159" t="b">
         <v>1</v>
@@ -15240,7 +15358,7 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
       <c r="B160" t="b">
         <v>1</v>
@@ -15255,7 +15373,7 @@
         <v>1</v>
       </c>
       <c r="F160">
-        <v>100</v>
+        <v>22.22</v>
       </c>
       <c r="G160" t="b">
         <v>1</v>
@@ -15263,7 +15381,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>154</v>
+        <v>27</v>
       </c>
       <c r="B161" t="b">
         <v>1</v>
@@ -15286,7 +15404,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>18</v>
+        <v>179</v>
       </c>
       <c r="B162" t="b">
         <v>1</v>
@@ -15304,12 +15422,12 @@
         <v>100</v>
       </c>
       <c r="G162" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B163" t="b">
         <v>1</v>
@@ -15324,7 +15442,7 @@
         <v>1</v>
       </c>
       <c r="F163">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G163" t="b">
         <v>1</v>
@@ -15332,7 +15450,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="B164" t="b">
         <v>1</v>
@@ -15355,7 +15473,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="B165" t="b">
         <v>1</v>
@@ -15378,7 +15496,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>163</v>
+        <v>42</v>
       </c>
       <c r="B166" t="b">
         <v>1</v>
@@ -15401,7 +15519,7 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>164</v>
+        <v>56</v>
       </c>
       <c r="B167" t="b">
         <v>1</v>
@@ -15424,7 +15542,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="B168" t="b">
         <v>1</v>
@@ -15447,7 +15565,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>181</v>
+        <v>129</v>
       </c>
       <c r="B169" t="b">
         <v>1</v>
@@ -15470,7 +15588,7 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>182</v>
+        <v>130</v>
       </c>
       <c r="B170" t="b">
         <v>1</v>
@@ -15492,11 +15610,31 @@
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A171" s="5"/>
+      <c r="A171" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B171" t="b">
+        <v>1</v>
+      </c>
+      <c r="C171" s="5">
+        <v>1</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171" s="5">
+        <v>1</v>
+      </c>
+      <c r="F171">
+        <v>100</v>
+      </c>
+      <c r="G171" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G170">
-    <sortCondition descending="1" ref="D2:D170"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G171">
+    <sortCondition ref="A5:A171"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed parameter and module descriptions
Still need to finish image and object measurements
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Java Projects\MIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stephen\Programming\Java Projects\mia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D34D9D6-900A-4788-83D9-591FC6B4B59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC74B6F5-72DD-4C1F-B879-DD006B3A7643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28095" windowHeight="16440" activeTab="1" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
   <si>
     <t>Date</t>
   </si>
@@ -460,9 +460,6 @@
   </si>
   <si>
     <t>Create measurement map</t>
-  </si>
-  <si>
-    <t>Create object density map</t>
   </si>
   <si>
     <t>Create orthogonal view</t>
@@ -1186,7 +1183,7 @@
                   <c:v>95.906432748538009</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>97.058823529411768</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1471,7 +1468,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="77"/>
                 <c:pt idx="0">
-                  <c:v>12.255965292841649</c:v>
+                  <c:v>12.196438208310846</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -1699,7 +1696,7 @@
                   <c:v>98.708983324367935</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>99.514301133297351</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2212,7 +2209,7 @@
                   <c:v>98.245614035087726</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>99.411764705882348</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3978,7 +3975,7 @@
                   <c:v>95.906432748538009</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>97.058823529411768</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4252,7 +4249,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="77"/>
                 <c:pt idx="0">
-                  <c:v>12.255965292841649</c:v>
+                  <c:v>12.196438208310846</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -4480,7 +4477,7 @@
                   <c:v>98.708983324367935</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>99.514301133297351</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4982,7 +4979,7 @@
                   <c:v>98.245614035087726</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>99.411764705882348</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7707,32 +7704,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
   <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Z48" sqref="Z48"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T40" sqref="T40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7779,7 +7776,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44054</v>
       </c>
@@ -7820,7 +7817,7 @@
       </c>
       <c r="O2" s="3">
         <f>100*G2/MAX(G:G)</f>
-        <v>12.255965292841649</v>
+        <v>12.196438208310846</v>
       </c>
       <c r="P2" s="3">
         <f t="shared" ref="P2:P7" si="1">100*H2/D2</f>
@@ -7835,7 +7832,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44055</v>
       </c>
@@ -7891,7 +7888,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44056</v>
       </c>
@@ -7947,7 +7944,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44057</v>
       </c>
@@ -8002,7 +7999,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44058</v>
       </c>
@@ -8057,7 +8054,7 @@
         <v>39.71291866028708</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44064</v>
       </c>
@@ -8112,7 +8109,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44069</v>
       </c>
@@ -8167,7 +8164,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44070</v>
       </c>
@@ -8222,7 +8219,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44081</v>
       </c>
@@ -8277,7 +8274,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44082</v>
       </c>
@@ -8332,7 +8329,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44083</v>
       </c>
@@ -8387,7 +8384,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44084</v>
       </c>
@@ -8442,7 +8439,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44085</v>
       </c>
@@ -8497,7 +8494,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44089</v>
       </c>
@@ -8552,7 +8549,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44090</v>
       </c>
@@ -8607,7 +8604,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44091</v>
       </c>
@@ -8662,7 +8659,7 @@
         <v>39.523809523809526</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44097</v>
       </c>
@@ -8717,7 +8714,7 @@
         <v>38.967136150234744</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44098</v>
       </c>
@@ -8772,7 +8769,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44099</v>
       </c>
@@ -8827,7 +8824,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44102</v>
       </c>
@@ -8882,7 +8879,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44103</v>
       </c>
@@ -8937,7 +8934,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44104</v>
       </c>
@@ -8992,7 +8989,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44110</v>
       </c>
@@ -9047,7 +9044,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44113</v>
       </c>
@@ -9102,7 +9099,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44116</v>
       </c>
@@ -9157,7 +9154,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44117</v>
       </c>
@@ -9212,7 +9209,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44118</v>
       </c>
@@ -9267,7 +9264,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44119</v>
       </c>
@@ -9322,7 +9319,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44120</v>
       </c>
@@ -9377,7 +9374,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44123</v>
       </c>
@@ -9432,7 +9429,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44124</v>
       </c>
@@ -9487,7 +9484,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44125</v>
       </c>
@@ -9542,7 +9539,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44126</v>
       </c>
@@ -9597,7 +9594,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44127</v>
       </c>
@@ -9652,7 +9649,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44130</v>
       </c>
@@ -9707,7 +9704,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44131</v>
       </c>
@@ -9762,7 +9759,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44132</v>
       </c>
@@ -9817,7 +9814,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44134</v>
       </c>
@@ -9872,7 +9869,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44137</v>
       </c>
@@ -9927,7 +9924,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44138</v>
       </c>
@@ -9982,7 +9979,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44139</v>
       </c>
@@ -10037,7 +10034,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44140</v>
       </c>
@@ -10092,7 +10089,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44141</v>
       </c>
@@ -10147,7 +10144,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44147</v>
       </c>
@@ -10202,7 +10199,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44148</v>
       </c>
@@ -10257,7 +10254,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44151</v>
       </c>
@@ -10312,7 +10309,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44152</v>
       </c>
@@ -10367,7 +10364,7 @@
         <v>40.375586854460096</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>44300</v>
       </c>
@@ -10422,7 +10419,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>44301</v>
       </c>
@@ -10477,7 +10474,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>44302</v>
       </c>
@@ -10532,7 +10529,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44306</v>
       </c>
@@ -10587,7 +10584,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>44308</v>
       </c>
@@ -10642,7 +10639,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>44341</v>
       </c>
@@ -10697,7 +10694,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>44342</v>
       </c>
@@ -10752,7 +10749,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>44343</v>
       </c>
@@ -10807,7 +10804,7 @@
         <v>39.449541284403672</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>44369</v>
       </c>
@@ -10862,7 +10859,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>44370</v>
       </c>
@@ -10917,7 +10914,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>44405</v>
       </c>
@@ -10972,7 +10969,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>44406</v>
       </c>
@@ -11027,7 +11024,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>44413</v>
       </c>
@@ -11082,7 +11079,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>44414</v>
       </c>
@@ -11137,7 +11134,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>44415</v>
       </c>
@@ -11192,7 +11189,7 @@
         <v>39.269406392694066</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>44419</v>
       </c>
@@ -11247,7 +11244,7 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>44420</v>
       </c>
@@ -11302,7 +11299,7 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>44421</v>
       </c>
@@ -11357,7 +11354,7 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>44427</v>
       </c>
@@ -11412,7 +11409,7 @@
         <v>36.324786324786324</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>44431</v>
       </c>
@@ -11467,7 +11464,7 @@
         <v>36.956521739130437</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>44433</v>
       </c>
@@ -11522,7 +11519,7 @@
         <v>37.387387387387385</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>44441</v>
       </c>
@@ -11577,7 +11574,7 @@
         <v>37.387387387387385</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>44449</v>
       </c>
@@ -11632,7 +11629,7 @@
         <v>36.403508771929822</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>44452</v>
       </c>
@@ -11687,7 +11684,7 @@
         <v>36.403508771929822</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>44453</v>
       </c>
@@ -11742,7 +11739,7 @@
         <v>37.053571428571431</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>44466</v>
       </c>
@@ -11797,7 +11794,7 @@
         <v>37.053571428571431</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>44469</v>
       </c>
@@ -11852,7 +11849,7 @@
         <v>36.888888888888886</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>44470</v>
       </c>
@@ -11907,7 +11904,7 @@
         <v>36.888888888888886</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>44474</v>
       </c>
@@ -11962,7 +11959,7 @@
         <v>36.888888888888886</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>44475</v>
       </c>
@@ -11973,16 +11970,16 @@
         <v>170</v>
       </c>
       <c r="E78">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="F78">
         <v>1853</v>
       </c>
       <c r="G78">
-        <v>1844</v>
+        <v>1853</v>
       </c>
       <c r="H78">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I78">
         <v>44</v>
@@ -11997,27 +11994,27 @@
         <v>83</v>
       </c>
       <c r="N78" s="3">
-        <f t="shared" ref="N78:N79" si="349">100*E78/D78</f>
-        <v>97.058823529411768</v>
+        <f t="shared" ref="N78" si="349">100*E78/D78</f>
+        <v>100</v>
       </c>
       <c r="O78" s="3">
-        <f t="shared" ref="O78:O79" si="350">100*G78/F78</f>
-        <v>99.514301133297351</v>
+        <f t="shared" ref="O78" si="350">100*G78/F78</f>
+        <v>100</v>
       </c>
       <c r="P78" s="3">
-        <f t="shared" ref="P78:P79" si="351">100*H78/D78</f>
-        <v>99.411764705882348</v>
+        <f t="shared" ref="P78" si="351">100*H78/D78</f>
+        <v>100</v>
       </c>
       <c r="Q78" s="3">
-        <f t="shared" ref="Q78:Q79" si="352">100*J78/I78</f>
+        <f t="shared" ref="Q78" si="352">100*J78/I78</f>
         <v>40.909090909090907</v>
       </c>
       <c r="R78" s="3">
-        <f t="shared" ref="R78:R79" si="353">100*L78/K78</f>
+        <f t="shared" ref="R78" si="353">100*L78/K78</f>
         <v>36.888888888888886</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N79" s="3"/>
       <c r="O79" s="3"/>
       <c r="P79" s="3"/>
@@ -12034,35 +12031,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60F2A9E-CB35-4818-B2AA-21716033EEE9}">
-  <dimension ref="A1:G171"/>
+  <dimension ref="A1:G170"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="B1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E1" s="5">
         <v>1</v>
@@ -12074,18 +12071,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -12094,21 +12091,21 @@
         <v>100</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
       <c r="B3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -12120,9 +12117,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>104</v>
+        <v>28</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -12134,7 +12131,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>100</v>
@@ -12143,9 +12140,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -12157,7 +12154,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -12166,9 +12163,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -12189,9 +12186,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -12212,9 +12209,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -12235,9 +12232,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -12249,7 +12246,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -12258,9 +12255,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -12281,9 +12278,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -12304,9 +12301,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -12318,7 +12315,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>100</v>
@@ -12327,9 +12324,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>165</v>
+        <v>45</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -12350,9 +12347,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -12373,9 +12370,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -12396,9 +12393,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -12419,9 +12416,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -12442,9 +12439,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -12465,9 +12462,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -12488,9 +12485,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -12511,9 +12508,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -12534,9 +12531,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -12557,9 +12554,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -12577,12 +12574,12 @@
         <v>100</v>
       </c>
       <c r="G23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -12603,9 +12600,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -12626,9 +12623,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
@@ -12649,9 +12646,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>19</v>
+        <v>176</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
@@ -12669,12 +12666,12 @@
         <v>100</v>
       </c>
       <c r="G27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
@@ -12695,9 +12692,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -12718,9 +12715,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
@@ -12741,9 +12738,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>177</v>
+        <v>41</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -12764,9 +12761,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -12787,12 +12784,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" s="5">
         <v>1</v>
@@ -12810,9 +12807,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
@@ -12833,9 +12830,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B35" t="b">
         <v>1</v>
@@ -12856,9 +12853,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B36" t="b">
         <v>1</v>
@@ -12879,9 +12876,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -12893,7 +12890,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37">
         <v>100</v>
@@ -12902,9 +12899,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -12922,12 +12919,12 @@
         <v>100</v>
       </c>
       <c r="G38" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -12948,9 +12945,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -12971,9 +12968,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B41" t="b">
         <v>1</v>
@@ -12985,7 +12982,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41">
         <v>100</v>
@@ -12994,9 +12991,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="B42" t="b">
         <v>1</v>
@@ -13014,12 +13011,12 @@
         <v>100</v>
       </c>
       <c r="G42" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B43" t="b">
         <v>1</v>
@@ -13040,9 +13037,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B44" t="b">
         <v>1</v>
@@ -13063,9 +13060,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B45" t="b">
         <v>1</v>
@@ -13086,9 +13083,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B46" t="b">
         <v>1</v>
@@ -13109,9 +13106,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="B47" t="b">
         <v>1</v>
@@ -13129,12 +13126,12 @@
         <v>100</v>
       </c>
       <c r="G47" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="B48" t="b">
         <v>1</v>
@@ -13155,9 +13152,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B49" t="b">
         <v>1</v>
@@ -13178,9 +13175,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B50" t="b">
         <v>1</v>
@@ -13198,12 +13195,12 @@
         <v>100</v>
       </c>
       <c r="G50" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>24</v>
+        <v>165</v>
       </c>
       <c r="B51" t="b">
         <v>1</v>
@@ -13221,12 +13218,12 @@
         <v>100</v>
       </c>
       <c r="G51" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>25</v>
+        <v>172</v>
       </c>
       <c r="B52" t="b">
         <v>1</v>
@@ -13247,9 +13244,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>67</v>
+        <v>166</v>
       </c>
       <c r="B53" t="b">
         <v>1</v>
@@ -13270,9 +13267,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="B54" t="b">
         <v>1</v>
@@ -13290,12 +13287,12 @@
         <v>100</v>
       </c>
       <c r="G54" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B55" t="b">
         <v>1</v>
@@ -13316,9 +13313,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B56" t="b">
         <v>1</v>
@@ -13339,9 +13336,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B57" t="b">
         <v>1</v>
@@ -13362,9 +13359,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>168</v>
+        <v>69</v>
       </c>
       <c r="B58" t="b">
         <v>1</v>
@@ -13385,9 +13382,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>169</v>
+        <v>70</v>
       </c>
       <c r="B59" t="b">
         <v>1</v>
@@ -13408,9 +13405,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>170</v>
+        <v>71</v>
       </c>
       <c r="B60" t="b">
         <v>1</v>
@@ -13431,9 +13428,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>171</v>
+        <v>72</v>
       </c>
       <c r="B61" t="b">
         <v>1</v>
@@ -13454,9 +13451,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B62" t="b">
         <v>1</v>
@@ -13477,9 +13474,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B63" t="b">
         <v>1</v>
@@ -13500,9 +13497,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="B64" t="b">
         <v>1</v>
@@ -13523,9 +13520,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B65" t="b">
         <v>1</v>
@@ -13546,9 +13543,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B66" t="b">
         <v>1</v>
@@ -13566,12 +13563,12 @@
         <v>100</v>
       </c>
       <c r="G66" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="B67" t="b">
         <v>1</v>
@@ -13592,9 +13589,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B68" t="b">
         <v>1</v>
@@ -13615,9 +13612,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
       <c r="B69" t="b">
         <v>1</v>
@@ -13635,12 +13632,12 @@
         <v>100</v>
       </c>
       <c r="G69" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B70" t="b">
         <v>1</v>
@@ -13661,9 +13658,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>78</v>
+        <v>179</v>
       </c>
       <c r="B71" t="b">
         <v>1</v>
@@ -13684,9 +13681,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>172</v>
+        <v>80</v>
       </c>
       <c r="B72" t="b">
         <v>1</v>
@@ -13701,15 +13698,15 @@
         <v>1</v>
       </c>
       <c r="F72">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G72" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B73" t="b">
         <v>1</v>
@@ -13730,9 +13727,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>180</v>
+        <v>82</v>
       </c>
       <c r="B74" t="b">
         <v>1</v>
@@ -13747,15 +13744,15 @@
         <v>1</v>
       </c>
       <c r="F74">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G74" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="B75" t="b">
         <v>1</v>
@@ -13776,9 +13773,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B76" t="b">
         <v>1</v>
@@ -13799,9 +13796,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B77" t="b">
         <v>1</v>
@@ -13822,9 +13819,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="B78" t="b">
         <v>1</v>
@@ -13839,15 +13836,15 @@
         <v>1</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G78" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B79" t="b">
         <v>1</v>
@@ -13868,9 +13865,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B80" t="b">
         <v>1</v>
@@ -13885,15 +13882,15 @@
         <v>1</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G80" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B81" t="b">
         <v>1</v>
@@ -13908,15 +13905,15 @@
         <v>1</v>
       </c>
       <c r="F81">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G81" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B82" t="b">
         <v>1</v>
@@ -13931,15 +13928,15 @@
         <v>1</v>
       </c>
       <c r="F82">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G82" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B83" t="b">
         <v>1</v>
@@ -13960,9 +13957,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B84" t="b">
         <v>1</v>
@@ -13977,15 +13974,15 @@
         <v>1</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G84" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B85" t="b">
         <v>1</v>
@@ -14000,15 +13997,15 @@
         <v>1</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G85" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B86" t="b">
         <v>1</v>
@@ -14023,15 +14020,15 @@
         <v>1</v>
       </c>
       <c r="F86">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G86" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B87" t="b">
         <v>1</v>
@@ -14052,9 +14049,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B88" t="b">
         <v>1</v>
@@ -14075,9 +14072,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B89" t="b">
         <v>1</v>
@@ -14098,9 +14095,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B90" t="b">
         <v>1</v>
@@ -14115,15 +14112,15 @@
         <v>1</v>
       </c>
       <c r="F90">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G90" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B91" t="b">
         <v>1</v>
@@ -14144,9 +14141,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B92" t="b">
         <v>1</v>
@@ -14161,15 +14158,15 @@
         <v>1</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G92" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B93" t="b">
         <v>1</v>
@@ -14190,9 +14187,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B94" t="b">
         <v>1</v>
@@ -14213,9 +14210,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B95" t="b">
         <v>1</v>
@@ -14230,38 +14227,38 @@
         <v>1</v>
       </c>
       <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B96" t="b">
+        <v>1</v>
+      </c>
+      <c r="C96" s="5">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96" s="5">
+        <v>1</v>
+      </c>
+      <c r="F96">
         <v>100</v>
       </c>
-      <c r="G95" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A96" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B96" t="b">
-        <v>0</v>
-      </c>
-      <c r="C96" s="5">
-        <v>1</v>
-      </c>
-      <c r="D96">
-        <v>0</v>
-      </c>
-      <c r="E96" s="5">
-        <v>1</v>
-      </c>
-      <c r="F96">
-        <v>0</v>
-      </c>
       <c r="G96" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B97" t="b">
         <v>1</v>
@@ -14282,9 +14279,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B98" t="b">
         <v>1</v>
@@ -14305,9 +14302,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B99" t="b">
         <v>1</v>
@@ -14322,84 +14319,84 @@
         <v>1</v>
       </c>
       <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B100" t="b">
+        <v>1</v>
+      </c>
+      <c r="C100" s="5">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100" s="5">
+        <v>1</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B101" t="b">
+        <v>1</v>
+      </c>
+      <c r="C101" s="5">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101" s="5">
+        <v>1</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B102" t="b">
+        <v>1</v>
+      </c>
+      <c r="C102" s="5">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102" s="5">
+        <v>1</v>
+      </c>
+      <c r="F102">
         <v>100</v>
       </c>
-      <c r="G99" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B100" t="b">
-        <v>1</v>
-      </c>
-      <c r="C100" s="5">
-        <v>1</v>
-      </c>
-      <c r="D100">
-        <v>0</v>
-      </c>
-      <c r="E100" s="5">
-        <v>1</v>
-      </c>
-      <c r="F100">
-        <v>0</v>
-      </c>
-      <c r="G100" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A101" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B101" t="b">
-        <v>1</v>
-      </c>
-      <c r="C101" s="5">
-        <v>1</v>
-      </c>
-      <c r="D101">
-        <v>0</v>
-      </c>
-      <c r="E101" s="5">
-        <v>1</v>
-      </c>
-      <c r="F101">
-        <v>0</v>
-      </c>
-      <c r="G101" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B102" t="b">
-        <v>1</v>
-      </c>
-      <c r="C102" s="5">
-        <v>1</v>
-      </c>
-      <c r="D102">
-        <v>0</v>
-      </c>
-      <c r="E102" s="5">
-        <v>1</v>
-      </c>
-      <c r="F102">
-        <v>0</v>
-      </c>
       <c r="G102" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>174</v>
+        <v>108</v>
       </c>
       <c r="B103" t="b">
         <v>1</v>
@@ -14414,18 +14411,18 @@
         <v>1</v>
       </c>
       <c r="F103">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G103" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B104" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C104" s="5">
         <v>1</v>
@@ -14443,9 +14440,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B105" t="b">
         <v>1</v>
@@ -14466,9 +14463,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>184</v>
+        <v>110</v>
       </c>
       <c r="B106" t="b">
         <v>1</v>
@@ -14489,9 +14486,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B107" t="b">
         <v>1</v>
@@ -14512,9 +14509,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B108" t="b">
         <v>1</v>
@@ -14535,9 +14532,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B109" t="b">
         <v>1</v>
@@ -14558,9 +14555,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>112</v>
+        <v>184</v>
       </c>
       <c r="B110" t="b">
         <v>1</v>
@@ -14575,15 +14572,15 @@
         <v>1</v>
       </c>
       <c r="F110">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G110" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B111" t="b">
         <v>1</v>
@@ -14604,9 +14601,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>185</v>
+        <v>115</v>
       </c>
       <c r="B112" t="b">
         <v>1</v>
@@ -14621,15 +14618,15 @@
         <v>1</v>
       </c>
       <c r="F112">
-        <v>0</v>
+        <v>22.22</v>
       </c>
       <c r="G112" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>114</v>
+        <v>174</v>
       </c>
       <c r="B113" t="b">
         <v>1</v>
@@ -14644,15 +14641,15 @@
         <v>1</v>
       </c>
       <c r="F113">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G113" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="B114" t="b">
         <v>1</v>
@@ -14673,9 +14670,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>175</v>
+        <v>116</v>
       </c>
       <c r="B115" t="b">
         <v>1</v>
@@ -14690,15 +14687,15 @@
         <v>1</v>
       </c>
       <c r="F115">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G115" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>183</v>
+        <v>117</v>
       </c>
       <c r="B116" t="b">
         <v>1</v>
@@ -14713,15 +14710,15 @@
         <v>1</v>
       </c>
       <c r="F116">
-        <v>22.22</v>
+        <v>100</v>
       </c>
       <c r="G116" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B117" t="b">
         <v>1</v>
@@ -14742,9 +14739,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B118" t="b">
         <v>1</v>
@@ -14765,9 +14762,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B119" t="b">
         <v>1</v>
@@ -14788,9 +14785,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B120" t="b">
         <v>1</v>
@@ -14811,9 +14808,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B121" t="b">
         <v>1</v>
@@ -14834,9 +14831,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="B122" t="b">
         <v>1</v>
@@ -14857,9 +14854,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="B123" t="b">
         <v>1</v>
@@ -14877,12 +14874,12 @@
         <v>100</v>
       </c>
       <c r="G123" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B124" t="b">
         <v>1</v>
@@ -14903,9 +14900,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>134</v>
+        <v>178</v>
       </c>
       <c r="B125" t="b">
         <v>1</v>
@@ -14923,12 +14920,12 @@
         <v>100</v>
       </c>
       <c r="G125" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B126" t="b">
         <v>1</v>
@@ -14949,9 +14946,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>179</v>
+        <v>124</v>
       </c>
       <c r="B127" t="b">
         <v>1</v>
@@ -14972,9 +14969,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B128" t="b">
         <v>1</v>
@@ -14995,9 +14992,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B129" t="b">
         <v>1</v>
@@ -15018,9 +15015,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="B130" t="b">
         <v>1</v>
@@ -15041,9 +15038,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>126</v>
+        <v>21</v>
       </c>
       <c r="B131" t="b">
         <v>1</v>
@@ -15064,9 +15061,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>176</v>
+        <v>127</v>
       </c>
       <c r="B132" t="b">
         <v>1</v>
@@ -15087,9 +15084,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="B133" t="b">
         <v>1</v>
@@ -15110,9 +15107,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B134" t="b">
         <v>1</v>
@@ -15133,9 +15130,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B135" t="b">
         <v>1</v>
@@ -15156,9 +15153,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B136" t="b">
         <v>1</v>
@@ -15179,9 +15176,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B137" t="b">
         <v>1</v>
@@ -15202,9 +15199,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B138" t="b">
         <v>1</v>
@@ -15225,9 +15222,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B139" t="b">
         <v>1</v>
@@ -15248,9 +15245,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>136</v>
+        <v>26</v>
       </c>
       <c r="B140" t="b">
         <v>1</v>
@@ -15271,9 +15268,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B141" t="b">
         <v>1</v>
@@ -15294,9 +15291,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>26</v>
+        <v>139</v>
       </c>
       <c r="B142" t="b">
         <v>1</v>
@@ -15317,9 +15314,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B143" t="b">
         <v>1</v>
@@ -15334,15 +15331,15 @@
         <v>1</v>
       </c>
       <c r="F143">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G143" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B144" t="b">
         <v>1</v>
@@ -15363,9 +15360,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B145" t="b">
         <v>1</v>
@@ -15380,15 +15377,15 @@
         <v>1</v>
       </c>
       <c r="F145">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G145" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="B146" t="b">
         <v>1</v>
@@ -15409,12 +15406,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>158</v>
       </c>
       <c r="B147" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C147" s="5">
         <v>1</v>
@@ -15432,7 +15429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>159</v>
       </c>
@@ -15455,7 +15452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>160</v>
       </c>
@@ -15475,10 +15472,10 @@
         <v>100</v>
       </c>
       <c r="G149" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>161</v>
       </c>
@@ -15498,12 +15495,12 @@
         <v>100</v>
       </c>
       <c r="G150" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B151" t="b">
         <v>1</v>
@@ -15524,7 +15521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>144</v>
       </c>
@@ -15547,7 +15544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>145</v>
       </c>
@@ -15570,7 +15567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>146</v>
       </c>
@@ -15593,7 +15590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>147</v>
       </c>
@@ -15616,7 +15613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>148</v>
       </c>
@@ -15639,7 +15636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>149</v>
       </c>
@@ -15662,7 +15659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>150</v>
       </c>
@@ -15685,7 +15682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>151</v>
       </c>
@@ -15708,7 +15705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>152</v>
       </c>
@@ -15731,7 +15728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>153</v>
       </c>
@@ -15754,9 +15751,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>154</v>
+        <v>18</v>
       </c>
       <c r="B162" t="b">
         <v>1</v>
@@ -15774,12 +15771,12 @@
         <v>100</v>
       </c>
       <c r="G162" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>18</v>
+        <v>154</v>
       </c>
       <c r="B163" t="b">
         <v>1</v>
@@ -15797,10 +15794,10 @@
         <v>100</v>
       </c>
       <c r="G163" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>155</v>
       </c>
@@ -15823,7 +15820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>156</v>
       </c>
@@ -15846,9 +15843,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="B166" t="b">
         <v>1</v>
@@ -15869,7 +15866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>163</v>
       </c>
@@ -15892,9 +15889,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>164</v>
+        <v>22</v>
       </c>
       <c r="B168" t="b">
         <v>1</v>
@@ -15915,9 +15912,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>22</v>
+        <v>180</v>
       </c>
       <c r="B169" t="b">
         <v>1</v>
@@ -15938,7 +15935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>181</v>
       </c>
@@ -15961,32 +15958,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A171" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B171" t="b">
-        <v>1</v>
-      </c>
-      <c r="C171" s="5">
-        <v>1</v>
-      </c>
-      <c r="D171">
-        <v>0</v>
-      </c>
-      <c r="E171" s="5">
-        <v>1</v>
-      </c>
-      <c r="F171">
-        <v>100</v>
-      </c>
-      <c r="G171" t="b">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G171">
-    <sortCondition descending="1" ref="D2:D171"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G170">
+    <sortCondition descending="1" ref="C4:C170"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed distance map error
- Distance maps should now work correctly
- Exported results will now be ordered alphabetically within groups
- Added junction-based linking to ridge detection
- Added documentation
</commit_message>
<xml_diff>
--- a/CoverageHistory.xlsx
+++ b/CoverageHistory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stephen\Programming\Java Projects\mia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Programming\Java Projects\mia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC74B6F5-72DD-4C1F-B879-DD006B3A7643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902DD4A1-2FDE-45C3-9F16-0F3F6CB0DD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28095" windowHeight="16440" activeTab="1" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1E1EBE36-CBC3-40F1-926B-7C5FE1426F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
   <si>
     <t>Date</t>
   </si>
@@ -210,9 +210,6 @@
     <t>White balance correction</t>
   </si>
   <si>
-    <t>Best focus stack</t>
-  </si>
-  <si>
     <t>Concatenate stacks</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
     <t>Flip stack</t>
   </si>
   <si>
-    <t>Focus stack</t>
-  </si>
-  <si>
     <t>Image type converter</t>
   </si>
   <si>
@@ -318,15 +312,9 @@
     <t>Calculate nearest neighbour</t>
   </si>
   <si>
-    <t>Convex hull 2D</t>
-  </si>
-  <si>
     <t>Fit ellipse</t>
   </si>
   <si>
-    <t>Fit ellipsoid</t>
-  </si>
-  <si>
     <t>Fit Gaussian 2D</t>
   </si>
   <si>
@@ -589,6 +577,36 @@
   </si>
   <si>
     <t>Rectangle detection</t>
+  </si>
+  <si>
+    <t>Measure greyscale K-function</t>
+  </si>
+  <si>
+    <t>Focus stack (global)</t>
+  </si>
+  <si>
+    <t>Focus stack (local)</t>
+  </si>
+  <si>
+    <t>Scale stack</t>
+  </si>
+  <si>
+    <t>Affine (fixed transform)</t>
+  </si>
+  <si>
+    <t>Cluster points</t>
+  </si>
+  <si>
+    <t>Measure object greyscale K-function</t>
+  </si>
+  <si>
+    <t>Measure texture along path</t>
+  </si>
+  <si>
+    <t>Fit concave hull 2D</t>
+  </si>
+  <si>
+    <t>Fit convex hull 2D</t>
   </si>
 </sst>
 </file>
@@ -665,7 +683,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -710,10 +728,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$78</c:f>
+              <c:f>Sheet1!$B$2:$B$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -944,16 +962,22 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$78</c:f>
+              <c:f>Sheet1!$N$2:$N$80</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -1184,6 +1208,12 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>98.86363636363636</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>98.86363636363636</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1223,10 +1253,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$78</c:f>
+              <c:f>Sheet1!$B$2:$B$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1457,18 +1487,24 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$78</c:f>
+              <c:f>Sheet1!$O$2:$O$80</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
-                  <c:v>12.196438208310846</c:v>
+                  <c:v>11.758584807492195</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -1697,6 +1733,12 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>96.136248093543472</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>97.712252160650735</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1736,10 +1778,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$78</c:f>
+              <c:f>Sheet1!$B$2:$B$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1970,16 +2012,22 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$78</c:f>
+              <c:f>Sheet1!$P$2:$P$80</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -2210,6 +2258,12 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>82.38636363636364</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>91.477272727272734</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2249,10 +2303,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$78</c:f>
+              <c:f>Sheet1!$B$2:$B$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2483,16 +2537,22 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$78</c:f>
+              <c:f>Sheet1!$Q$2:$Q$80</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2722,6 +2782,12 @@
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="76">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="78">
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
               </c:numCache>
@@ -2762,10 +2828,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$78</c:f>
+              <c:f>Sheet1!$B$2:$B$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2996,16 +3062,22 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$78</c:f>
+              <c:f>Sheet1!$R$2:$R$80</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -3236,6 +3308,12 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>36.888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>39.33649289099526</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>39.33649289099526</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3458,7 +3536,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3502,10 +3580,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$78</c:f>
+              <c:f>Sheet1!$A$2:$A$80</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -3736,16 +3814,22 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>44475</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>44754</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>44755</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$78</c:f>
+              <c:f>Sheet1!$N$2:$N$80</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>39.751552795031053</c:v>
                 </c:pt>
@@ -3976,6 +4060,12 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>98.86363636363636</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>98.86363636363636</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4004,10 +4094,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$78</c:f>
+              <c:f>Sheet1!$A$2:$A$80</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4238,18 +4328,24 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>44475</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>44754</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>44755</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$78</c:f>
+              <c:f>Sheet1!$O$2:$O$80</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
-                  <c:v>12.196438208310846</c:v>
+                  <c:v>11.758584807492195</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.049833887043189</c:v>
@@ -4478,6 +4574,12 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>96.136248093543472</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>97.712252160650735</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4506,10 +4608,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$78</c:f>
+              <c:f>Sheet1!$A$2:$A$80</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -4740,16 +4842,22 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>44475</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>44754</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>44755</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$78</c:f>
+              <c:f>Sheet1!$P$2:$P$80</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>14.285714285714286</c:v>
                 </c:pt>
@@ -4980,6 +5088,12 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>82.38636363636364</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>91.477272727272734</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5008,10 +5122,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$78</c:f>
+              <c:f>Sheet1!$A$2:$A$80</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -5242,16 +5356,22 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>44475</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>44754</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>44755</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$78</c:f>
+              <c:f>Sheet1!$Q$2:$Q$80</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -5481,6 +5601,12 @@
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="76">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="78">
                   <c:v>40.909090909090907</c:v>
                 </c:pt>
               </c:numCache>
@@ -5510,10 +5636,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$78</c:f>
+              <c:f>Sheet1!$A$2:$A$80</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>44054</c:v>
                 </c:pt>
@@ -5744,16 +5870,22 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>44475</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>44754</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>44755</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$78</c:f>
+              <c:f>Sheet1!$R$2:$R$80</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="77"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>39.71291866028708</c:v>
                 </c:pt>
@@ -5984,6 +6116,12 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>36.888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>39.33649289099526</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>39.33649289099526</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6010,7 +6148,6 @@
         <c:axId val="412970511"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="44484"/>
           <c:min val="44054"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -7702,10 +7839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3A4CB9-B2C9-4F6A-BDD3-E5AE50E57391}">
-  <dimension ref="A1:R79"/>
+  <dimension ref="A1:R80"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="T40" sqref="T40"/>
+    <sheetView topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="X38" sqref="X38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7817,7 +7954,7 @@
       </c>
       <c r="O2" s="3">
         <f>100*G2/MAX(G:G)</f>
-        <v>12.196438208310846</v>
+        <v>11.758584807492195</v>
       </c>
       <c r="P2" s="3">
         <f t="shared" ref="P2:P7" si="1">100*H2/D2</f>
@@ -12015,11 +12152,114 @@
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N79" s="3"/>
-      <c r="O79" s="3"/>
-      <c r="P79" s="3"/>
-      <c r="Q79" s="3"/>
-      <c r="R79" s="3"/>
+      <c r="A79" s="2">
+        <v>44754</v>
+      </c>
+      <c r="B79" s="4">
+        <v>77</v>
+      </c>
+      <c r="D79">
+        <v>176</v>
+      </c>
+      <c r="E79">
+        <v>174</v>
+      </c>
+      <c r="F79">
+        <v>1967</v>
+      </c>
+      <c r="G79">
+        <v>1891</v>
+      </c>
+      <c r="H79">
+        <v>145</v>
+      </c>
+      <c r="I79">
+        <v>44</v>
+      </c>
+      <c r="J79">
+        <v>18</v>
+      </c>
+      <c r="K79">
+        <v>211</v>
+      </c>
+      <c r="L79">
+        <v>83</v>
+      </c>
+      <c r="N79" s="3">
+        <f t="shared" ref="N79" si="354">100*E79/D79</f>
+        <v>98.86363636363636</v>
+      </c>
+      <c r="O79" s="3">
+        <f t="shared" ref="O79" si="355">100*G79/F79</f>
+        <v>96.136248093543472</v>
+      </c>
+      <c r="P79" s="3">
+        <f t="shared" ref="P79" si="356">100*H79/D79</f>
+        <v>82.38636363636364</v>
+      </c>
+      <c r="Q79" s="3">
+        <f t="shared" ref="Q79" si="357">100*J79/I79</f>
+        <v>40.909090909090907</v>
+      </c>
+      <c r="R79" s="3">
+        <f t="shared" ref="R79" si="358">100*L79/K79</f>
+        <v>39.33649289099526</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>44755</v>
+      </c>
+      <c r="B80" s="4">
+        <v>78</v>
+      </c>
+      <c r="D80">
+        <v>176</v>
+      </c>
+      <c r="E80">
+        <v>174</v>
+      </c>
+      <c r="F80">
+        <v>1967</v>
+      </c>
+      <c r="G80">
+        <v>1922</v>
+      </c>
+      <c r="H80">
+        <v>161</v>
+      </c>
+      <c r="I80">
+        <v>44</v>
+      </c>
+      <c r="J80">
+        <v>18</v>
+      </c>
+      <c r="K80">
+        <v>211</v>
+      </c>
+      <c r="L80">
+        <v>83</v>
+      </c>
+      <c r="N80" s="3">
+        <f t="shared" ref="N80" si="359">100*E80/D80</f>
+        <v>98.86363636363636</v>
+      </c>
+      <c r="O80" s="3">
+        <f t="shared" ref="O80" si="360">100*G80/F80</f>
+        <v>97.712252160650735</v>
+      </c>
+      <c r="P80" s="3">
+        <f t="shared" ref="P80" si="361">100*H80/D80</f>
+        <v>91.477272727272734</v>
+      </c>
+      <c r="Q80" s="3">
+        <f t="shared" ref="Q80" si="362">100*J80/I80</f>
+        <v>40.909090909090907</v>
+      </c>
+      <c r="R80" s="3">
+        <f t="shared" ref="R80" si="363">100*L80/K80</f>
+        <v>39.33649289099526</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -12031,18 +12271,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60F2A9E-CB35-4818-B2AA-21716033EEE9}">
-  <dimension ref="A1:G170"/>
+  <dimension ref="A1:G176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
@@ -12056,10 +12296,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="5">
-        <v>1</v>
+        <v>0.93330000000000002</v>
       </c>
       <c r="D1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1" s="5">
         <v>1</v>
@@ -12096,7 +12336,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -12119,19 +12359,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>28</v>
+        <v>140</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>1</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>100</v>
@@ -12142,7 +12382,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>29</v>
+        <v>160</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -12154,7 +12394,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -12165,7 +12405,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -12188,7 +12428,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -12200,7 +12440,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>100</v>
@@ -12211,19 +12451,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>32</v>
+        <v>181</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
       <c r="C8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>100</v>
@@ -12234,7 +12474,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -12246,7 +12486,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -12257,7 +12497,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -12280,7 +12520,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -12303,7 +12543,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -12315,7 +12555,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>100</v>
@@ -12326,7 +12566,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -12349,7 +12589,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -12372,7 +12612,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -12395,7 +12635,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -12418,7 +12658,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -12441,7 +12681,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -12464,7 +12704,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -12487,7 +12727,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -12510,7 +12750,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -12533,7 +12773,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -12556,7 +12796,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -12574,12 +12814,12 @@
         <v>100</v>
       </c>
       <c r="G23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -12602,7 +12842,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -12625,7 +12865,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
@@ -12643,12 +12883,12 @@
         <v>100</v>
       </c>
       <c r="G26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>176</v>
+        <v>35</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
@@ -12671,7 +12911,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
@@ -12694,7 +12934,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -12717,7 +12957,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>40</v>
+        <v>172</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
@@ -12740,7 +12980,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -12763,7 +13003,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -12786,7 +13026,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
@@ -12809,7 +13049,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
@@ -12832,7 +13072,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B35" t="b">
         <v>1</v>
@@ -12855,16 +13095,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B36" t="b">
         <v>1</v>
       </c>
       <c r="C36" s="5">
-        <v>1</v>
+        <v>0.81820000000000004</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E36" s="5">
         <v>1</v>
@@ -12878,7 +13118,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -12890,7 +13130,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37">
         <v>100</v>
@@ -12901,7 +13141,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -12919,12 +13159,12 @@
         <v>100</v>
       </c>
       <c r="G38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -12947,7 +13187,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -12965,12 +13205,12 @@
         <v>100</v>
       </c>
       <c r="G40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B41" t="b">
         <v>1</v>
@@ -12993,7 +13233,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B42" t="b">
         <v>1</v>
@@ -13016,7 +13256,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B43" t="b">
         <v>1</v>
@@ -13039,7 +13279,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B44" t="b">
         <v>1</v>
@@ -13062,7 +13302,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B45" t="b">
         <v>1</v>
@@ -13085,7 +13325,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>66</v>
+        <v>182</v>
       </c>
       <c r="B46" t="b">
         <v>1</v>
@@ -13097,7 +13337,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46">
         <v>100</v>
@@ -13108,16 +13348,16 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>24</v>
+        <v>183</v>
       </c>
       <c r="B47" t="b">
         <v>1</v>
       </c>
       <c r="C47" s="5">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E47" s="5">
         <v>1</v>
@@ -13126,12 +13366,12 @@
         <v>100</v>
       </c>
       <c r="G47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="B48" t="b">
         <v>1</v>
@@ -13154,7 +13394,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="B49" t="b">
         <v>1</v>
@@ -13172,12 +13412,12 @@
         <v>100</v>
       </c>
       <c r="G49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B50" t="b">
         <v>1</v>
@@ -13195,12 +13435,12 @@
         <v>100</v>
       </c>
       <c r="G50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>165</v>
+        <v>66</v>
       </c>
       <c r="B51" t="b">
         <v>1</v>
@@ -13218,12 +13458,12 @@
         <v>100</v>
       </c>
       <c r="G51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="B52" t="b">
         <v>1</v>
@@ -13246,7 +13486,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B53" t="b">
         <v>1</v>
@@ -13269,7 +13509,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B54" t="b">
         <v>1</v>
@@ -13292,16 +13532,16 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="B55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E55" s="5">
         <v>1</v>
@@ -13315,7 +13555,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B56" t="b">
         <v>1</v>
@@ -13338,7 +13578,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B57" t="b">
         <v>1</v>
@@ -13361,7 +13601,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>69</v>
+        <v>164</v>
       </c>
       <c r="B58" t="b">
         <v>1</v>
@@ -13384,7 +13624,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="B59" t="b">
         <v>1</v>
@@ -13407,7 +13647,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>71</v>
+        <v>165</v>
       </c>
       <c r="B60" t="b">
         <v>1</v>
@@ -13430,7 +13670,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>72</v>
+        <v>166</v>
       </c>
       <c r="B61" t="b">
         <v>1</v>
@@ -13453,7 +13693,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B62" t="b">
         <v>1</v>
@@ -13476,7 +13716,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B63" t="b">
         <v>1</v>
@@ -13499,7 +13739,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="B64" t="b">
         <v>1</v>
@@ -13522,7 +13762,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B65" t="b">
         <v>1</v>
@@ -13545,7 +13785,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B66" t="b">
         <v>1</v>
@@ -13563,12 +13803,12 @@
         <v>100</v>
       </c>
       <c r="G66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B67" t="b">
         <v>1</v>
@@ -13591,7 +13831,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="B68" t="b">
         <v>1</v>
@@ -13614,7 +13854,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>171</v>
+        <v>113</v>
       </c>
       <c r="B69" t="b">
         <v>1</v>
@@ -13637,7 +13877,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="B70" t="b">
         <v>1</v>
@@ -13660,7 +13900,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B71" t="b">
         <v>1</v>
@@ -13675,7 +13915,7 @@
         <v>1</v>
       </c>
       <c r="F71">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G71" t="b">
         <v>1</v>
@@ -13683,22 +13923,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>80</v>
+        <v>186</v>
       </c>
       <c r="B72" t="b">
         <v>1</v>
       </c>
       <c r="C72" s="5">
-        <v>1</v>
+        <v>0.625</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E72" s="5">
         <v>1</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G72" t="b">
         <v>1</v>
@@ -13706,16 +13946,16 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="B73" t="b">
         <v>1</v>
       </c>
       <c r="C73" s="5">
-        <v>1</v>
+        <v>0.88890000000000002</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E73" s="5">
         <v>1</v>
@@ -13729,22 +13969,22 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B74" t="b">
         <v>1</v>
       </c>
       <c r="C74" s="5">
-        <v>1</v>
+        <v>0.90910000000000002</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74" s="5">
         <v>1</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G74" t="b">
         <v>1</v>
@@ -13752,7 +13992,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>23</v>
+        <v>180</v>
       </c>
       <c r="B75" t="b">
         <v>1</v>
@@ -13775,16 +14015,16 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="B76" t="b">
         <v>1</v>
       </c>
       <c r="C76" s="5">
-        <v>1</v>
+        <v>0.88239999999999996</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E76" s="5">
         <v>1</v>
@@ -13798,7 +14038,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="B77" t="b">
         <v>1</v>
@@ -13813,7 +14053,7 @@
         <v>1</v>
       </c>
       <c r="F77">
-        <v>0</v>
+        <v>22.22</v>
       </c>
       <c r="G77" t="b">
         <v>1</v>
@@ -13821,7 +14061,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="B78" t="b">
         <v>1</v>
@@ -13836,7 +14076,7 @@
         <v>1</v>
       </c>
       <c r="F78">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G78" t="b">
         <v>1</v>
@@ -13844,22 +14084,22 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>86</v>
+        <v>178</v>
       </c>
       <c r="B79" t="b">
         <v>1</v>
       </c>
       <c r="C79" s="5">
-        <v>1</v>
+        <v>0.88890000000000002</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" s="5">
         <v>1</v>
       </c>
       <c r="F79">
-        <v>100</v>
+        <v>22.22</v>
       </c>
       <c r="G79" t="b">
         <v>1</v>
@@ -13867,7 +14107,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="B80" t="b">
         <v>1</v>
@@ -13890,7 +14130,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
       <c r="B81" t="b">
         <v>1</v>
@@ -13905,7 +14145,7 @@
         <v>1</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G81" t="b">
         <v>1</v>
@@ -13913,7 +14153,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="B82" t="b">
         <v>1</v>
@@ -13928,7 +14168,7 @@
         <v>1</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G82" t="b">
         <v>1</v>
@@ -13936,7 +14176,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="B83" t="b">
         <v>1</v>
@@ -13959,7 +14199,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
       <c r="B84" t="b">
         <v>1</v>
@@ -13982,7 +14222,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="B85" t="b">
         <v>1</v>
@@ -14005,7 +14245,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="B86" t="b">
         <v>1</v>
@@ -14020,7 +14260,7 @@
         <v>1</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G86" t="b">
         <v>1</v>
@@ -14028,7 +14268,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="B87" t="b">
         <v>1</v>
@@ -14051,7 +14291,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="B88" t="b">
         <v>1</v>
@@ -14074,7 +14314,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="B89" t="b">
         <v>1</v>
@@ -14089,7 +14329,7 @@
         <v>1</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G89" t="b">
         <v>1</v>
@@ -14097,7 +14337,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>97</v>
+        <v>175</v>
       </c>
       <c r="B90" t="b">
         <v>1</v>
@@ -14112,7 +14352,7 @@
         <v>1</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G90" t="b">
         <v>1</v>
@@ -14120,7 +14360,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="B91" t="b">
         <v>1</v>
@@ -14135,7 +14375,7 @@
         <v>1</v>
       </c>
       <c r="F91">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G91" t="b">
         <v>1</v>
@@ -14143,16 +14383,16 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>99</v>
+        <v>187</v>
       </c>
       <c r="B92" t="b">
         <v>1</v>
       </c>
       <c r="C92" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E92" s="5">
         <v>1</v>
@@ -14166,22 +14406,22 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" t="b">
+        <v>1</v>
+      </c>
+      <c r="C93" s="5">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93" s="5">
+        <v>1</v>
+      </c>
+      <c r="F93">
         <v>100</v>
-      </c>
-      <c r="B93" t="b">
-        <v>1</v>
-      </c>
-      <c r="C93" s="5">
-        <v>1</v>
-      </c>
-      <c r="D93">
-        <v>0</v>
-      </c>
-      <c r="E93" s="5">
-        <v>1</v>
-      </c>
-      <c r="F93">
-        <v>0</v>
       </c>
       <c r="G93" t="b">
         <v>1</v>
@@ -14189,7 +14429,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="B94" t="b">
         <v>1</v>
@@ -14204,7 +14444,7 @@
         <v>1</v>
       </c>
       <c r="F94">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G94" t="b">
         <v>1</v>
@@ -14212,7 +14452,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>102</v>
+        <v>23</v>
       </c>
       <c r="B95" t="b">
         <v>1</v>
@@ -14235,7 +14475,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>103</v>
+        <v>188</v>
       </c>
       <c r="B96" t="b">
         <v>1</v>
@@ -14250,7 +14490,7 @@
         <v>1</v>
       </c>
       <c r="F96">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G96" t="b">
         <v>1</v>
@@ -14258,7 +14498,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="B97" t="b">
         <v>1</v>
@@ -14281,7 +14521,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="B98" t="b">
         <v>1</v>
@@ -14304,7 +14544,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="B99" t="b">
         <v>1</v>
@@ -14319,7 +14559,7 @@
         <v>1</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G99" t="b">
         <v>1</v>
@@ -14327,7 +14567,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B100" t="b">
         <v>1</v>
@@ -14342,7 +14582,7 @@
         <v>1</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G100" t="b">
         <v>1</v>
@@ -14350,7 +14590,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>173</v>
+        <v>85</v>
       </c>
       <c r="B101" t="b">
         <v>1</v>
@@ -14365,7 +14605,7 @@
         <v>1</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G101" t="b">
         <v>1</v>
@@ -14373,7 +14613,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>177</v>
+        <v>86</v>
       </c>
       <c r="B102" t="b">
         <v>1</v>
@@ -14388,7 +14628,7 @@
         <v>1</v>
       </c>
       <c r="F102">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G102" t="b">
         <v>1</v>
@@ -14396,7 +14636,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="B103" t="b">
         <v>1</v>
@@ -14411,7 +14651,7 @@
         <v>1</v>
       </c>
       <c r="F103">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G103" t="b">
         <v>1</v>
@@ -14419,7 +14659,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>183</v>
+        <v>88</v>
       </c>
       <c r="B104" t="b">
         <v>1</v>
@@ -14442,7 +14682,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B105" t="b">
         <v>1</v>
@@ -14465,7 +14705,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="B106" t="b">
         <v>1</v>
@@ -14488,7 +14728,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="B107" t="b">
         <v>1</v>
@@ -14503,7 +14743,7 @@
         <v>1</v>
       </c>
       <c r="F107">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G107" t="b">
         <v>1</v>
@@ -14511,7 +14751,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="B108" t="b">
         <v>1</v>
@@ -14534,7 +14774,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="B109" t="b">
         <v>1</v>
@@ -14549,7 +14789,7 @@
         <v>1</v>
       </c>
       <c r="F109">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G109" t="b">
         <v>1</v>
@@ -14557,7 +14797,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>184</v>
+        <v>97</v>
       </c>
       <c r="B110" t="b">
         <v>1</v>
@@ -14572,7 +14812,7 @@
         <v>1</v>
       </c>
       <c r="F110">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G110" t="b">
         <v>1</v>
@@ -14580,7 +14820,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="B111" t="b">
         <v>1</v>
@@ -14595,7 +14835,7 @@
         <v>1</v>
       </c>
       <c r="F111">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G111" t="b">
         <v>1</v>
@@ -14603,7 +14843,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B112" t="b">
         <v>1</v>
@@ -14618,7 +14858,7 @@
         <v>1</v>
       </c>
       <c r="F112">
-        <v>22.22</v>
+        <v>100</v>
       </c>
       <c r="G112" t="b">
         <v>1</v>
@@ -14626,7 +14866,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>174</v>
+        <v>100</v>
       </c>
       <c r="B113" t="b">
         <v>1</v>
@@ -14641,7 +14881,7 @@
         <v>1</v>
       </c>
       <c r="F113">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G113" t="b">
         <v>1</v>
@@ -14649,7 +14889,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>182</v>
+        <v>101</v>
       </c>
       <c r="B114" t="b">
         <v>1</v>
@@ -14664,7 +14904,7 @@
         <v>1</v>
       </c>
       <c r="F114">
-        <v>22.22</v>
+        <v>0</v>
       </c>
       <c r="G114" t="b">
         <v>1</v>
@@ -14672,7 +14912,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B115" t="b">
         <v>1</v>
@@ -14687,7 +14927,7 @@
         <v>1</v>
       </c>
       <c r="F115">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G115" t="b">
         <v>1</v>
@@ -14695,7 +14935,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B116" t="b">
         <v>1</v>
@@ -14710,7 +14950,7 @@
         <v>1</v>
       </c>
       <c r="F116">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G116" t="b">
         <v>1</v>
@@ -14718,7 +14958,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>118</v>
+        <v>173</v>
       </c>
       <c r="B117" t="b">
         <v>1</v>
@@ -14741,7 +14981,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B118" t="b">
         <v>1</v>
@@ -14764,7 +15004,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="B119" t="b">
         <v>1</v>
@@ -14787,7 +15027,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>121</v>
+        <v>189</v>
       </c>
       <c r="B120" t="b">
         <v>1</v>
@@ -14810,7 +15050,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>122</v>
+        <v>190</v>
       </c>
       <c r="B121" t="b">
         <v>1</v>
@@ -14833,7 +15073,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="B122" t="b">
         <v>1</v>
@@ -14856,7 +15096,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="B123" t="b">
         <v>1</v>
@@ -14871,15 +15111,15 @@
         <v>1</v>
       </c>
       <c r="F123">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G123" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="B124" t="b">
         <v>1</v>
@@ -14902,7 +15142,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>178</v>
+        <v>105</v>
       </c>
       <c r="B125" t="b">
         <v>1</v>
@@ -14925,7 +15165,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="B126" t="b">
         <v>1</v>
@@ -14948,10 +15188,10 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B127" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C127" s="5">
         <v>1</v>
@@ -14971,7 +15211,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B128" t="b">
         <v>1</v>
@@ -14994,7 +15234,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B129" t="b">
         <v>1</v>
@@ -15017,7 +15257,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>175</v>
+        <v>26</v>
       </c>
       <c r="B130" t="b">
         <v>1</v>
@@ -15040,7 +15280,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
       <c r="B131" t="b">
         <v>1</v>
@@ -15063,7 +15303,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B132" t="b">
         <v>1</v>
@@ -15086,22 +15326,22 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B133" t="b">
         <v>1</v>
       </c>
       <c r="C133" s="5">
-        <v>1</v>
+        <v>0.95240000000000002</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E133" s="5">
         <v>1</v>
       </c>
       <c r="F133">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G133" t="b">
         <v>1</v>
@@ -15109,7 +15349,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B134" t="b">
         <v>1</v>
@@ -15132,7 +15372,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B135" t="b">
         <v>1</v>
@@ -15155,7 +15395,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B136" t="b">
         <v>1</v>
@@ -15178,7 +15418,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B137" t="b">
         <v>1</v>
@@ -15201,16 +15441,16 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B138" t="b">
         <v>1</v>
       </c>
       <c r="C138" s="5">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D138">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E138" s="5">
         <v>1</v>
@@ -15224,7 +15464,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="B139" t="b">
         <v>1</v>
@@ -15247,7 +15487,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>26</v>
+        <v>127</v>
       </c>
       <c r="B140" t="b">
         <v>1</v>
@@ -15270,7 +15510,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B141" t="b">
         <v>1</v>
@@ -15288,12 +15528,12 @@
         <v>100</v>
       </c>
       <c r="G141" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="B142" t="b">
         <v>1</v>
@@ -15316,7 +15556,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="B143" t="b">
         <v>1</v>
@@ -15331,7 +15571,7 @@
         <v>1</v>
       </c>
       <c r="F143">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G143" t="b">
         <v>1</v>
@@ -15339,7 +15579,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="B144" t="b">
         <v>1</v>
@@ -15362,7 +15602,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="B145" t="b">
         <v>1</v>
@@ -15385,7 +15625,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>157</v>
+        <v>77</v>
       </c>
       <c r="B146" t="b">
         <v>1</v>
@@ -15408,7 +15648,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>158</v>
+        <v>17</v>
       </c>
       <c r="B147" t="b">
         <v>1</v>
@@ -15431,7 +15671,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>159</v>
+        <v>73</v>
       </c>
       <c r="B148" t="b">
         <v>1</v>
@@ -15454,7 +15694,7 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>160</v>
+        <v>74</v>
       </c>
       <c r="B149" t="b">
         <v>1</v>
@@ -15477,7 +15717,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>161</v>
+        <v>65</v>
       </c>
       <c r="B150" t="b">
         <v>1</v>
@@ -15500,7 +15740,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B151" t="b">
         <v>1</v>
@@ -15523,7 +15763,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B152" t="b">
         <v>1</v>
@@ -15546,7 +15786,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B153" t="b">
         <v>1</v>
@@ -15569,7 +15809,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B154" t="b">
         <v>1</v>
@@ -15592,7 +15832,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B155" t="b">
         <v>1</v>
@@ -15615,7 +15855,7 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B156" t="b">
         <v>1</v>
@@ -15638,7 +15878,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B157" t="b">
         <v>1</v>
@@ -15656,12 +15896,12 @@
         <v>100</v>
       </c>
       <c r="G157" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B158" t="b">
         <v>1</v>
@@ -15684,7 +15924,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B159" t="b">
         <v>1</v>
@@ -15707,7 +15947,7 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B160" t="b">
         <v>1</v>
@@ -15730,7 +15970,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B161" t="b">
         <v>1</v>
@@ -15753,7 +15993,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>18</v>
+        <v>144</v>
       </c>
       <c r="B162" t="b">
         <v>1</v>
@@ -15771,12 +16011,12 @@
         <v>100</v>
       </c>
       <c r="G162" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B163" t="b">
         <v>1</v>
@@ -15799,7 +16039,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B164" t="b">
         <v>1</v>
@@ -15822,7 +16062,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B165" t="b">
         <v>1</v>
@@ -15845,7 +16085,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B166" t="b">
         <v>1</v>
@@ -15868,7 +16108,7 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B167" t="b">
         <v>1</v>
@@ -15891,7 +16131,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B168" t="b">
         <v>1</v>
@@ -15909,12 +16149,12 @@
         <v>100</v>
       </c>
       <c r="G168" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="B169" t="b">
         <v>1</v>
@@ -15937,7 +16177,7 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="B170" t="b">
         <v>1</v>
@@ -15958,10 +16198,145 @@
         <v>1</v>
       </c>
     </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B171" t="b">
+        <v>1</v>
+      </c>
+      <c r="C171" s="5">
+        <v>1</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171" s="5">
+        <v>1</v>
+      </c>
+      <c r="F171">
+        <v>100</v>
+      </c>
+      <c r="G171" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B172" t="b">
+        <v>1</v>
+      </c>
+      <c r="C172" s="5">
+        <v>1</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172" s="5">
+        <v>1</v>
+      </c>
+      <c r="F172">
+        <v>100</v>
+      </c>
+      <c r="G172" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B173" t="b">
+        <v>1</v>
+      </c>
+      <c r="C173" s="5">
+        <v>1</v>
+      </c>
+      <c r="D173">
+        <v>0</v>
+      </c>
+      <c r="E173" s="5">
+        <v>1</v>
+      </c>
+      <c r="F173">
+        <v>100</v>
+      </c>
+      <c r="G173" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B174" t="b">
+        <v>1</v>
+      </c>
+      <c r="C174" s="5">
+        <v>1</v>
+      </c>
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174" s="5">
+        <v>1</v>
+      </c>
+      <c r="F174">
+        <v>100</v>
+      </c>
+      <c r="G174" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B175" t="b">
+        <v>1</v>
+      </c>
+      <c r="C175" s="5">
+        <v>1</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175" s="5">
+        <v>1</v>
+      </c>
+      <c r="F175">
+        <v>100</v>
+      </c>
+      <c r="G175" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B176" t="b">
+        <v>1</v>
+      </c>
+      <c r="C176" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="D176">
+        <v>1</v>
+      </c>
+      <c r="E176" s="5">
+        <v>1</v>
+      </c>
+      <c r="F176">
+        <v>100</v>
+      </c>
+      <c r="G176" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G170">
-    <sortCondition descending="1" ref="C4:C170"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>